<commit_message>
Bugfix for Tierra del Fuego abbrev.
</commit_message>
<xml_diff>
--- a/inst/extdata/political_units.xlsx
+++ b/inst/extdata/political_units.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2866" uniqueCount="1580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2866" uniqueCount="1581">
   <si>
     <t xml:space="preserve">Abbrev</t>
   </si>
@@ -4534,6 +4534,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tierra del Fuego</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARG_V</t>
   </si>
   <si>
     <t xml:space="preserve">Tucumán</t>
@@ -4778,6 +4781,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -4799,6 +4803,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4897,36 +4902,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.8775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.1530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.0867346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.8469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="8.48469387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="24.2908163265306"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.1530612244898"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="23.3010204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="25.8367346938776"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="25.9795918367347"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="19.9132653061224"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.1581632653061"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.1785714285714"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="12.2908163265306"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="10.3214285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.7448979591837"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="12.1581632653061"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="10.1785714285714"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="12.2908163265306"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="10.3214285714286"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="10.7448979591837"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="10.6020408163265"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="8.63265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.7551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="19.1683673469388"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14179,10 +14184,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14423,7 +14428,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -14439,20 +14444,20 @@
   <dimension ref="A1:J948"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B900" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B894" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A900" activeCellId="0" sqref="A900"/>
-      <selection pane="bottomRight" activeCell="E903" activeCellId="0" sqref="E903"/>
+      <selection pane="bottomLeft" activeCell="A894" activeCellId="0" sqref="A894"/>
+      <selection pane="bottomRight" activeCell="B919" activeCellId="0" sqref="B919"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.4081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0051020408163"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23570,7 +23575,7 @@
         <v>1503</v>
       </c>
       <c r="B918" s="0" t="s">
-        <v>1502</v>
+        <v>1504</v>
       </c>
       <c r="C918" s="0" t="s">
         <v>43</v>
@@ -23581,10 +23586,10 @@
     </row>
     <row r="919" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A919" s="0" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="B919" s="0" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="C919" s="0" t="s">
         <v>43</v>
@@ -23595,24 +23600,24 @@
     </row>
     <row r="920" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A920" s="0" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="B920" s="0" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="C920" s="0" t="s">
         <v>293</v>
       </c>
       <c r="J920" s="0" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="921" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A921" s="0" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="B921" s="0" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="C921" s="0" t="s">
         <v>293</v>
@@ -23621,15 +23626,15 @@
         <v>1</v>
       </c>
       <c r="J921" s="0" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="922" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A922" s="0" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="B922" s="0" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="C922" s="0" t="s">
         <v>293</v>
@@ -23638,15 +23643,15 @@
         <v>1</v>
       </c>
       <c r="J922" s="0" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="923" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A923" s="0" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="B923" s="0" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="C923" s="0" t="s">
         <v>293</v>
@@ -23655,7 +23660,7 @@
         <v>1</v>
       </c>
       <c r="J923" s="0" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="924" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23663,7 +23668,7 @@
         <v>716</v>
       </c>
       <c r="B924" s="0" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="C924" s="0" t="s">
         <v>293</v>
@@ -23672,15 +23677,15 @@
         <v>1</v>
       </c>
       <c r="J924" s="0" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="925" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A925" s="0" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="B925" s="0" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="C925" s="0" t="s">
         <v>293</v>
@@ -23689,15 +23694,15 @@
         <v>1</v>
       </c>
       <c r="J925" s="0" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="926" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A926" s="0" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="B926" s="0" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="C926" s="0" t="s">
         <v>293</v>
@@ -23706,15 +23711,15 @@
         <v>1</v>
       </c>
       <c r="J926" s="0" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="927" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A927" s="0" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="B927" s="0" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="C927" s="0" t="s">
         <v>293</v>
@@ -23723,15 +23728,15 @@
         <v>1</v>
       </c>
       <c r="J927" s="0" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="928" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A928" s="0" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="B928" s="0" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="C928" s="0" t="s">
         <v>293</v>
@@ -23740,15 +23745,15 @@
         <v>1</v>
       </c>
       <c r="J928" s="0" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="929" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A929" s="0" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="B929" s="0" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="C929" s="0" t="s">
         <v>293</v>
@@ -23757,15 +23762,15 @@
         <v>1</v>
       </c>
       <c r="J929" s="0" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="930" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A930" s="0" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="B930" s="0" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="C930" s="0" t="s">
         <v>293</v>
@@ -23774,7 +23779,7 @@
         <v>1</v>
       </c>
       <c r="J930" s="0" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="931" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23782,7 +23787,7 @@
         <v>722</v>
       </c>
       <c r="B931" s="0" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="C931" s="0" t="s">
         <v>293</v>
@@ -23791,15 +23796,15 @@
         <v>1</v>
       </c>
       <c r="J931" s="0" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="932" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A932" s="0" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="B932" s="0" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="C932" s="0" t="s">
         <v>293</v>
@@ -23808,15 +23813,15 @@
         <v>1</v>
       </c>
       <c r="J932" s="0" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="933" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A933" s="0" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="B933" s="0" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="C933" s="0" t="s">
         <v>293</v>
@@ -23825,15 +23830,15 @@
         <v>1</v>
       </c>
       <c r="J933" s="0" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="934" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A934" s="0" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="B934" s="0" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="C934" s="0" t="s">
         <v>293</v>
@@ -23842,15 +23847,15 @@
         <v>1</v>
       </c>
       <c r="J934" s="0" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="935" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A935" s="0" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="B935" s="0" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="C935" s="0" t="s">
         <v>293</v>
@@ -23859,15 +23864,15 @@
         <v>1</v>
       </c>
       <c r="J935" s="0" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="936" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A936" s="0" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="B936" s="0" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="C936" s="0" t="s">
         <v>293</v>
@@ -23876,15 +23881,15 @@
         <v>1</v>
       </c>
       <c r="J936" s="0" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="937" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A937" s="0" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="B937" s="0" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="C937" s="0" t="s">
         <v>293</v>
@@ -23893,15 +23898,15 @@
         <v>1</v>
       </c>
       <c r="J937" s="0" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="938" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A938" s="0" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="B938" s="0" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="C938" s="0" t="s">
         <v>293</v>
@@ -23910,7 +23915,7 @@
         <v>1</v>
       </c>
       <c r="J938" s="0" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="939" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23927,15 +23932,15 @@
         <v>1</v>
       </c>
       <c r="J939" s="0" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="940" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A940" s="0" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="B940" s="0" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="C940" s="0" t="s">
         <v>293</v>
@@ -23944,15 +23949,15 @@
         <v>1</v>
       </c>
       <c r="J940" s="0" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="941" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A941" s="0" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="B941" s="0" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="C941" s="0" t="s">
         <v>293</v>
@@ -23961,15 +23966,15 @@
         <v>1</v>
       </c>
       <c r="J941" s="0" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="942" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A942" s="0" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="B942" s="0" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="C942" s="0" t="s">
         <v>293</v>
@@ -23978,7 +23983,7 @@
         <v>1</v>
       </c>
       <c r="J942" s="0" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="943" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23986,7 +23991,7 @@
         <v>749</v>
       </c>
       <c r="B943" s="0" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="C943" s="0" t="s">
         <v>293</v>
@@ -23995,15 +24000,15 @@
         <v>1</v>
       </c>
       <c r="J943" s="0" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="944" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A944" s="0" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="B944" s="0" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="C944" s="0" t="s">
         <v>293</v>
@@ -24012,15 +24017,15 @@
         <v>1</v>
       </c>
       <c r="J944" s="0" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="945" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A945" s="0" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="B945" s="0" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="C945" s="0" t="s">
         <v>293</v>
@@ -24029,15 +24034,15 @@
         <v>1</v>
       </c>
       <c r="J945" s="0" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="946" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A946" s="0" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="B946" s="0" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="C946" s="0" t="s">
         <v>293</v>
@@ -24046,15 +24051,15 @@
         <v>1</v>
       </c>
       <c r="J946" s="0" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="947" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A947" s="0" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="B947" s="0" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="C947" s="0" t="s">
         <v>293</v>
@@ -24063,15 +24068,15 @@
         <v>1</v>
       </c>
       <c r="J947" s="0" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="948" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A948" s="0" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="B948" s="0" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="C948" s="0" t="s">
         <v>293</v>
@@ -24080,13 +24085,13 @@
         <v>1</v>
       </c>
       <c r="J948" s="0" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
1. Updated MOD_LASSO. It now uses a progress bar. Updated manual. Updated tests.
2. Slight updates to political units.

3. New knitrs about optimal string joining and political units.
</commit_message>
<xml_diff>
--- a/inst/extdata/political_units.xlsx
+++ b/inst/extdata/political_units.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2866" uniqueCount="1581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2869" uniqueCount="1582">
   <si>
     <t xml:space="preserve">Abbrev</t>
   </si>
@@ -4414,6 +4414,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ciudad Autónoma de Buenos Aires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buenos Aires DC</t>
   </si>
   <si>
     <t xml:space="preserve">Catamarca</t>
@@ -4776,7 +4779,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -4804,6 +4807,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4848,7 +4856,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4870,6 +4878,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4902,36 +4914,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.7551020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="18.8979591836735"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14184,10 +14196,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.2244897959184"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14441,23 +14451,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J948"/>
+  <dimension ref="A1:J949"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B894" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B879" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A894" activeCellId="0" sqref="A894"/>
-      <selection pane="bottomRight" activeCell="B919" activeCellId="0" sqref="B919"/>
+      <selection pane="bottomLeft" activeCell="A879" activeCellId="0" sqref="A879"/>
+      <selection pane="bottomRight" activeCell="G898" activeCellId="0" sqref="G898"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.1122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.280612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23291,11 +23299,11 @@
       </c>
     </row>
     <row r="898" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A898" s="0" t="s">
+      <c r="A898" s="6" t="s">
         <v>1464</v>
       </c>
       <c r="B898" s="0" t="s">
-        <v>1465</v>
+        <v>1462</v>
       </c>
       <c r="C898" s="0" t="s">
         <v>43</v>
@@ -23306,10 +23314,10 @@
     </row>
     <row r="899" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A899" s="0" t="s">
+        <v>1465</v>
+      </c>
+      <c r="B899" s="0" t="s">
         <v>1466</v>
-      </c>
-      <c r="B899" s="0" t="s">
-        <v>1467</v>
       </c>
       <c r="C899" s="0" t="s">
         <v>43</v>
@@ -23320,10 +23328,10 @@
     </row>
     <row r="900" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A900" s="0" t="s">
+        <v>1467</v>
+      </c>
+      <c r="B900" s="0" t="s">
         <v>1468</v>
-      </c>
-      <c r="B900" s="0" t="s">
-        <v>1469</v>
       </c>
       <c r="C900" s="0" t="s">
         <v>43</v>
@@ -23334,7 +23342,7 @@
     </row>
     <row r="901" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A901" s="0" t="s">
-        <v>731</v>
+        <v>1469</v>
       </c>
       <c r="B901" s="0" t="s">
         <v>1470</v>
@@ -23348,10 +23356,10 @@
     </row>
     <row r="902" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A902" s="0" t="s">
+        <v>731</v>
+      </c>
+      <c r="B902" s="0" t="s">
         <v>1471</v>
-      </c>
-      <c r="B902" s="0" t="s">
-        <v>1472</v>
       </c>
       <c r="C902" s="0" t="s">
         <v>43</v>
@@ -23362,10 +23370,10 @@
     </row>
     <row r="903" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A903" s="0" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B903" s="0" t="s">
         <v>1473</v>
-      </c>
-      <c r="B903" s="0" t="s">
-        <v>1474</v>
       </c>
       <c r="C903" s="0" t="s">
         <v>43</v>
@@ -23376,10 +23384,10 @@
     </row>
     <row r="904" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A904" s="0" t="s">
+        <v>1474</v>
+      </c>
+      <c r="B904" s="0" t="s">
         <v>1475</v>
-      </c>
-      <c r="B904" s="0" t="s">
-        <v>1476</v>
       </c>
       <c r="C904" s="0" t="s">
         <v>43</v>
@@ -23390,10 +23398,10 @@
     </row>
     <row r="905" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A905" s="0" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B905" s="0" t="s">
         <v>1477</v>
-      </c>
-      <c r="B905" s="0" t="s">
-        <v>1478</v>
       </c>
       <c r="C905" s="0" t="s">
         <v>43</v>
@@ -23404,10 +23412,10 @@
     </row>
     <row r="906" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A906" s="0" t="s">
+        <v>1478</v>
+      </c>
+      <c r="B906" s="0" t="s">
         <v>1479</v>
-      </c>
-      <c r="B906" s="0" t="s">
-        <v>1480</v>
       </c>
       <c r="C906" s="0" t="s">
         <v>43</v>
@@ -23418,10 +23426,10 @@
     </row>
     <row r="907" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A907" s="0" t="s">
+        <v>1480</v>
+      </c>
+      <c r="B907" s="0" t="s">
         <v>1481</v>
-      </c>
-      <c r="B907" s="0" t="s">
-        <v>1482</v>
       </c>
       <c r="C907" s="0" t="s">
         <v>43</v>
@@ -23432,10 +23440,10 @@
     </row>
     <row r="908" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A908" s="0" t="s">
+        <v>1482</v>
+      </c>
+      <c r="B908" s="0" t="s">
         <v>1483</v>
-      </c>
-      <c r="B908" s="0" t="s">
-        <v>1484</v>
       </c>
       <c r="C908" s="0" t="s">
         <v>43</v>
@@ -23446,10 +23454,10 @@
     </row>
     <row r="909" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A909" s="0" t="s">
+        <v>1484</v>
+      </c>
+      <c r="B909" s="0" t="s">
         <v>1485</v>
-      </c>
-      <c r="B909" s="0" t="s">
-        <v>1486</v>
       </c>
       <c r="C909" s="0" t="s">
         <v>43</v>
@@ -23460,10 +23468,10 @@
     </row>
     <row r="910" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A910" s="0" t="s">
+        <v>1486</v>
+      </c>
+      <c r="B910" s="0" t="s">
         <v>1487</v>
-      </c>
-      <c r="B910" s="0" t="s">
-        <v>1488</v>
       </c>
       <c r="C910" s="0" t="s">
         <v>43</v>
@@ -23474,10 +23482,10 @@
     </row>
     <row r="911" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A911" s="0" t="s">
+        <v>1488</v>
+      </c>
+      <c r="B911" s="0" t="s">
         <v>1489</v>
-      </c>
-      <c r="B911" s="0" t="s">
-        <v>1490</v>
       </c>
       <c r="C911" s="0" t="s">
         <v>43</v>
@@ -23488,10 +23496,10 @@
     </row>
     <row r="912" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A912" s="0" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B912" s="0" t="s">
         <v>1491</v>
-      </c>
-      <c r="B912" s="0" t="s">
-        <v>1492</v>
       </c>
       <c r="C912" s="0" t="s">
         <v>43</v>
@@ -23502,10 +23510,10 @@
     </row>
     <row r="913" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A913" s="0" t="s">
+        <v>1492</v>
+      </c>
+      <c r="B913" s="0" t="s">
         <v>1493</v>
-      </c>
-      <c r="B913" s="0" t="s">
-        <v>1494</v>
       </c>
       <c r="C913" s="0" t="s">
         <v>43</v>
@@ -23516,10 +23524,10 @@
     </row>
     <row r="914" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A914" s="0" t="s">
+        <v>1494</v>
+      </c>
+      <c r="B914" s="0" t="s">
         <v>1495</v>
-      </c>
-      <c r="B914" s="0" t="s">
-        <v>1496</v>
       </c>
       <c r="C914" s="0" t="s">
         <v>43</v>
@@ -23530,10 +23538,10 @@
     </row>
     <row r="915" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A915" s="0" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B915" s="0" t="s">
         <v>1497</v>
-      </c>
-      <c r="B915" s="0" t="s">
-        <v>1498</v>
       </c>
       <c r="C915" s="0" t="s">
         <v>43</v>
@@ -23544,10 +23552,10 @@
     </row>
     <row r="916" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A916" s="0" t="s">
+        <v>1498</v>
+      </c>
+      <c r="B916" s="0" t="s">
         <v>1499</v>
-      </c>
-      <c r="B916" s="0" t="s">
-        <v>1500</v>
       </c>
       <c r="C916" s="0" t="s">
         <v>43</v>
@@ -23558,10 +23566,10 @@
     </row>
     <row r="917" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A917" s="0" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B917" s="0" t="s">
         <v>1501</v>
-      </c>
-      <c r="B917" s="0" t="s">
-        <v>1502</v>
       </c>
       <c r="C917" s="0" t="s">
         <v>43</v>
@@ -23572,10 +23580,10 @@
     </row>
     <row r="918" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A918" s="0" t="s">
+        <v>1502</v>
+      </c>
+      <c r="B918" s="0" t="s">
         <v>1503</v>
-      </c>
-      <c r="B918" s="0" t="s">
-        <v>1504</v>
       </c>
       <c r="C918" s="0" t="s">
         <v>43</v>
@@ -23586,10 +23594,10 @@
     </row>
     <row r="919" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A919" s="0" t="s">
+        <v>1504</v>
+      </c>
+      <c r="B919" s="0" t="s">
         <v>1505</v>
-      </c>
-      <c r="B919" s="0" t="s">
-        <v>1506</v>
       </c>
       <c r="C919" s="0" t="s">
         <v>43</v>
@@ -23600,41 +23608,38 @@
     </row>
     <row r="920" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A920" s="0" t="s">
+        <v>1506</v>
+      </c>
+      <c r="B920" s="0" t="s">
         <v>1507</v>
       </c>
-      <c r="B920" s="0" t="s">
-        <v>1508</v>
-      </c>
       <c r="C920" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="J920" s="0" t="s">
-        <v>1509</v>
+        <v>43</v>
+      </c>
+      <c r="F920" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="921" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A921" s="0" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
       <c r="B921" s="0" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
       <c r="C921" s="0" t="s">
         <v>293</v>
       </c>
-      <c r="F921" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="J921" s="0" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="922" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A922" s="0" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
       <c r="B922" s="0" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="C922" s="0" t="s">
         <v>293</v>
@@ -23643,7 +23648,7 @@
         <v>1</v>
       </c>
       <c r="J922" s="0" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="923" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23651,7 +23656,7 @@
         <v>1514</v>
       </c>
       <c r="B923" s="0" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="C923" s="0" t="s">
         <v>293</v>
@@ -23660,15 +23665,15 @@
         <v>1</v>
       </c>
       <c r="J923" s="0" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="924" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A924" s="0" t="s">
-        <v>716</v>
+        <v>1515</v>
       </c>
       <c r="B924" s="0" t="s">
-        <v>1515</v>
+        <v>1512</v>
       </c>
       <c r="C924" s="0" t="s">
         <v>293</v>
@@ -23677,15 +23682,15 @@
         <v>1</v>
       </c>
       <c r="J924" s="0" t="s">
-        <v>1516</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="925" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A925" s="0" t="s">
-        <v>1517</v>
+        <v>716</v>
       </c>
       <c r="B925" s="0" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="C925" s="0" t="s">
         <v>293</v>
@@ -23694,7 +23699,7 @@
         <v>1</v>
       </c>
       <c r="J925" s="0" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="926" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23702,7 +23707,7 @@
         <v>1518</v>
       </c>
       <c r="B926" s="0" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="C926" s="0" t="s">
         <v>293</v>
@@ -23711,7 +23716,7 @@
         <v>1</v>
       </c>
       <c r="J926" s="0" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="927" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23719,7 +23724,7 @@
         <v>1519</v>
       </c>
       <c r="B927" s="0" t="s">
-        <v>1520</v>
+        <v>1516</v>
       </c>
       <c r="C927" s="0" t="s">
         <v>293</v>
@@ -23728,15 +23733,15 @@
         <v>1</v>
       </c>
       <c r="J927" s="0" t="s">
-        <v>1521</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="928" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A928" s="0" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="B928" s="0" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="C928" s="0" t="s">
         <v>293</v>
@@ -23745,15 +23750,15 @@
         <v>1</v>
       </c>
       <c r="J928" s="0" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="929" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A929" s="0" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
       <c r="B929" s="0" t="s">
-        <v>1526</v>
+        <v>1524</v>
       </c>
       <c r="C929" s="0" t="s">
         <v>293</v>
@@ -23762,15 +23767,15 @@
         <v>1</v>
       </c>
       <c r="J929" s="0" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="930" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A930" s="0" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
       <c r="B930" s="0" t="s">
-        <v>1529</v>
+        <v>1527</v>
       </c>
       <c r="C930" s="0" t="s">
         <v>293</v>
@@ -23779,15 +23784,15 @@
         <v>1</v>
       </c>
       <c r="J930" s="0" t="s">
-        <v>1530</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="931" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A931" s="0" t="s">
-        <v>722</v>
+        <v>1529</v>
       </c>
       <c r="B931" s="0" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="C931" s="0" t="s">
         <v>293</v>
@@ -23796,15 +23801,15 @@
         <v>1</v>
       </c>
       <c r="J931" s="0" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="932" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A932" s="0" t="s">
-        <v>1533</v>
+        <v>722</v>
       </c>
       <c r="B932" s="0" t="s">
-        <v>1534</v>
+        <v>1532</v>
       </c>
       <c r="C932" s="0" t="s">
         <v>293</v>
@@ -23813,15 +23818,15 @@
         <v>1</v>
       </c>
       <c r="J932" s="0" t="s">
-        <v>1535</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="933" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A933" s="0" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
       <c r="B933" s="0" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
       <c r="C933" s="0" t="s">
         <v>293</v>
@@ -23830,15 +23835,15 @@
         <v>1</v>
       </c>
       <c r="J933" s="0" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="934" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A934" s="0" t="s">
-        <v>1539</v>
+        <v>1537</v>
       </c>
       <c r="B934" s="0" t="s">
-        <v>1540</v>
+        <v>1538</v>
       </c>
       <c r="C934" s="0" t="s">
         <v>293</v>
@@ -23847,15 +23852,15 @@
         <v>1</v>
       </c>
       <c r="J934" s="0" t="s">
-        <v>1541</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="935" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A935" s="0" t="s">
-        <v>1542</v>
+        <v>1540</v>
       </c>
       <c r="B935" s="0" t="s">
-        <v>1543</v>
+        <v>1541</v>
       </c>
       <c r="C935" s="0" t="s">
         <v>293</v>
@@ -23864,15 +23869,15 @@
         <v>1</v>
       </c>
       <c r="J935" s="0" t="s">
-        <v>1544</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="936" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A936" s="0" t="s">
-        <v>1545</v>
+        <v>1543</v>
       </c>
       <c r="B936" s="0" t="s">
-        <v>1546</v>
+        <v>1544</v>
       </c>
       <c r="C936" s="0" t="s">
         <v>293</v>
@@ -23881,15 +23886,15 @@
         <v>1</v>
       </c>
       <c r="J936" s="0" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="937" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A937" s="0" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
       <c r="B937" s="0" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
       <c r="C937" s="0" t="s">
         <v>293</v>
@@ -23898,15 +23903,15 @@
         <v>1</v>
       </c>
       <c r="J937" s="0" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="938" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A938" s="0" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="B938" s="0" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="C938" s="0" t="s">
         <v>293</v>
@@ -23915,15 +23920,15 @@
         <v>1</v>
       </c>
       <c r="J938" s="0" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="939" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A939" s="0" t="s">
-        <v>1085</v>
+        <v>1552</v>
       </c>
       <c r="B939" s="0" t="s">
-        <v>1086</v>
+        <v>1553</v>
       </c>
       <c r="C939" s="0" t="s">
         <v>293</v>
@@ -23937,10 +23942,10 @@
     </row>
     <row r="940" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A940" s="0" t="s">
-        <v>1555</v>
+        <v>1085</v>
       </c>
       <c r="B940" s="0" t="s">
-        <v>1556</v>
+        <v>1086</v>
       </c>
       <c r="C940" s="0" t="s">
         <v>293</v>
@@ -23949,15 +23954,15 @@
         <v>1</v>
       </c>
       <c r="J940" s="0" t="s">
-        <v>1557</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="941" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A941" s="0" t="s">
-        <v>1558</v>
+        <v>1556</v>
       </c>
       <c r="B941" s="0" t="s">
-        <v>1559</v>
+        <v>1557</v>
       </c>
       <c r="C941" s="0" t="s">
         <v>293</v>
@@ -23966,15 +23971,15 @@
         <v>1</v>
       </c>
       <c r="J941" s="0" t="s">
-        <v>1560</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="942" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A942" s="0" t="s">
-        <v>1561</v>
+        <v>1559</v>
       </c>
       <c r="B942" s="0" t="s">
-        <v>1562</v>
+        <v>1560</v>
       </c>
       <c r="C942" s="0" t="s">
         <v>293</v>
@@ -23983,15 +23988,15 @@
         <v>1</v>
       </c>
       <c r="J942" s="0" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="943" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A943" s="0" t="s">
-        <v>749</v>
+        <v>1562</v>
       </c>
       <c r="B943" s="0" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="C943" s="0" t="s">
         <v>293</v>
@@ -24000,15 +24005,15 @@
         <v>1</v>
       </c>
       <c r="J943" s="0" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="944" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A944" s="0" t="s">
-        <v>1566</v>
+        <v>749</v>
       </c>
       <c r="B944" s="0" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
       <c r="C944" s="0" t="s">
         <v>293</v>
@@ -24017,15 +24022,15 @@
         <v>1</v>
       </c>
       <c r="J944" s="0" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="945" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A945" s="0" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="B945" s="0" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
       <c r="C945" s="0" t="s">
         <v>293</v>
@@ -24034,15 +24039,15 @@
         <v>1</v>
       </c>
       <c r="J945" s="0" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="946" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A946" s="0" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="B946" s="0" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
       <c r="C946" s="0" t="s">
         <v>293</v>
@@ -24051,15 +24056,15 @@
         <v>1</v>
       </c>
       <c r="J946" s="0" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="947" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A947" s="0" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="B947" s="0" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
       <c r="C947" s="0" t="s">
         <v>293</v>
@@ -24068,15 +24073,15 @@
         <v>1</v>
       </c>
       <c r="J947" s="0" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="948" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A948" s="0" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
       <c r="B948" s="0" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="C948" s="0" t="s">
         <v>293</v>
@@ -24085,7 +24090,24 @@
         <v>1</v>
       </c>
       <c r="J948" s="0" t="s">
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="949" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A949" s="0" t="s">
+        <v>1579</v>
+      </c>
+      <c r="B949" s="0" t="s">
         <v>1580</v>
+      </c>
+      <c r="C949" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="F949" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J949" s="0" t="s">
+        <v>1581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Added one missing German country name.
2. Renamed df_add_column_affix to df_add__affix. Removed the old names. This breaks any code, but this is a minor function.
</commit_message>
<xml_diff>
--- a/inst/extdata/political_units.xlsx
+++ b/inst/extdata/political_units.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3033" uniqueCount="1620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3036" uniqueCount="1621">
   <si>
     <t xml:space="preserve">Abbrev</t>
   </si>
@@ -3847,6 +3847,9 @@
   </si>
   <si>
     <t xml:space="preserve">Slovak Republic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slowakei</t>
   </si>
   <si>
     <t xml:space="preserve">Slovenia</t>
@@ -5027,36 +5030,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14309,8 +14311,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14564,21 +14568,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1009"/>
+  <dimension ref="A1:J1010"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B687" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E24" activeCellId="0" sqref="E24"/>
+      <selection pane="bottomLeft" activeCell="A687" activeCellId="0" sqref="A687"/>
+      <selection pane="bottomRight" activeCell="C713" activeCellId="0" sqref="C713"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.8163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21447,12 +21453,15 @@
         <v>261</v>
       </c>
     </row>
-    <row r="713" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A713" s="0" t="s">
+    <row r="713" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A713" s="5" t="s">
         <v>1275</v>
       </c>
       <c r="B713" s="0" t="s">
-        <v>262</v>
+        <v>261</v>
+      </c>
+      <c r="E713" s="0" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="714" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21462,27 +21471,27 @@
       <c r="B714" s="0" t="s">
         <v>262</v>
       </c>
-      <c r="E714" s="0" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="715" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A715" s="5" t="s">
+    </row>
+    <row r="715" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A715" s="0" t="s">
         <v>1277</v>
       </c>
       <c r="B715" s="0" t="s">
         <v>262</v>
       </c>
       <c r="E715" s="0" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="716" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A716" s="5" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B716" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="E716" s="0" t="s">
         <v>557</v>
-      </c>
-    </row>
-    <row r="716" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A716" s="0" t="s">
-        <v>1278</v>
-      </c>
-      <c r="B716" s="0" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="717" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21498,7 +21507,7 @@
         <v>1280</v>
       </c>
       <c r="B718" s="0" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="719" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21506,7 +21515,7 @@
         <v>1281</v>
       </c>
       <c r="B719" s="0" t="s">
-        <v>462</v>
+        <v>251</v>
       </c>
     </row>
     <row r="720" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21514,26 +21523,26 @@
         <v>1282</v>
       </c>
       <c r="B720" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="721" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A721" s="5" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="721" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A721" s="0" t="s">
         <v>1283</v>
       </c>
       <c r="B721" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="E721" s="0" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="722" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A722" s="0" t="s">
+    </row>
+    <row r="722" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A722" s="5" t="s">
         <v>1284</v>
       </c>
       <c r="B722" s="0" t="s">
         <v>305</v>
+      </c>
+      <c r="E722" s="0" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="723" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21543,9 +21552,6 @@
       <c r="B723" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="E723" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="724" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A724" s="0" t="s">
@@ -21554,6 +21560,9 @@
       <c r="B724" s="0" t="s">
         <v>305</v>
       </c>
+      <c r="E724" s="0" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="725" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A725" s="0" t="s">
@@ -21576,7 +21585,7 @@
         <v>1289</v>
       </c>
       <c r="B727" s="0" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="728" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21584,7 +21593,7 @@
         <v>1290</v>
       </c>
       <c r="B728" s="0" t="s">
-        <v>464</v>
+        <v>306</v>
       </c>
     </row>
     <row r="729" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21592,7 +21601,7 @@
         <v>1291</v>
       </c>
       <c r="B729" s="0" t="s">
-        <v>257</v>
+        <v>464</v>
       </c>
     </row>
     <row r="730" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21600,7 +21609,7 @@
         <v>1292</v>
       </c>
       <c r="B730" s="0" t="s">
-        <v>111</v>
+        <v>257</v>
       </c>
     </row>
     <row r="731" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21626,16 +21635,16 @@
       <c r="B733" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="E733" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="734" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A734" s="0" t="s">
         <v>1296</v>
       </c>
       <c r="B734" s="0" t="s">
-        <v>174</v>
+        <v>111</v>
+      </c>
+      <c r="E734" s="0" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="735" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21651,7 +21660,7 @@
         <v>1298</v>
       </c>
       <c r="B736" s="0" t="s">
-        <v>242</v>
+        <v>174</v>
       </c>
     </row>
     <row r="737" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21659,7 +21668,7 @@
         <v>1299</v>
       </c>
       <c r="B737" s="0" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
     </row>
     <row r="738" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21667,15 +21676,15 @@
         <v>1300</v>
       </c>
       <c r="B738" s="0" t="s">
-        <v>1301</v>
+        <v>260</v>
       </c>
     </row>
     <row r="739" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A739" s="0" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B739" s="0" t="s">
         <v>1302</v>
-      </c>
-      <c r="B739" s="0" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="740" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21683,7 +21692,7 @@
         <v>1303</v>
       </c>
       <c r="B740" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="741" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21693,9 +21702,6 @@
       <c r="B741" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="E741" s="0" t="s">
-        <v>824</v>
-      </c>
     </row>
     <row r="742" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A742" s="0" t="s">
@@ -21705,26 +21711,29 @@
         <v>263</v>
       </c>
       <c r="E742" s="0" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="743" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A743" s="5" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="743" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A743" s="0" t="s">
         <v>1306</v>
       </c>
       <c r="B743" s="0" t="s">
         <v>263</v>
       </c>
       <c r="E743" s="0" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="744" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A744" s="5" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B744" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="E744" s="0" t="s">
         <v>557</v>
-      </c>
-    </row>
-    <row r="744" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A744" s="0" t="s">
-        <v>1307</v>
-      </c>
-      <c r="B744" s="0" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="745" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21750,7 +21759,6 @@
       <c r="B747" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="E747" s="6"/>
     </row>
     <row r="748" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A748" s="0" t="s">
@@ -21759,15 +21767,13 @@
       <c r="B748" s="0" t="s">
         <v>77</v>
       </c>
+      <c r="E748" s="6"/>
     </row>
     <row r="749" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A749" s="0" t="s">
         <v>1312</v>
       </c>
       <c r="B749" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="C749" s="0" t="s">
         <v>77</v>
       </c>
     </row>
@@ -21776,7 +21782,7 @@
         <v>1313</v>
       </c>
       <c r="B750" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C750" s="0" t="s">
         <v>77</v>
@@ -21787,7 +21793,10 @@
         <v>1314</v>
       </c>
       <c r="B751" s="0" t="s">
-        <v>267</v>
+        <v>78</v>
+      </c>
+      <c r="C751" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="752" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21805,9 +21814,6 @@
       <c r="B753" s="0" t="s">
         <v>267</v>
       </c>
-      <c r="E753" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="754" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A754" s="0" t="s">
@@ -21816,13 +21822,16 @@
       <c r="B754" s="0" t="s">
         <v>267</v>
       </c>
+      <c r="E754" s="0" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="755" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A755" s="0" t="s">
         <v>1318</v>
       </c>
       <c r="B755" s="0" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
     </row>
     <row r="756" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21878,7 +21887,7 @@
         <v>1325</v>
       </c>
       <c r="B762" s="0" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
     </row>
     <row r="763" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21886,7 +21895,7 @@
         <v>1326</v>
       </c>
       <c r="B763" s="0" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
     </row>
     <row r="764" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21918,7 +21927,7 @@
         <v>1330</v>
       </c>
       <c r="B767" s="0" t="s">
-        <v>272</v>
+        <v>285</v>
       </c>
     </row>
     <row r="768" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21934,7 +21943,7 @@
         <v>1332</v>
       </c>
       <c r="B769" s="0" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="770" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21950,7 +21959,7 @@
         <v>1334</v>
       </c>
       <c r="B771" s="0" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="772" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21958,7 +21967,7 @@
         <v>1335</v>
       </c>
       <c r="B772" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="773" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21966,7 +21975,7 @@
         <v>1336</v>
       </c>
       <c r="B773" s="0" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="774" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21974,7 +21983,7 @@
         <v>1337</v>
       </c>
       <c r="B774" s="0" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="775" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21982,7 +21991,7 @@
         <v>1338</v>
       </c>
       <c r="B775" s="0" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="776" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21992,9 +22001,6 @@
       <c r="B776" s="0" t="s">
         <v>280</v>
       </c>
-      <c r="E776" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="777" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A777" s="0" t="s">
@@ -22003,6 +22009,9 @@
       <c r="B777" s="0" t="s">
         <v>280</v>
       </c>
+      <c r="E777" s="0" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="778" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A778" s="0" t="s">
@@ -22017,7 +22026,7 @@
         <v>1342</v>
       </c>
       <c r="B779" s="0" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="780" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22027,35 +22036,35 @@
       <c r="B780" s="0" t="s">
         <v>281</v>
       </c>
-      <c r="E780" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="781" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A781" s="0" t="s">
         <v>1344</v>
       </c>
       <c r="B781" s="0" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="782" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A782" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="E781" s="0" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="782" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A782" s="0" t="s">
         <v>1345</v>
       </c>
       <c r="B782" s="0" t="s">
         <v>282</v>
       </c>
-      <c r="E782" s="0" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="783" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A783" s="0" t="s">
+    </row>
+    <row r="783" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A783" s="5" t="s">
         <v>1346</v>
       </c>
       <c r="B783" s="0" t="s">
         <v>282</v>
+      </c>
+      <c r="E783" s="0" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="784" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22065,9 +22074,6 @@
       <c r="B784" s="0" t="s">
         <v>282</v>
       </c>
-      <c r="E784" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="785" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A785" s="0" t="s">
@@ -22076,15 +22082,15 @@
       <c r="B785" s="0" t="s">
         <v>282</v>
       </c>
+      <c r="E785" s="0" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="786" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A786" s="0" t="s">
         <v>1349</v>
       </c>
       <c r="B786" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="C786" s="0" t="s">
         <v>282</v>
       </c>
     </row>
@@ -22104,7 +22110,10 @@
         <v>1351</v>
       </c>
       <c r="B788" s="0" t="s">
-        <v>276</v>
+        <v>315</v>
+      </c>
+      <c r="C788" s="0" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="789" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22112,7 +22121,7 @@
         <v>1352</v>
       </c>
       <c r="B789" s="0" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
     </row>
     <row r="790" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22120,7 +22129,7 @@
         <v>1353</v>
       </c>
       <c r="B790" s="0" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="791" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22128,7 +22137,7 @@
         <v>1354</v>
       </c>
       <c r="B791" s="0" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="792" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22136,7 +22145,7 @@
         <v>1355</v>
       </c>
       <c r="B792" s="0" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="793" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22160,7 +22169,7 @@
         <v>1358</v>
       </c>
       <c r="B795" s="0" t="s">
-        <v>42</v>
+        <v>287</v>
       </c>
     </row>
     <row r="796" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22200,7 +22209,7 @@
         <v>1363</v>
       </c>
       <c r="B800" s="0" t="s">
-        <v>123</v>
+        <v>42</v>
       </c>
     </row>
     <row r="801" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22218,9 +22227,6 @@
       <c r="B802" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="E802" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="803" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A803" s="0" t="s">
@@ -22230,7 +22236,7 @@
         <v>123</v>
       </c>
       <c r="E803" s="0" t="s">
-        <v>824</v>
+        <v>549</v>
       </c>
     </row>
     <row r="804" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22240,6 +22246,9 @@
       <c r="B804" s="0" t="s">
         <v>123</v>
       </c>
+      <c r="E804" s="0" t="s">
+        <v>824</v>
+      </c>
     </row>
     <row r="805" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A805" s="0" t="s">
@@ -22249,23 +22258,23 @@
         <v>123</v>
       </c>
     </row>
-    <row r="806" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A806" s="5" t="s">
+    <row r="806" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A806" s="0" t="s">
         <v>1369</v>
       </c>
       <c r="B806" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="E806" s="0" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="807" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A807" s="0" t="s">
+    </row>
+    <row r="807" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A807" s="5" t="s">
         <v>1370</v>
       </c>
       <c r="B807" s="0" t="s">
         <v>123</v>
+      </c>
+      <c r="E807" s="0" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="808" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22273,9 +22282,6 @@
         <v>1371</v>
       </c>
       <c r="B808" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="C808" s="0" t="s">
         <v>123</v>
       </c>
     </row>
@@ -22295,7 +22301,7 @@
         <v>1373</v>
       </c>
       <c r="B810" s="0" t="s">
-        <v>241</v>
+        <v>108</v>
       </c>
       <c r="C810" s="0" t="s">
         <v>123</v>
@@ -22306,7 +22312,7 @@
         <v>1374</v>
       </c>
       <c r="B811" s="0" t="s">
-        <v>211</v>
+        <v>241</v>
       </c>
       <c r="C811" s="0" t="s">
         <v>123</v>
@@ -22317,20 +22323,23 @@
         <v>1375</v>
       </c>
       <c r="B812" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="C812" s="0" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="813" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A813" s="0" t="s">
-        <v>289</v>
+        <v>1376</v>
       </c>
       <c r="B813" s="0" t="s">
-        <v>289</v>
+        <v>123</v>
       </c>
     </row>
     <row r="814" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A814" s="0" t="s">
-        <v>1376</v>
+        <v>289</v>
       </c>
       <c r="B814" s="0" t="s">
         <v>289</v>
@@ -22365,21 +22374,12 @@
         <v>1380</v>
       </c>
       <c r="B818" s="0" t="s">
-        <v>1381</v>
-      </c>
-      <c r="C818" s="0" t="s">
         <v>289</v>
-      </c>
-      <c r="G818" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H818" s="0" t="s">
-        <v>1382</v>
       </c>
     </row>
     <row r="819" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A819" s="0" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="B819" s="0" t="s">
         <v>1382</v>
@@ -22387,13 +22387,19 @@
       <c r="C819" s="0" t="s">
         <v>289</v>
       </c>
+      <c r="G819" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H819" s="0" t="s">
+        <v>1383</v>
+      </c>
     </row>
     <row r="820" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A820" s="0" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B820" s="0" t="s">
         <v>1383</v>
-      </c>
-      <c r="B820" s="0" t="s">
-        <v>313</v>
       </c>
       <c r="C820" s="0" t="s">
         <v>289</v>
@@ -22404,13 +22410,10 @@
         <v>1384</v>
       </c>
       <c r="B821" s="0" t="s">
-        <v>407</v>
+        <v>313</v>
       </c>
       <c r="C821" s="0" t="s">
         <v>289</v>
-      </c>
-      <c r="F821" s="0" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="822" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22418,7 +22421,7 @@
         <v>1385</v>
       </c>
       <c r="B822" s="0" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C822" s="0" t="s">
         <v>289</v>
@@ -22432,7 +22435,7 @@
         <v>1386</v>
       </c>
       <c r="B823" s="0" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C823" s="0" t="s">
         <v>289</v>
@@ -22446,7 +22449,7 @@
         <v>1387</v>
       </c>
       <c r="B824" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C824" s="0" t="s">
         <v>289</v>
@@ -22460,7 +22463,7 @@
         <v>1388</v>
       </c>
       <c r="B825" s="0" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C825" s="0" t="s">
         <v>289</v>
@@ -22474,7 +22477,7 @@
         <v>1389</v>
       </c>
       <c r="B826" s="0" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C826" s="0" t="s">
         <v>289</v>
@@ -22488,7 +22491,7 @@
         <v>1390</v>
       </c>
       <c r="B827" s="0" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C827" s="0" t="s">
         <v>289</v>
@@ -22502,7 +22505,7 @@
         <v>1391</v>
       </c>
       <c r="B828" s="0" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C828" s="0" t="s">
         <v>289</v>
@@ -22516,7 +22519,7 @@
         <v>1392</v>
       </c>
       <c r="B829" s="0" t="s">
-        <v>1393</v>
+        <v>414</v>
       </c>
       <c r="C829" s="0" t="s">
         <v>289</v>
@@ -22527,10 +22530,10 @@
     </row>
     <row r="830" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A830" s="0" t="s">
+        <v>1393</v>
+      </c>
+      <c r="B830" s="0" t="s">
         <v>1394</v>
-      </c>
-      <c r="B830" s="0" t="s">
-        <v>415</v>
       </c>
       <c r="C830" s="0" t="s">
         <v>289</v>
@@ -22544,7 +22547,7 @@
         <v>1395</v>
       </c>
       <c r="B831" s="0" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C831" s="0" t="s">
         <v>289</v>
@@ -22572,7 +22575,7 @@
         <v>1397</v>
       </c>
       <c r="B833" s="0" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C833" s="0" t="s">
         <v>289</v>
@@ -22586,7 +22589,7 @@
         <v>1398</v>
       </c>
       <c r="B834" s="0" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C834" s="0" t="s">
         <v>289</v>
@@ -22600,7 +22603,7 @@
         <v>1399</v>
       </c>
       <c r="B835" s="0" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C835" s="0" t="s">
         <v>289</v>
@@ -22614,7 +22617,7 @@
         <v>1400</v>
       </c>
       <c r="B836" s="0" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C836" s="0" t="s">
         <v>289</v>
@@ -22628,7 +22631,7 @@
         <v>1401</v>
       </c>
       <c r="B837" s="0" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C837" s="0" t="s">
         <v>289</v>
@@ -22642,7 +22645,7 @@
         <v>1402</v>
       </c>
       <c r="B838" s="0" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C838" s="0" t="s">
         <v>289</v>
@@ -22656,7 +22659,7 @@
         <v>1403</v>
       </c>
       <c r="B839" s="0" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C839" s="0" t="s">
         <v>289</v>
@@ -22670,7 +22673,7 @@
         <v>1404</v>
       </c>
       <c r="B840" s="0" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C840" s="0" t="s">
         <v>289</v>
@@ -22684,7 +22687,7 @@
         <v>1405</v>
       </c>
       <c r="B841" s="0" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C841" s="0" t="s">
         <v>289</v>
@@ -22698,7 +22701,7 @@
         <v>1406</v>
       </c>
       <c r="B842" s="0" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C842" s="0" t="s">
         <v>289</v>
@@ -22712,7 +22715,7 @@
         <v>1407</v>
       </c>
       <c r="B843" s="0" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C843" s="0" t="s">
         <v>289</v>
@@ -22726,7 +22729,7 @@
         <v>1408</v>
       </c>
       <c r="B844" s="0" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C844" s="0" t="s">
         <v>289</v>
@@ -22740,7 +22743,7 @@
         <v>1409</v>
       </c>
       <c r="B845" s="0" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C845" s="0" t="s">
         <v>289</v>
@@ -22754,7 +22757,7 @@
         <v>1410</v>
       </c>
       <c r="B846" s="0" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C846" s="0" t="s">
         <v>289</v>
@@ -22768,7 +22771,7 @@
         <v>1411</v>
       </c>
       <c r="B847" s="0" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C847" s="0" t="s">
         <v>289</v>
@@ -22782,7 +22785,7 @@
         <v>1412</v>
       </c>
       <c r="B848" s="0" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C848" s="0" t="s">
         <v>289</v>
@@ -22796,7 +22799,7 @@
         <v>1413</v>
       </c>
       <c r="B849" s="0" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C849" s="0" t="s">
         <v>289</v>
@@ -22810,7 +22813,7 @@
         <v>1414</v>
       </c>
       <c r="B850" s="0" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C850" s="0" t="s">
         <v>289</v>
@@ -22824,7 +22827,7 @@
         <v>1415</v>
       </c>
       <c r="B851" s="0" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C851" s="0" t="s">
         <v>289</v>
@@ -22838,7 +22841,7 @@
         <v>1416</v>
       </c>
       <c r="B852" s="0" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C852" s="0" t="s">
         <v>289</v>
@@ -22852,7 +22855,7 @@
         <v>1417</v>
       </c>
       <c r="B853" s="0" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C853" s="0" t="s">
         <v>289</v>
@@ -22866,7 +22869,7 @@
         <v>1418</v>
       </c>
       <c r="B854" s="0" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C854" s="0" t="s">
         <v>289</v>
@@ -22880,7 +22883,7 @@
         <v>1419</v>
       </c>
       <c r="B855" s="0" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C855" s="0" t="s">
         <v>289</v>
@@ -22894,7 +22897,7 @@
         <v>1420</v>
       </c>
       <c r="B856" s="0" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C856" s="0" t="s">
         <v>289</v>
@@ -22908,7 +22911,7 @@
         <v>1421</v>
       </c>
       <c r="B857" s="0" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C857" s="0" t="s">
         <v>289</v>
@@ -22922,7 +22925,7 @@
         <v>1422</v>
       </c>
       <c r="B858" s="0" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C858" s="0" t="s">
         <v>289</v>
@@ -22936,7 +22939,7 @@
         <v>1423</v>
       </c>
       <c r="B859" s="0" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C859" s="0" t="s">
         <v>289</v>
@@ -22950,7 +22953,7 @@
         <v>1424</v>
       </c>
       <c r="B860" s="0" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C860" s="0" t="s">
         <v>289</v>
@@ -22964,7 +22967,7 @@
         <v>1425</v>
       </c>
       <c r="B861" s="0" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C861" s="0" t="s">
         <v>289</v>
@@ -22978,7 +22981,7 @@
         <v>1426</v>
       </c>
       <c r="B862" s="0" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C862" s="0" t="s">
         <v>289</v>
@@ -22992,7 +22995,7 @@
         <v>1427</v>
       </c>
       <c r="B863" s="0" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C863" s="0" t="s">
         <v>289</v>
@@ -23006,7 +23009,7 @@
         <v>1428</v>
       </c>
       <c r="B864" s="0" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C864" s="0" t="s">
         <v>289</v>
@@ -23020,7 +23023,7 @@
         <v>1429</v>
       </c>
       <c r="B865" s="0" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C865" s="0" t="s">
         <v>289</v>
@@ -23034,7 +23037,7 @@
         <v>1430</v>
       </c>
       <c r="B866" s="0" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C866" s="0" t="s">
         <v>289</v>
@@ -23048,7 +23051,7 @@
         <v>1431</v>
       </c>
       <c r="B867" s="0" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C867" s="0" t="s">
         <v>289</v>
@@ -23062,7 +23065,7 @@
         <v>1432</v>
       </c>
       <c r="B868" s="0" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C868" s="0" t="s">
         <v>289</v>
@@ -23076,7 +23079,7 @@
         <v>1433</v>
       </c>
       <c r="B869" s="0" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C869" s="0" t="s">
         <v>289</v>
@@ -23090,7 +23093,7 @@
         <v>1434</v>
       </c>
       <c r="B870" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C870" s="0" t="s">
         <v>289</v>
@@ -23104,7 +23107,7 @@
         <v>1435</v>
       </c>
       <c r="B871" s="0" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C871" s="0" t="s">
         <v>289</v>
@@ -23118,7 +23121,7 @@
         <v>1436</v>
       </c>
       <c r="B872" s="0" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C872" s="0" t="s">
         <v>289</v>
@@ -23132,7 +23135,13 @@
         <v>1437</v>
       </c>
       <c r="B873" s="0" t="s">
-        <v>288</v>
+        <v>456</v>
+      </c>
+      <c r="C873" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="F873" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="874" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23140,7 +23149,7 @@
         <v>1438</v>
       </c>
       <c r="B874" s="0" t="s">
-        <v>259</v>
+        <v>288</v>
       </c>
     </row>
     <row r="875" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23158,16 +23167,16 @@
       <c r="B876" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="E876" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="877" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A877" s="0" t="s">
         <v>1441</v>
       </c>
       <c r="B877" s="0" t="s">
-        <v>290</v>
+        <v>259</v>
+      </c>
+      <c r="E877" s="0" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="878" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23177,16 +23186,16 @@
       <c r="B878" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="E878" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="879" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A879" s="0" t="s">
         <v>1443</v>
       </c>
       <c r="B879" s="0" t="s">
-        <v>297</v>
+        <v>290</v>
+      </c>
+      <c r="E879" s="0" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="880" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23194,7 +23203,7 @@
         <v>1444</v>
       </c>
       <c r="B880" s="0" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="881" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23234,10 +23243,7 @@
         <v>1449</v>
       </c>
       <c r="B885" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="E885" s="0" t="s">
-        <v>549</v>
+        <v>293</v>
       </c>
     </row>
     <row r="886" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23247,30 +23253,21 @@
       <c r="B886" s="0" t="s">
         <v>296</v>
       </c>
+      <c r="E886" s="0" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="887" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A887" s="0" t="s">
         <v>1451</v>
       </c>
       <c r="B887" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="C887" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="G887" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H887" s="0" t="s">
-        <v>1452</v>
-      </c>
-      <c r="I887" s="0" t="s">
-        <v>1453</v>
+        <v>296</v>
       </c>
     </row>
     <row r="888" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A888" s="0" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="B888" s="0" t="s">
         <v>294</v>
@@ -23282,18 +23279,18 @@
         <v>1</v>
       </c>
       <c r="H888" s="0" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="I888" s="0" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="889" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A889" s="0" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="B889" s="0" t="s">
-        <v>1452</v>
+        <v>294</v>
       </c>
       <c r="C889" s="0" t="s">
         <v>123</v>
@@ -23302,30 +23299,30 @@
         <v>1</v>
       </c>
       <c r="H889" s="0" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="I889" s="0" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="890" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A890" s="0" t="s">
+        <v>1455</v>
+      </c>
+      <c r="B890" s="0" t="s">
+        <v>1453</v>
+      </c>
+      <c r="C890" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G890" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H890" s="0" t="s">
         <v>1456</v>
       </c>
-      <c r="B890" s="0" t="s">
-        <v>295</v>
-      </c>
-      <c r="C890" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="G890" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H890" s="0" t="s">
-        <v>1455</v>
-      </c>
       <c r="I890" s="0" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="891" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23342,10 +23339,10 @@
         <v>1</v>
       </c>
       <c r="H891" s="0" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="I891" s="0" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="892" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23362,10 +23359,10 @@
         <v>1</v>
       </c>
       <c r="H892" s="0" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="I892" s="0" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="893" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23382,10 +23379,10 @@
         <v>1</v>
       </c>
       <c r="H893" s="0" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="I893" s="0" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="894" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23402,10 +23399,10 @@
         <v>1</v>
       </c>
       <c r="H894" s="0" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="I894" s="0" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="895" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23422,10 +23419,10 @@
         <v>1</v>
       </c>
       <c r="H895" s="0" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="I895" s="0" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="896" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23442,10 +23439,10 @@
         <v>1</v>
       </c>
       <c r="H896" s="0" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="I896" s="0" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="897" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23462,29 +23459,41 @@
         <v>1</v>
       </c>
       <c r="H897" s="0" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="I897" s="0" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="898" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A898" s="0" t="s">
-        <v>1458</v>
+        <v>1464</v>
       </c>
       <c r="B898" s="0" t="s">
-        <v>1455</v>
+        <v>295</v>
       </c>
       <c r="C898" s="0" t="s">
         <v>289</v>
       </c>
+      <c r="G898" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H898" s="0" t="s">
+        <v>1456</v>
+      </c>
+      <c r="I898" s="0" t="s">
+        <v>1454</v>
+      </c>
     </row>
     <row r="899" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A899" s="0" t="s">
-        <v>1464</v>
+        <v>1459</v>
       </c>
       <c r="B899" s="0" t="s">
-        <v>300</v>
+        <v>1456</v>
+      </c>
+      <c r="C899" s="0" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="900" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23500,7 +23509,7 @@
         <v>1466</v>
       </c>
       <c r="B901" s="0" t="s">
-        <v>110</v>
+        <v>300</v>
       </c>
     </row>
     <row r="902" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23524,7 +23533,7 @@
         <v>1469</v>
       </c>
       <c r="B904" s="0" t="s">
-        <v>301</v>
+        <v>110</v>
       </c>
     </row>
     <row r="905" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23532,7 +23541,7 @@
         <v>1470</v>
       </c>
       <c r="B905" s="0" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="906" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23564,10 +23573,7 @@
         <v>1474</v>
       </c>
       <c r="B909" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="D909" s="0" t="n">
-        <v>1</v>
+        <v>302</v>
       </c>
     </row>
     <row r="910" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23597,7 +23603,7 @@
         <v>1477</v>
       </c>
       <c r="B912" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D912" s="0" t="n">
         <v>1</v>
@@ -23624,9 +23630,6 @@
       <c r="D914" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E914" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="915" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A915" s="0" t="s">
@@ -23638,13 +23641,19 @@
       <c r="D915" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E915" s="0" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="916" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A916" s="0" t="s">
         <v>1481</v>
       </c>
       <c r="B916" s="0" t="s">
-        <v>307</v>
+        <v>303</v>
+      </c>
+      <c r="D916" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="917" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23652,7 +23661,7 @@
         <v>1482</v>
       </c>
       <c r="B917" s="0" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="918" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23660,7 +23669,7 @@
         <v>1483</v>
       </c>
       <c r="B918" s="0" t="s">
-        <v>105</v>
+        <v>308</v>
       </c>
     </row>
     <row r="919" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23668,7 +23677,7 @@
         <v>1484</v>
       </c>
       <c r="B919" s="0" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="920" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23676,21 +23685,12 @@
         <v>1485</v>
       </c>
       <c r="B920" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="C920" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="G920" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H920" s="0" t="s">
-        <v>1486</v>
+        <v>114</v>
       </c>
     </row>
     <row r="921" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A921" s="0" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="B921" s="0" t="s">
         <v>76</v>
@@ -23702,7 +23702,7 @@
         <v>1</v>
       </c>
       <c r="H921" s="0" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="922" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23719,15 +23719,24 @@
         <v>1</v>
       </c>
       <c r="H922" s="0" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="923" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A923" s="0" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="B923" s="0" t="s">
-        <v>1486</v>
+        <v>76</v>
+      </c>
+      <c r="C923" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G923" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H923" s="0" t="s">
+        <v>1487</v>
       </c>
     </row>
     <row r="924" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23735,7 +23744,7 @@
         <v>1489</v>
       </c>
       <c r="B924" s="0" t="s">
-        <v>458</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="925" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23743,7 +23752,7 @@
         <v>1490</v>
       </c>
       <c r="B925" s="0" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="926" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23751,7 +23760,7 @@
         <v>1491</v>
       </c>
       <c r="B926" s="0" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="927" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23759,7 +23768,7 @@
         <v>1492</v>
       </c>
       <c r="B927" s="0" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="928" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23767,7 +23776,7 @@
         <v>1493</v>
       </c>
       <c r="B928" s="0" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="929" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23775,7 +23784,7 @@
         <v>1494</v>
       </c>
       <c r="B929" s="0" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="930" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23783,21 +23792,15 @@
         <v>1495</v>
       </c>
       <c r="B930" s="0" t="s">
-        <v>1496</v>
-      </c>
-      <c r="C930" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="F930" s="0" t="n">
-        <v>1</v>
+        <v>468</v>
       </c>
     </row>
     <row r="931" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A931" s="0" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B931" s="0" t="s">
         <v>1497</v>
-      </c>
-      <c r="B931" s="0" t="s">
-        <v>1498</v>
       </c>
       <c r="C931" s="0" t="s">
         <v>43</v>
@@ -23808,10 +23811,10 @@
     </row>
     <row r="932" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A932" s="0" t="s">
+        <v>1498</v>
+      </c>
+      <c r="B932" s="0" t="s">
         <v>1499</v>
-      </c>
-      <c r="B932" s="0" t="s">
-        <v>1498</v>
       </c>
       <c r="C932" s="0" t="s">
         <v>43</v>
@@ -23820,12 +23823,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="933" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A933" s="5" t="s">
+    <row r="933" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A933" s="0" t="s">
         <v>1500</v>
       </c>
       <c r="B933" s="0" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="C933" s="0" t="s">
         <v>43</v>
@@ -23834,12 +23837,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="934" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A934" s="7" t="s">
+    <row r="934" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A934" s="5" t="s">
         <v>1501</v>
       </c>
       <c r="B934" s="0" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="C934" s="0" t="s">
         <v>43</v>
@@ -23853,7 +23856,7 @@
         <v>1502</v>
       </c>
       <c r="B935" s="0" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="C935" s="0" t="s">
         <v>43</v>
@@ -23863,11 +23866,11 @@
       </c>
     </row>
     <row r="936" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A936" s="0" t="s">
+      <c r="A936" s="7" t="s">
         <v>1503</v>
       </c>
       <c r="B936" s="0" t="s">
-        <v>1504</v>
+        <v>1499</v>
       </c>
       <c r="C936" s="0" t="s">
         <v>43</v>
@@ -23878,10 +23881,10 @@
     </row>
     <row r="937" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A937" s="0" t="s">
+        <v>1504</v>
+      </c>
+      <c r="B937" s="0" t="s">
         <v>1505</v>
-      </c>
-      <c r="B937" s="0" t="s">
-        <v>1506</v>
       </c>
       <c r="C937" s="0" t="s">
         <v>43</v>
@@ -23892,10 +23895,10 @@
     </row>
     <row r="938" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A938" s="0" t="s">
+        <v>1506</v>
+      </c>
+      <c r="B938" s="0" t="s">
         <v>1507</v>
-      </c>
-      <c r="B938" s="0" t="s">
-        <v>1508</v>
       </c>
       <c r="C938" s="0" t="s">
         <v>43</v>
@@ -23906,7 +23909,7 @@
     </row>
     <row r="939" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A939" s="0" t="s">
-        <v>737</v>
+        <v>1508</v>
       </c>
       <c r="B939" s="0" t="s">
         <v>1509</v>
@@ -23920,10 +23923,10 @@
     </row>
     <row r="940" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A940" s="0" t="s">
+        <v>737</v>
+      </c>
+      <c r="B940" s="0" t="s">
         <v>1510</v>
-      </c>
-      <c r="B940" s="0" t="s">
-        <v>1511</v>
       </c>
       <c r="C940" s="0" t="s">
         <v>43</v>
@@ -23934,10 +23937,10 @@
     </row>
     <row r="941" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A941" s="0" t="s">
+        <v>1511</v>
+      </c>
+      <c r="B941" s="0" t="s">
         <v>1512</v>
-      </c>
-      <c r="B941" s="0" t="s">
-        <v>1513</v>
       </c>
       <c r="C941" s="0" t="s">
         <v>43</v>
@@ -23948,10 +23951,10 @@
     </row>
     <row r="942" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A942" s="0" t="s">
+        <v>1513</v>
+      </c>
+      <c r="B942" s="0" t="s">
         <v>1514</v>
-      </c>
-      <c r="B942" s="0" t="s">
-        <v>1515</v>
       </c>
       <c r="C942" s="0" t="s">
         <v>43</v>
@@ -23962,10 +23965,10 @@
     </row>
     <row r="943" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A943" s="0" t="s">
+        <v>1515</v>
+      </c>
+      <c r="B943" s="0" t="s">
         <v>1516</v>
-      </c>
-      <c r="B943" s="0" t="s">
-        <v>1517</v>
       </c>
       <c r="C943" s="0" t="s">
         <v>43</v>
@@ -23976,10 +23979,10 @@
     </row>
     <row r="944" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A944" s="0" t="s">
+        <v>1517</v>
+      </c>
+      <c r="B944" s="0" t="s">
         <v>1518</v>
-      </c>
-      <c r="B944" s="0" t="s">
-        <v>1519</v>
       </c>
       <c r="C944" s="0" t="s">
         <v>43</v>
@@ -23990,10 +23993,10 @@
     </row>
     <row r="945" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A945" s="0" t="s">
+        <v>1519</v>
+      </c>
+      <c r="B945" s="0" t="s">
         <v>1520</v>
-      </c>
-      <c r="B945" s="0" t="s">
-        <v>1521</v>
       </c>
       <c r="C945" s="0" t="s">
         <v>43</v>
@@ -24004,10 +24007,10 @@
     </row>
     <row r="946" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A946" s="0" t="s">
+        <v>1521</v>
+      </c>
+      <c r="B946" s="0" t="s">
         <v>1522</v>
-      </c>
-      <c r="B946" s="0" t="s">
-        <v>1523</v>
       </c>
       <c r="C946" s="0" t="s">
         <v>43</v>
@@ -24018,10 +24021,10 @@
     </row>
     <row r="947" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A947" s="0" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B947" s="0" t="s">
         <v>1524</v>
-      </c>
-      <c r="B947" s="0" t="s">
-        <v>1525</v>
       </c>
       <c r="C947" s="0" t="s">
         <v>43</v>
@@ -24032,10 +24035,10 @@
     </row>
     <row r="948" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A948" s="0" t="s">
+        <v>1525</v>
+      </c>
+      <c r="B948" s="0" t="s">
         <v>1526</v>
-      </c>
-      <c r="B948" s="0" t="s">
-        <v>1527</v>
       </c>
       <c r="C948" s="0" t="s">
         <v>43</v>
@@ -24046,10 +24049,10 @@
     </row>
     <row r="949" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A949" s="0" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B949" s="0" t="s">
         <v>1528</v>
-      </c>
-      <c r="B949" s="0" t="s">
-        <v>1529</v>
       </c>
       <c r="C949" s="0" t="s">
         <v>43</v>
@@ -24060,10 +24063,10 @@
     </row>
     <row r="950" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A950" s="0" t="s">
+        <v>1529</v>
+      </c>
+      <c r="B950" s="0" t="s">
         <v>1530</v>
-      </c>
-      <c r="B950" s="0" t="s">
-        <v>1531</v>
       </c>
       <c r="C950" s="0" t="s">
         <v>43</v>
@@ -24074,10 +24077,10 @@
     </row>
     <row r="951" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A951" s="0" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B951" s="0" t="s">
         <v>1532</v>
-      </c>
-      <c r="B951" s="0" t="s">
-        <v>1533</v>
       </c>
       <c r="C951" s="0" t="s">
         <v>43</v>
@@ -24088,10 +24091,10 @@
     </row>
     <row r="952" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A952" s="0" t="s">
+        <v>1533</v>
+      </c>
+      <c r="B952" s="0" t="s">
         <v>1534</v>
-      </c>
-      <c r="B952" s="0" t="s">
-        <v>1535</v>
       </c>
       <c r="C952" s="0" t="s">
         <v>43</v>
@@ -24102,10 +24105,10 @@
     </row>
     <row r="953" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A953" s="0" t="s">
+        <v>1535</v>
+      </c>
+      <c r="B953" s="0" t="s">
         <v>1536</v>
-      </c>
-      <c r="B953" s="0" t="s">
-        <v>1537</v>
       </c>
       <c r="C953" s="0" t="s">
         <v>43</v>
@@ -24116,10 +24119,10 @@
     </row>
     <row r="954" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A954" s="0" t="s">
+        <v>1537</v>
+      </c>
+      <c r="B954" s="0" t="s">
         <v>1538</v>
-      </c>
-      <c r="B954" s="0" t="s">
-        <v>1539</v>
       </c>
       <c r="C954" s="0" t="s">
         <v>43</v>
@@ -24130,10 +24133,10 @@
     </row>
     <row r="955" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A955" s="0" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B955" s="0" t="s">
         <v>1540</v>
-      </c>
-      <c r="B955" s="0" t="s">
-        <v>1541</v>
       </c>
       <c r="C955" s="0" t="s">
         <v>43</v>
@@ -24144,10 +24147,10 @@
     </row>
     <row r="956" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A956" s="0" t="s">
+        <v>1541</v>
+      </c>
+      <c r="B956" s="0" t="s">
         <v>1542</v>
-      </c>
-      <c r="B956" s="0" t="s">
-        <v>1543</v>
       </c>
       <c r="C956" s="0" t="s">
         <v>43</v>
@@ -24158,10 +24161,10 @@
     </row>
     <row r="957" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A957" s="0" t="s">
+        <v>1543</v>
+      </c>
+      <c r="B957" s="0" t="s">
         <v>1544</v>
-      </c>
-      <c r="B957" s="0" t="s">
-        <v>1545</v>
       </c>
       <c r="C957" s="0" t="s">
         <v>43</v>
@@ -24171,11 +24174,11 @@
       </c>
     </row>
     <row r="958" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A958" s="0" t="n">
-        <v>1701</v>
+      <c r="A958" s="0" t="s">
+        <v>1545</v>
       </c>
       <c r="B958" s="0" t="s">
-        <v>1498</v>
+        <v>1546</v>
       </c>
       <c r="C958" s="0" t="s">
         <v>43</v>
@@ -24186,10 +24189,10 @@
     </row>
     <row r="959" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A959" s="0" t="n">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="B959" s="0" t="s">
-        <v>1509</v>
+        <v>1499</v>
       </c>
       <c r="C959" s="0" t="s">
         <v>43</v>
@@ -24200,10 +24203,10 @@
     </row>
     <row r="960" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A960" s="0" t="n">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="B960" s="0" t="s">
-        <v>1539</v>
+        <v>1510</v>
       </c>
       <c r="C960" s="0" t="s">
         <v>43</v>
@@ -24214,10 +24217,10 @@
     </row>
     <row r="961" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A961" s="0" t="n">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="B961" s="0" t="s">
-        <v>1513</v>
+        <v>1540</v>
       </c>
       <c r="C961" s="0" t="s">
         <v>43</v>
@@ -24228,10 +24231,10 @@
     </row>
     <row r="962" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A962" s="0" t="n">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="B962" s="0" t="s">
-        <v>1525</v>
+        <v>1514</v>
       </c>
       <c r="C962" s="0" t="s">
         <v>43</v>
@@ -24242,10 +24245,10 @@
     </row>
     <row r="963" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A963" s="0" t="n">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="B963" s="0" t="s">
-        <v>1511</v>
+        <v>1526</v>
       </c>
       <c r="C963" s="0" t="s">
         <v>43</v>
@@ -24256,10 +24259,10 @@
     </row>
     <row r="964" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A964" s="0" t="n">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="B964" s="0" t="s">
-        <v>1506</v>
+        <v>1512</v>
       </c>
       <c r="C964" s="0" t="s">
         <v>43</v>
@@ -24270,10 +24273,10 @@
     </row>
     <row r="965" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A965" s="0" t="n">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B965" s="0" t="s">
-        <v>1515</v>
+        <v>1507</v>
       </c>
       <c r="C965" s="0" t="s">
         <v>43</v>
@@ -24284,10 +24287,10 @@
     </row>
     <row r="966" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A966" s="0" t="n">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="B966" s="0" t="s">
-        <v>1531</v>
+        <v>1516</v>
       </c>
       <c r="C966" s="0" t="s">
         <v>43</v>
@@ -24298,10 +24301,10 @@
     </row>
     <row r="967" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A967" s="0" t="n">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="B967" s="0" t="s">
-        <v>1541</v>
+        <v>1532</v>
       </c>
       <c r="C967" s="0" t="s">
         <v>43</v>
@@ -24312,10 +24315,10 @@
     </row>
     <row r="968" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A968" s="0" t="n">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="B968" s="0" t="s">
-        <v>1545</v>
+        <v>1542</v>
       </c>
       <c r="C968" s="0" t="s">
         <v>43</v>
@@ -24326,10 +24329,10 @@
     </row>
     <row r="969" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A969" s="0" t="n">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="B969" s="0" t="s">
-        <v>1504</v>
+        <v>1546</v>
       </c>
       <c r="C969" s="0" t="s">
         <v>43</v>
@@ -24340,10 +24343,10 @@
     </row>
     <row r="970" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A970" s="0" t="n">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="B970" s="0" t="s">
-        <v>1517</v>
+        <v>1505</v>
       </c>
       <c r="C970" s="0" t="s">
         <v>43</v>
@@ -24354,10 +24357,10 @@
     </row>
     <row r="971" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A971" s="0" t="n">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="B971" s="0" t="s">
-        <v>1523</v>
+        <v>1518</v>
       </c>
       <c r="C971" s="0" t="s">
         <v>43</v>
@@ -24368,10 +24371,10 @@
     </row>
     <row r="972" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A972" s="0" t="n">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="B972" s="0" t="s">
-        <v>1533</v>
+        <v>1524</v>
       </c>
       <c r="C972" s="0" t="s">
         <v>43</v>
@@ -24382,10 +24385,10 @@
     </row>
     <row r="973" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A973" s="0" t="n">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="B973" s="0" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="C973" s="0" t="s">
         <v>43</v>
@@ -24396,10 +24399,10 @@
     </row>
     <row r="974" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A974" s="0" t="n">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="B974" s="0" t="s">
-        <v>1521</v>
+        <v>1536</v>
       </c>
       <c r="C974" s="0" t="s">
         <v>43</v>
@@ -24410,10 +24413,10 @@
     </row>
     <row r="975" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A975" s="0" t="n">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="B975" s="0" t="s">
-        <v>1508</v>
+        <v>1522</v>
       </c>
       <c r="C975" s="0" t="s">
         <v>43</v>
@@ -24424,10 +24427,10 @@
     </row>
     <row r="976" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A976" s="0" t="n">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="B976" s="0" t="s">
-        <v>1527</v>
+        <v>1509</v>
       </c>
       <c r="C976" s="0" t="s">
         <v>43</v>
@@ -24438,10 +24441,10 @@
     </row>
     <row r="977" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A977" s="0" t="n">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="B977" s="0" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="C977" s="0" t="s">
         <v>43</v>
@@ -24452,10 +24455,10 @@
     </row>
     <row r="978" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A978" s="0" t="n">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="B978" s="0" t="s">
-        <v>1543</v>
+        <v>1530</v>
       </c>
       <c r="C978" s="0" t="s">
         <v>43</v>
@@ -24466,10 +24469,10 @@
     </row>
     <row r="979" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A979" s="0" t="n">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="B979" s="0" t="s">
-        <v>1496</v>
+        <v>1544</v>
       </c>
       <c r="C979" s="0" t="s">
         <v>43</v>
@@ -24480,10 +24483,10 @@
     </row>
     <row r="980" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A980" s="0" t="n">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="B980" s="0" t="s">
-        <v>1519</v>
+        <v>1497</v>
       </c>
       <c r="C980" s="0" t="s">
         <v>43</v>
@@ -24493,42 +24496,39 @@
       </c>
     </row>
     <row r="981" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A981" s="0" t="s">
-        <v>1546</v>
+      <c r="A981" s="0" t="n">
+        <v>1723</v>
       </c>
       <c r="B981" s="0" t="s">
-        <v>1547</v>
+        <v>1520</v>
       </c>
       <c r="C981" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="J981" s="0" t="s">
-        <v>1548</v>
+        <v>43</v>
+      </c>
+      <c r="F981" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="982" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A982" s="0" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
       <c r="B982" s="0" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
       <c r="C982" s="0" t="s">
         <v>293</v>
       </c>
-      <c r="F982" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="J982" s="0" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="983" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A983" s="0" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="B983" s="0" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="C983" s="0" t="s">
         <v>293</v>
@@ -24537,7 +24537,7 @@
         <v>1</v>
       </c>
       <c r="J983" s="0" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="984" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24545,7 +24545,7 @@
         <v>1553</v>
       </c>
       <c r="B984" s="0" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="C984" s="0" t="s">
         <v>293</v>
@@ -24554,15 +24554,15 @@
         <v>1</v>
       </c>
       <c r="J984" s="0" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="985" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A985" s="0" t="s">
-        <v>722</v>
+        <v>1554</v>
       </c>
       <c r="B985" s="0" t="s">
-        <v>1554</v>
+        <v>1551</v>
       </c>
       <c r="C985" s="0" t="s">
         <v>293</v>
@@ -24571,15 +24571,15 @@
         <v>1</v>
       </c>
       <c r="J985" s="0" t="s">
-        <v>1555</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="986" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A986" s="0" t="s">
-        <v>1556</v>
+        <v>722</v>
       </c>
       <c r="B986" s="0" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="C986" s="0" t="s">
         <v>293</v>
@@ -24588,7 +24588,7 @@
         <v>1</v>
       </c>
       <c r="J986" s="0" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="987" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24596,7 +24596,7 @@
         <v>1557</v>
       </c>
       <c r="B987" s="0" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="C987" s="0" t="s">
         <v>293</v>
@@ -24605,7 +24605,7 @@
         <v>1</v>
       </c>
       <c r="J987" s="0" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="988" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24613,7 +24613,7 @@
         <v>1558</v>
       </c>
       <c r="B988" s="0" t="s">
-        <v>1559</v>
+        <v>1555</v>
       </c>
       <c r="C988" s="0" t="s">
         <v>293</v>
@@ -24622,15 +24622,15 @@
         <v>1</v>
       </c>
       <c r="J988" s="0" t="s">
-        <v>1560</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="989" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A989" s="0" t="s">
-        <v>1561</v>
+        <v>1559</v>
       </c>
       <c r="B989" s="0" t="s">
-        <v>1562</v>
+        <v>1560</v>
       </c>
       <c r="C989" s="0" t="s">
         <v>293</v>
@@ -24639,15 +24639,15 @@
         <v>1</v>
       </c>
       <c r="J989" s="0" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="990" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A990" s="0" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
       <c r="B990" s="0" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
       <c r="C990" s="0" t="s">
         <v>293</v>
@@ -24656,15 +24656,15 @@
         <v>1</v>
       </c>
       <c r="J990" s="0" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="991" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A991" s="0" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
       <c r="B991" s="0" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="C991" s="0" t="s">
         <v>293</v>
@@ -24673,15 +24673,15 @@
         <v>1</v>
       </c>
       <c r="J991" s="0" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="992" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A992" s="0" t="s">
-        <v>728</v>
+        <v>1568</v>
       </c>
       <c r="B992" s="0" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="C992" s="0" t="s">
         <v>293</v>
@@ -24690,15 +24690,15 @@
         <v>1</v>
       </c>
       <c r="J992" s="0" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="993" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A993" s="0" t="s">
-        <v>1572</v>
+        <v>728</v>
       </c>
       <c r="B993" s="0" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
       <c r="C993" s="0" t="s">
         <v>293</v>
@@ -24707,15 +24707,15 @@
         <v>1</v>
       </c>
       <c r="J993" s="0" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="994" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A994" s="0" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="B994" s="0" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
       <c r="C994" s="0" t="s">
         <v>293</v>
@@ -24724,15 +24724,15 @@
         <v>1</v>
       </c>
       <c r="J994" s="0" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="995" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A995" s="0" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
       <c r="B995" s="0" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="C995" s="0" t="s">
         <v>293</v>
@@ -24741,15 +24741,15 @@
         <v>1</v>
       </c>
       <c r="J995" s="0" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="996" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A996" s="0" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
       <c r="B996" s="0" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="C996" s="0" t="s">
         <v>293</v>
@@ -24758,15 +24758,15 @@
         <v>1</v>
       </c>
       <c r="J996" s="0" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="997" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A997" s="0" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="B997" s="0" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="C997" s="0" t="s">
         <v>293</v>
@@ -24775,15 +24775,15 @@
         <v>1</v>
       </c>
       <c r="J997" s="0" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="998" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A998" s="0" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="B998" s="0" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
       <c r="C998" s="0" t="s">
         <v>293</v>
@@ -24792,15 +24792,15 @@
         <v>1</v>
       </c>
       <c r="J998" s="0" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="999" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A999" s="0" t="s">
-        <v>1590</v>
+        <v>1588</v>
       </c>
       <c r="B999" s="0" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
       <c r="C999" s="0" t="s">
         <v>293</v>
@@ -24809,15 +24809,15 @@
         <v>1</v>
       </c>
       <c r="J999" s="0" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="1000" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1000" s="0" t="s">
-        <v>1108</v>
+        <v>1591</v>
       </c>
       <c r="B1000" s="0" t="s">
-        <v>1109</v>
+        <v>1592</v>
       </c>
       <c r="C1000" s="0" t="s">
         <v>293</v>
@@ -24831,10 +24831,10 @@
     </row>
     <row r="1001" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1001" s="0" t="s">
-        <v>1594</v>
+        <v>1108</v>
       </c>
       <c r="B1001" s="0" t="s">
-        <v>1595</v>
+        <v>1109</v>
       </c>
       <c r="C1001" s="0" t="s">
         <v>293</v>
@@ -24843,15 +24843,15 @@
         <v>1</v>
       </c>
       <c r="J1001" s="0" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="1002" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1002" s="0" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
       <c r="B1002" s="0" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
       <c r="C1002" s="0" t="s">
         <v>293</v>
@@ -24860,15 +24860,15 @@
         <v>1</v>
       </c>
       <c r="J1002" s="0" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="1003" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1003" s="0" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
       <c r="B1003" s="0" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
       <c r="C1003" s="0" t="s">
         <v>293</v>
@@ -24877,15 +24877,15 @@
         <v>1</v>
       </c>
       <c r="J1003" s="0" t="s">
-        <v>1602</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="1004" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1004" s="0" t="s">
-        <v>755</v>
+        <v>1601</v>
       </c>
       <c r="B1004" s="0" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="C1004" s="0" t="s">
         <v>293</v>
@@ -24894,15 +24894,15 @@
         <v>1</v>
       </c>
       <c r="J1004" s="0" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="1005" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1005" s="0" t="s">
-        <v>1605</v>
+        <v>755</v>
       </c>
       <c r="B1005" s="0" t="s">
-        <v>1606</v>
+        <v>1604</v>
       </c>
       <c r="C1005" s="0" t="s">
         <v>293</v>
@@ -24911,15 +24911,15 @@
         <v>1</v>
       </c>
       <c r="J1005" s="0" t="s">
-        <v>1607</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="1006" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1006" s="0" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
       <c r="B1006" s="0" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="C1006" s="0" t="s">
         <v>293</v>
@@ -24928,15 +24928,15 @@
         <v>1</v>
       </c>
       <c r="J1006" s="0" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="1007" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1007" s="0" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
       <c r="B1007" s="0" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
       <c r="C1007" s="0" t="s">
         <v>293</v>
@@ -24945,15 +24945,15 @@
         <v>1</v>
       </c>
       <c r="J1007" s="0" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="1008" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1008" s="0" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
       <c r="B1008" s="0" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
       <c r="C1008" s="0" t="s">
         <v>293</v>
@@ -24962,15 +24962,15 @@
         <v>1</v>
       </c>
       <c r="J1008" s="0" t="s">
-        <v>1616</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="1009" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1009" s="0" t="s">
-        <v>1617</v>
+        <v>1615</v>
       </c>
       <c r="B1009" s="0" t="s">
-        <v>1618</v>
+        <v>1616</v>
       </c>
       <c r="C1009" s="0" t="s">
         <v>293</v>
@@ -24979,7 +24979,24 @@
         <v>1</v>
       </c>
       <c r="J1009" s="0" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="1010" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1010" s="0" t="s">
+        <v>1618</v>
+      </c>
+      <c r="B1010" s="0" t="s">
         <v>1619</v>
+      </c>
+      <c r="C1010" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="F1010" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J1010" s="0" t="s">
+        <v>1620</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reordered a few names to get better standard names. E.g. "South Korea" instead of "Korea, Republic of".
</commit_message>
<xml_diff>
--- a/inst/extdata/political_units.xlsx
+++ b/inst/extdata/political_units.xlsx
@@ -2475,12 +2475,12 @@
     <t xml:space="preserve">Tsjekkia</t>
   </si>
   <si>
+    <t xml:space="preserve">Czechslovakia</t>
+  </si>
+  <si>
     <t xml:space="preserve">Czechoslov.</t>
   </si>
   <si>
-    <t xml:space="preserve">Czechslovakia</t>
-  </si>
-  <si>
     <t xml:space="preserve">Czechoslovakia</t>
   </si>
   <si>
@@ -2937,6 +2937,9 @@
     <t xml:space="preserve">Kosovo</t>
   </si>
   <si>
+    <t xml:space="preserve">North Korea</t>
+  </si>
+  <si>
     <t xml:space="preserve">Korea Democratic People's Republic of</t>
   </si>
   <si>
@@ -2949,9 +2952,6 @@
     <t xml:space="preserve">Korea North</t>
   </si>
   <si>
-    <t xml:space="preserve">North Korea</t>
-  </si>
-  <si>
     <t xml:space="preserve">Korea, North is missing</t>
   </si>
   <si>
@@ -2973,6 +2973,9 @@
     <t xml:space="preserve">Nordkorea</t>
   </si>
   <si>
+    <t xml:space="preserve">South Korea</t>
+  </si>
+  <si>
     <t xml:space="preserve">Korea Republic of</t>
   </si>
   <si>
@@ -3001,9 +3004,6 @@
   </si>
   <si>
     <t xml:space="preserve">Korea, South</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Korea</t>
   </si>
   <si>
     <t xml:space="preserve">Soer-Korea</t>
@@ -5030,35 +5030,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14311,10 +14312,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14571,20 +14572,20 @@
   <dimension ref="A1:J1010"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B687" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B242" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A687" activeCellId="0" sqref="A687"/>
-      <selection pane="bottomRight" activeCell="C713" activeCellId="0" sqref="C713"/>
+      <selection pane="bottomLeft" activeCell="A242" activeCellId="0" sqref="A242"/>
+      <selection pane="bottomRight" activeCell="A265" activeCellId="0" sqref="A265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17327,7 +17328,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="270" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="270" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="5" t="s">
         <v>825</v>
       </c>
@@ -17477,7 +17478,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="288" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="288" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="5" t="s">
         <v>843</v>
       </c>
@@ -17566,7 +17567,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="298" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="298" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="5" t="s">
         <v>853</v>
       </c>
@@ -17658,7 +17659,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="308" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="308" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="5" t="s">
         <v>863</v>
       </c>
@@ -17715,7 +17716,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="314" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="314" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="5" t="s">
         <v>869</v>
       </c>
@@ -17876,7 +17877,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="333" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="333" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="5" t="s">
         <v>889</v>
       </c>
@@ -18004,7 +18005,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="346" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="346" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="5" t="s">
         <v>903</v>
       </c>
@@ -18553,7 +18554,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="406" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="406" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="5" t="s">
         <v>964</v>
       </c>
@@ -18583,7 +18584,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="409" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="409" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="5" t="s">
         <v>967</v>
       </c>
@@ -18733,23 +18734,23 @@
         <v>165</v>
       </c>
     </row>
-    <row r="427" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A427" s="5" t="s">
+    <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A427" s="0" t="s">
         <v>985</v>
       </c>
       <c r="B427" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="E427" s="0" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A428" s="0" t="s">
+    </row>
+    <row r="428" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A428" s="5" t="s">
         <v>986</v>
       </c>
       <c r="B428" s="0" t="s">
         <v>165</v>
+      </c>
+      <c r="E428" s="0" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18945,7 +18946,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="452" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="452" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="5" t="s">
         <v>1010</v>
       </c>
@@ -19091,7 +19092,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="468" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="468" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="5" t="s">
         <v>1026</v>
       </c>
@@ -19232,7 +19233,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="483" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="483" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="5" t="s">
         <v>1041</v>
       </c>
@@ -20022,7 +20023,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="551" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="551" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A551" s="5" t="s">
         <v>1112</v>
       </c>
@@ -20228,7 +20229,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="576" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="576" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A576" s="5" t="s">
         <v>1137</v>
       </c>
@@ -20600,7 +20601,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="618" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="618" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A618" s="5" t="s">
         <v>1180</v>
       </c>
@@ -20831,7 +20832,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="642" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="642" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A642" s="5" t="s">
         <v>1204</v>
       </c>
@@ -20877,7 +20878,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="647" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="647" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A647" s="5" t="s">
         <v>1209</v>
       </c>
@@ -21453,7 +21454,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="713" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="713" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A713" s="5" t="s">
         <v>1275</v>
       </c>
@@ -21483,7 +21484,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="716" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="716" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A716" s="5" t="s">
         <v>1278</v>
       </c>
@@ -21534,7 +21535,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="722" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="722" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A722" s="5" t="s">
         <v>1284</v>
       </c>
@@ -22056,7 +22057,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="783" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="783" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A783" s="5" t="s">
         <v>1346</v>
       </c>

</xml_diff>

<commit_message>
Small update to PU data
</commit_message>
<xml_diff>
--- a/inst/extdata/political_units.xlsx
+++ b/inst/extdata/political_units.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3039" uniqueCount="1621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3043" uniqueCount="1622">
   <si>
     <t xml:space="preserve">Abbrev</t>
   </si>
@@ -3507,6 +3507,9 @@
     <t xml:space="preserve">Palau</t>
   </si>
   <si>
+    <t xml:space="preserve">Occupied Palestinian Territory</t>
+  </si>
+  <si>
     <t xml:space="preserve">Palestine, State of</t>
   </si>
   <si>
@@ -3519,9 +3522,6 @@
     <t xml:space="preserve">Palestina</t>
   </si>
   <si>
-    <t xml:space="preserve">Occupied Palestinian Territory</t>
-  </si>
-  <si>
     <t xml:space="preserve">West Bank and Gaza</t>
   </si>
   <si>
@@ -3538,6 +3538,9 @@
   </si>
   <si>
     <t xml:space="preserve">Palæstina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palästinensische Gebiete</t>
   </si>
   <si>
     <t xml:space="preserve">Gaza Strip</t>
@@ -5030,33 +5033,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14309,10 +14315,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1989795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14566,23 +14570,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1011"/>
+  <dimension ref="A1:J1012"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B76" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B718" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A76" activeCellId="0" sqref="A76"/>
-      <selection pane="bottomRight" activeCell="F87" activeCellId="0" sqref="F87"/>
+      <selection pane="bottomLeft" activeCell="A718" activeCellId="0" sqref="A718"/>
+      <selection pane="bottomRight" activeCell="A766" activeCellId="0" sqref="A766"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3877551020408"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20517,6 +20519,9 @@
       <c r="B607" s="0" t="s">
         <v>232</v>
       </c>
+      <c r="E607" s="0" t="s">
+        <v>824</v>
+      </c>
     </row>
     <row r="608" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A608" s="0" t="s">
@@ -20553,7 +20558,10 @@
         <v>1172</v>
       </c>
       <c r="B611" s="0" t="s">
-        <v>122</v>
+        <v>232</v>
+      </c>
+      <c r="E611" s="0" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="612" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20561,7 +20569,7 @@
         <v>1173</v>
       </c>
       <c r="B612" s="0" t="s">
-        <v>298</v>
+        <v>122</v>
       </c>
     </row>
     <row r="613" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20569,7 +20577,7 @@
         <v>1174</v>
       </c>
       <c r="B613" s="0" t="s">
-        <v>221</v>
+        <v>298</v>
       </c>
     </row>
     <row r="614" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20577,7 +20585,7 @@
         <v>1175</v>
       </c>
       <c r="B614" s="0" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="615" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20593,7 +20601,7 @@
         <v>1177</v>
       </c>
       <c r="B616" s="0" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="617" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20601,7 +20609,7 @@
         <v>1178</v>
       </c>
       <c r="B617" s="0" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
     </row>
     <row r="618" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20609,26 +20617,26 @@
         <v>1179</v>
       </c>
       <c r="B618" s="0" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="619" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A619" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="619" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A619" s="0" t="s">
         <v>1180</v>
       </c>
       <c r="B619" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="E619" s="0" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="620" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A620" s="0" t="s">
+    </row>
+    <row r="620" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A620" s="5" t="s">
         <v>1181</v>
       </c>
       <c r="B620" s="0" t="s">
         <v>224</v>
+      </c>
+      <c r="E620" s="0" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="621" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20662,16 +20670,16 @@
       <c r="B624" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="E624" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="625" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A625" s="0" t="s">
         <v>1186</v>
       </c>
       <c r="B625" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
+      </c>
+      <c r="E625" s="0" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="626" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20687,7 +20695,7 @@
         <v>1188</v>
       </c>
       <c r="B627" s="0" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="628" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20705,16 +20713,16 @@
       <c r="B629" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="E629" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="630" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A630" s="0" t="s">
         <v>1191</v>
       </c>
       <c r="B630" s="0" t="s">
-        <v>230</v>
+        <v>227</v>
+      </c>
+      <c r="E630" s="0" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="631" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20730,21 +20738,12 @@
         <v>1193</v>
       </c>
       <c r="B632" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="C632" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="G632" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H632" s="0" t="s">
-        <v>1194</v>
+        <v>230</v>
       </c>
     </row>
     <row r="633" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A633" s="0" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="B633" s="0" t="s">
         <v>228</v>
@@ -20756,26 +20755,35 @@
         <v>1</v>
       </c>
       <c r="H633" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="634" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A634" s="0" t="s">
-        <v>1193</v>
+        <v>1196</v>
       </c>
       <c r="B634" s="0" t="s">
-        <v>1194</v>
+        <v>228</v>
       </c>
       <c r="C634" s="0" t="s">
         <v>289</v>
       </c>
+      <c r="G634" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H634" s="0" t="s">
+        <v>1195</v>
+      </c>
     </row>
     <row r="635" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A635" s="0" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="B635" s="0" t="s">
-        <v>234</v>
+        <v>1195</v>
+      </c>
+      <c r="C635" s="0" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="636" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20783,7 +20791,7 @@
         <v>1197</v>
       </c>
       <c r="B636" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="637" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20801,9 +20809,6 @@
       <c r="B638" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="C638" s="0" t="s">
-        <v>118</v>
-      </c>
     </row>
     <row r="639" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A639" s="0" t="s">
@@ -20821,7 +20826,10 @@
         <v>1201</v>
       </c>
       <c r="B640" s="0" t="s">
-        <v>236</v>
+        <v>235</v>
+      </c>
+      <c r="C640" s="0" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="641" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20839,27 +20847,27 @@
       <c r="B642" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="E642" s="0" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="643" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A643" s="5" t="s">
+    </row>
+    <row r="643" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A643" s="0" t="s">
         <v>1204</v>
       </c>
       <c r="B643" s="0" t="s">
         <v>236</v>
       </c>
       <c r="E643" s="0" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="644" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A644" s="5" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B644" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="E644" s="0" t="s">
         <v>557</v>
-      </c>
-    </row>
-    <row r="644" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A644" s="0" t="s">
-        <v>1205</v>
-      </c>
-      <c r="B644" s="0" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="645" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20869,9 +20877,6 @@
       <c r="B645" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="E645" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="646" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A646" s="0" t="s">
@@ -20880,6 +20885,9 @@
       <c r="B646" s="0" t="s">
         <v>237</v>
       </c>
+      <c r="E646" s="0" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="647" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A647" s="0" t="s">
@@ -20889,23 +20897,23 @@
         <v>237</v>
       </c>
     </row>
-    <row r="648" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A648" s="5" t="s">
+    <row r="648" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A648" s="0" t="s">
         <v>1209</v>
       </c>
       <c r="B648" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="E648" s="0" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="649" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A649" s="0" t="s">
+    </row>
+    <row r="649" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A649" s="5" t="s">
         <v>1210</v>
       </c>
       <c r="B649" s="0" t="s">
         <v>237</v>
+      </c>
+      <c r="E649" s="0" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="650" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20913,7 +20921,7 @@
         <v>1211</v>
       </c>
       <c r="B650" s="0" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="651" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20929,10 +20937,7 @@
         <v>1213</v>
       </c>
       <c r="B652" s="0" t="s">
-        <v>460</v>
-      </c>
-      <c r="C652" s="0" t="s">
-        <v>118</v>
+        <v>238</v>
       </c>
     </row>
     <row r="653" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20951,7 +20956,10 @@
         <v>1215</v>
       </c>
       <c r="B654" s="0" t="s">
-        <v>246</v>
+        <v>460</v>
+      </c>
+      <c r="C654" s="0" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="655" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20967,7 +20975,7 @@
         <v>1217</v>
       </c>
       <c r="B656" s="0" t="s">
-        <v>457</v>
+        <v>246</v>
       </c>
     </row>
     <row r="657" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20975,7 +20983,7 @@
         <v>1218</v>
       </c>
       <c r="B657" s="0" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
     </row>
     <row r="658" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20991,7 +20999,7 @@
         <v>1220</v>
       </c>
       <c r="B659" s="0" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
     </row>
     <row r="660" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20999,7 +21007,7 @@
         <v>1221</v>
       </c>
       <c r="B660" s="0" t="s">
-        <v>164</v>
+        <v>459</v>
       </c>
     </row>
     <row r="661" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21031,7 +21039,7 @@
         <v>1225</v>
       </c>
       <c r="B664" s="0" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="665" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21047,10 +21055,7 @@
         <v>1227</v>
       </c>
       <c r="B666" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="C666" s="0" t="s">
-        <v>118</v>
+        <v>172</v>
       </c>
     </row>
     <row r="667" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21069,7 +21074,10 @@
         <v>1229</v>
       </c>
       <c r="B668" s="0" t="s">
-        <v>253</v>
+        <v>180</v>
+      </c>
+      <c r="C668" s="0" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="669" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21085,7 +21093,7 @@
         <v>1231</v>
       </c>
       <c r="B670" s="0" t="s">
-        <v>292</v>
+        <v>253</v>
       </c>
     </row>
     <row r="671" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21133,7 +21141,7 @@
         <v>1237</v>
       </c>
       <c r="B676" s="0" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
     </row>
     <row r="677" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21157,21 +21165,12 @@
         <v>1240</v>
       </c>
       <c r="B679" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C679" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="G679" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H679" s="0" t="s">
-        <v>1241</v>
+        <v>301</v>
       </c>
     </row>
     <row r="680" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A680" s="0" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="B680" s="0" t="s">
         <v>46</v>
@@ -21183,15 +21182,24 @@
         <v>1</v>
       </c>
       <c r="H680" s="0" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="681" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A681" s="0" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B681" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C681" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="G681" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H681" s="0" t="s">
         <v>1242</v>
-      </c>
-      <c r="B681" s="0" t="s">
-        <v>1241</v>
       </c>
     </row>
     <row r="682" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21199,7 +21207,7 @@
         <v>1243</v>
       </c>
       <c r="B682" s="0" t="s">
-        <v>250</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="683" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21207,7 +21215,7 @@
         <v>1244</v>
       </c>
       <c r="B683" s="0" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="684" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21239,7 +21247,7 @@
         <v>1248</v>
       </c>
       <c r="B687" s="0" t="s">
-        <v>240</v>
+        <v>258</v>
       </c>
     </row>
     <row r="688" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21263,7 +21271,7 @@
         <v>1251</v>
       </c>
       <c r="B690" s="0" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="691" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21271,7 +21279,7 @@
         <v>1252</v>
       </c>
       <c r="B691" s="0" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
     </row>
     <row r="692" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21281,16 +21289,16 @@
       <c r="B692" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="E692" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="693" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A693" s="0" t="s">
         <v>1254</v>
       </c>
       <c r="B693" s="0" t="s">
-        <v>255</v>
+        <v>254</v>
+      </c>
+      <c r="E693" s="0" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="694" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21316,20 +21324,20 @@
       <c r="B696" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="E696" s="0" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="697" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A697" s="5" t="s">
+    </row>
+    <row r="697" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A697" s="0" t="s">
         <v>1258</v>
       </c>
       <c r="B697" s="0" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="698" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A698" s="0" t="s">
+      <c r="E697" s="0" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="698" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A698" s="5" t="s">
         <v>1259</v>
       </c>
       <c r="B698" s="0" t="s">
@@ -21357,7 +21365,7 @@
         <v>1262</v>
       </c>
       <c r="B701" s="0" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
     </row>
     <row r="702" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21365,7 +21373,7 @@
         <v>1263</v>
       </c>
       <c r="B702" s="0" t="s">
-        <v>245</v>
+        <v>266</v>
       </c>
     </row>
     <row r="703" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21381,7 +21389,7 @@
         <v>1265</v>
       </c>
       <c r="B704" s="0" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="705" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21397,7 +21405,7 @@
         <v>1267</v>
       </c>
       <c r="B706" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="707" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21405,10 +21413,7 @@
         <v>1268</v>
       </c>
       <c r="B707" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="C707" s="0" t="s">
-        <v>213</v>
+        <v>244</v>
       </c>
     </row>
     <row r="708" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21427,7 +21432,10 @@
         <v>1270</v>
       </c>
       <c r="B709" s="0" t="s">
-        <v>261</v>
+        <v>265</v>
+      </c>
+      <c r="C709" s="0" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="710" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21453,9 +21461,6 @@
       <c r="B712" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="E712" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="713" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A713" s="0" t="s">
@@ -21464,24 +21469,27 @@
       <c r="B713" s="0" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="714" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A714" s="5" t="s">
+      <c r="E713" s="0" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="714" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A714" s="0" t="s">
         <v>1275</v>
       </c>
       <c r="B714" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="E714" s="0" t="s">
+    </row>
+    <row r="715" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A715" s="5" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B715" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="E715" s="0" t="s">
         <v>557</v>
-      </c>
-    </row>
-    <row r="715" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A715" s="0" t="s">
-        <v>1276</v>
-      </c>
-      <c r="B715" s="0" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="716" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21491,27 +21499,27 @@
       <c r="B716" s="0" t="s">
         <v>262</v>
       </c>
-      <c r="E716" s="0" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="717" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A717" s="5" t="s">
+    </row>
+    <row r="717" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A717" s="0" t="s">
         <v>1278</v>
       </c>
       <c r="B717" s="0" t="s">
         <v>262</v>
       </c>
       <c r="E717" s="0" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="718" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A718" s="5" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B718" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="E718" s="0" t="s">
         <v>557</v>
-      </c>
-    </row>
-    <row r="718" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A718" s="0" t="s">
-        <v>1279</v>
-      </c>
-      <c r="B718" s="0" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="719" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21527,7 +21535,7 @@
         <v>1281</v>
       </c>
       <c r="B720" s="0" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="721" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21535,7 +21543,7 @@
         <v>1282</v>
       </c>
       <c r="B721" s="0" t="s">
-        <v>462</v>
+        <v>251</v>
       </c>
     </row>
     <row r="722" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21543,26 +21551,26 @@
         <v>1283</v>
       </c>
       <c r="B722" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="723" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A723" s="5" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="723" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A723" s="0" t="s">
         <v>1284</v>
       </c>
       <c r="B723" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="E723" s="0" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="724" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A724" s="0" t="s">
+    </row>
+    <row r="724" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A724" s="5" t="s">
         <v>1285</v>
       </c>
       <c r="B724" s="0" t="s">
         <v>305</v>
+      </c>
+      <c r="E724" s="0" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="725" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21572,9 +21580,6 @@
       <c r="B725" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="E725" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="726" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A726" s="0" t="s">
@@ -21583,6 +21588,9 @@
       <c r="B726" s="0" t="s">
         <v>305</v>
       </c>
+      <c r="E726" s="0" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="727" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A727" s="0" t="s">
@@ -21605,7 +21613,7 @@
         <v>1290</v>
       </c>
       <c r="B729" s="0" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="730" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21613,7 +21621,7 @@
         <v>1291</v>
       </c>
       <c r="B730" s="0" t="s">
-        <v>464</v>
+        <v>306</v>
       </c>
     </row>
     <row r="731" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21621,7 +21629,7 @@
         <v>1292</v>
       </c>
       <c r="B731" s="0" t="s">
-        <v>257</v>
+        <v>464</v>
       </c>
     </row>
     <row r="732" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21629,7 +21637,7 @@
         <v>1293</v>
       </c>
       <c r="B732" s="0" t="s">
-        <v>111</v>
+        <v>257</v>
       </c>
     </row>
     <row r="733" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21655,16 +21663,16 @@
       <c r="B735" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="E735" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="736" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A736" s="0" t="s">
         <v>1297</v>
       </c>
       <c r="B736" s="0" t="s">
-        <v>174</v>
+        <v>111</v>
+      </c>
+      <c r="E736" s="0" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="737" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21680,7 +21688,7 @@
         <v>1299</v>
       </c>
       <c r="B738" s="0" t="s">
-        <v>242</v>
+        <v>174</v>
       </c>
     </row>
     <row r="739" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21688,7 +21696,7 @@
         <v>1300</v>
       </c>
       <c r="B739" s="0" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
     </row>
     <row r="740" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21696,15 +21704,15 @@
         <v>1301</v>
       </c>
       <c r="B740" s="0" t="s">
-        <v>1302</v>
+        <v>260</v>
       </c>
     </row>
     <row r="741" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A741" s="0" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B741" s="0" t="s">
         <v>1303</v>
-      </c>
-      <c r="B741" s="0" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="742" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21712,7 +21720,7 @@
         <v>1304</v>
       </c>
       <c r="B742" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="743" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21722,9 +21730,6 @@
       <c r="B743" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="E743" s="0" t="s">
-        <v>824</v>
-      </c>
     </row>
     <row r="744" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A744" s="0" t="s">
@@ -21734,26 +21739,29 @@
         <v>263</v>
       </c>
       <c r="E744" s="0" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="745" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A745" s="5" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="745" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A745" s="0" t="s">
         <v>1307</v>
       </c>
       <c r="B745" s="0" t="s">
         <v>263</v>
       </c>
       <c r="E745" s="0" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="746" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A746" s="5" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B746" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="E746" s="0" t="s">
         <v>557</v>
-      </c>
-    </row>
-    <row r="746" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A746" s="0" t="s">
-        <v>1308</v>
-      </c>
-      <c r="B746" s="0" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="747" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21779,7 +21787,6 @@
       <c r="B749" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="E749" s="6"/>
     </row>
     <row r="750" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A750" s="0" t="s">
@@ -21788,15 +21795,13 @@
       <c r="B750" s="0" t="s">
         <v>77</v>
       </c>
+      <c r="E750" s="6"/>
     </row>
     <row r="751" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A751" s="0" t="s">
         <v>1313</v>
       </c>
       <c r="B751" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="C751" s="0" t="s">
         <v>77</v>
       </c>
     </row>
@@ -21805,7 +21810,7 @@
         <v>1314</v>
       </c>
       <c r="B752" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C752" s="0" t="s">
         <v>77</v>
@@ -21816,7 +21821,10 @@
         <v>1315</v>
       </c>
       <c r="B753" s="0" t="s">
-        <v>267</v>
+        <v>78</v>
+      </c>
+      <c r="C753" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="754" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21834,9 +21842,6 @@
       <c r="B755" s="0" t="s">
         <v>267</v>
       </c>
-      <c r="E755" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="756" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A756" s="0" t="s">
@@ -21845,13 +21850,16 @@
       <c r="B756" s="0" t="s">
         <v>267</v>
       </c>
+      <c r="E756" s="0" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="757" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A757" s="0" t="s">
         <v>1319</v>
       </c>
       <c r="B757" s="0" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
     </row>
     <row r="758" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21907,7 +21915,7 @@
         <v>1326</v>
       </c>
       <c r="B764" s="0" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
     </row>
     <row r="765" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21915,7 +21923,7 @@
         <v>1327</v>
       </c>
       <c r="B765" s="0" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
     </row>
     <row r="766" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21947,7 +21955,7 @@
         <v>1331</v>
       </c>
       <c r="B769" s="0" t="s">
-        <v>272</v>
+        <v>285</v>
       </c>
     </row>
     <row r="770" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21963,7 +21971,7 @@
         <v>1333</v>
       </c>
       <c r="B771" s="0" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="772" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21979,7 +21987,7 @@
         <v>1335</v>
       </c>
       <c r="B773" s="0" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="774" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21987,7 +21995,7 @@
         <v>1336</v>
       </c>
       <c r="B774" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="775" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21995,7 +22003,7 @@
         <v>1337</v>
       </c>
       <c r="B775" s="0" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="776" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22003,7 +22011,7 @@
         <v>1338</v>
       </c>
       <c r="B776" s="0" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="777" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22011,7 +22019,7 @@
         <v>1339</v>
       </c>
       <c r="B777" s="0" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="778" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22021,9 +22029,6 @@
       <c r="B778" s="0" t="s">
         <v>280</v>
       </c>
-      <c r="E778" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="779" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A779" s="0" t="s">
@@ -22032,6 +22037,9 @@
       <c r="B779" s="0" t="s">
         <v>280</v>
       </c>
+      <c r="E779" s="0" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="780" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A780" s="0" t="s">
@@ -22046,7 +22054,7 @@
         <v>1343</v>
       </c>
       <c r="B781" s="0" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="782" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22056,35 +22064,35 @@
       <c r="B782" s="0" t="s">
         <v>281</v>
       </c>
-      <c r="E782" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="783" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A783" s="0" t="s">
         <v>1345</v>
       </c>
       <c r="B783" s="0" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="784" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A784" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="E783" s="0" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="784" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A784" s="0" t="s">
         <v>1346</v>
       </c>
       <c r="B784" s="0" t="s">
         <v>282</v>
       </c>
-      <c r="E784" s="0" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="785" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A785" s="0" t="s">
+    </row>
+    <row r="785" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A785" s="5" t="s">
         <v>1347</v>
       </c>
       <c r="B785" s="0" t="s">
         <v>282</v>
+      </c>
+      <c r="E785" s="0" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="786" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22094,9 +22102,6 @@
       <c r="B786" s="0" t="s">
         <v>282</v>
       </c>
-      <c r="E786" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="787" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A787" s="0" t="s">
@@ -22105,15 +22110,15 @@
       <c r="B787" s="0" t="s">
         <v>282</v>
       </c>
+      <c r="E787" s="0" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="788" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A788" s="0" t="s">
         <v>1350</v>
       </c>
       <c r="B788" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="C788" s="0" t="s">
         <v>282</v>
       </c>
     </row>
@@ -22133,7 +22138,10 @@
         <v>1352</v>
       </c>
       <c r="B790" s="0" t="s">
-        <v>276</v>
+        <v>315</v>
+      </c>
+      <c r="C790" s="0" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="791" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22141,7 +22149,7 @@
         <v>1353</v>
       </c>
       <c r="B791" s="0" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
     </row>
     <row r="792" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22149,7 +22157,7 @@
         <v>1354</v>
       </c>
       <c r="B792" s="0" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="793" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22157,7 +22165,7 @@
         <v>1355</v>
       </c>
       <c r="B793" s="0" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="794" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22165,7 +22173,7 @@
         <v>1356</v>
       </c>
       <c r="B794" s="0" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="795" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22189,7 +22197,7 @@
         <v>1359</v>
       </c>
       <c r="B797" s="0" t="s">
-        <v>42</v>
+        <v>287</v>
       </c>
     </row>
     <row r="798" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22229,7 +22237,7 @@
         <v>1364</v>
       </c>
       <c r="B802" s="0" t="s">
-        <v>123</v>
+        <v>42</v>
       </c>
     </row>
     <row r="803" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22247,9 +22255,6 @@
       <c r="B804" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="E804" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="805" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A805" s="0" t="s">
@@ -22259,7 +22264,7 @@
         <v>123</v>
       </c>
       <c r="E805" s="0" t="s">
-        <v>824</v>
+        <v>549</v>
       </c>
     </row>
     <row r="806" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22269,6 +22274,9 @@
       <c r="B806" s="0" t="s">
         <v>123</v>
       </c>
+      <c r="E806" s="0" t="s">
+        <v>824</v>
+      </c>
     </row>
     <row r="807" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A807" s="0" t="s">
@@ -22278,23 +22286,23 @@
         <v>123</v>
       </c>
     </row>
-    <row r="808" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A808" s="5" t="s">
+    <row r="808" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A808" s="0" t="s">
         <v>1370</v>
       </c>
       <c r="B808" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="E808" s="0" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="809" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A809" s="0" t="s">
+    </row>
+    <row r="809" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A809" s="5" t="s">
         <v>1371</v>
       </c>
       <c r="B809" s="0" t="s">
         <v>123</v>
+      </c>
+      <c r="E809" s="0" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="810" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22302,9 +22310,6 @@
         <v>1372</v>
       </c>
       <c r="B810" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="C810" s="0" t="s">
         <v>123</v>
       </c>
     </row>
@@ -22324,7 +22329,7 @@
         <v>1374</v>
       </c>
       <c r="B812" s="0" t="s">
-        <v>241</v>
+        <v>108</v>
       </c>
       <c r="C812" s="0" t="s">
         <v>123</v>
@@ -22335,7 +22340,7 @@
         <v>1375</v>
       </c>
       <c r="B813" s="0" t="s">
-        <v>211</v>
+        <v>241</v>
       </c>
       <c r="C813" s="0" t="s">
         <v>123</v>
@@ -22346,20 +22351,23 @@
         <v>1376</v>
       </c>
       <c r="B814" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="C814" s="0" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="815" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A815" s="0" t="s">
-        <v>289</v>
+        <v>1377</v>
       </c>
       <c r="B815" s="0" t="s">
-        <v>289</v>
+        <v>123</v>
       </c>
     </row>
     <row r="816" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A816" s="0" t="s">
-        <v>1377</v>
+        <v>289</v>
       </c>
       <c r="B816" s="0" t="s">
         <v>289</v>
@@ -22394,21 +22402,12 @@
         <v>1381</v>
       </c>
       <c r="B820" s="0" t="s">
-        <v>1382</v>
-      </c>
-      <c r="C820" s="0" t="s">
         <v>289</v>
-      </c>
-      <c r="G820" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H820" s="0" t="s">
-        <v>1383</v>
       </c>
     </row>
     <row r="821" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A821" s="0" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="B821" s="0" t="s">
         <v>1383</v>
@@ -22416,13 +22415,19 @@
       <c r="C821" s="0" t="s">
         <v>289</v>
       </c>
+      <c r="G821" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H821" s="0" t="s">
+        <v>1384</v>
+      </c>
     </row>
     <row r="822" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A822" s="0" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B822" s="0" t="s">
         <v>1384</v>
-      </c>
-      <c r="B822" s="0" t="s">
-        <v>313</v>
       </c>
       <c r="C822" s="0" t="s">
         <v>289</v>
@@ -22433,13 +22438,10 @@
         <v>1385</v>
       </c>
       <c r="B823" s="0" t="s">
-        <v>407</v>
+        <v>313</v>
       </c>
       <c r="C823" s="0" t="s">
         <v>289</v>
-      </c>
-      <c r="F823" s="0" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="824" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22447,7 +22449,7 @@
         <v>1386</v>
       </c>
       <c r="B824" s="0" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C824" s="0" t="s">
         <v>289</v>
@@ -22461,7 +22463,7 @@
         <v>1387</v>
       </c>
       <c r="B825" s="0" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C825" s="0" t="s">
         <v>289</v>
@@ -22475,7 +22477,7 @@
         <v>1388</v>
       </c>
       <c r="B826" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C826" s="0" t="s">
         <v>289</v>
@@ -22489,7 +22491,7 @@
         <v>1389</v>
       </c>
       <c r="B827" s="0" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C827" s="0" t="s">
         <v>289</v>
@@ -22503,7 +22505,7 @@
         <v>1390</v>
       </c>
       <c r="B828" s="0" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C828" s="0" t="s">
         <v>289</v>
@@ -22517,7 +22519,7 @@
         <v>1391</v>
       </c>
       <c r="B829" s="0" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C829" s="0" t="s">
         <v>289</v>
@@ -22531,7 +22533,7 @@
         <v>1392</v>
       </c>
       <c r="B830" s="0" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C830" s="0" t="s">
         <v>289</v>
@@ -22545,7 +22547,7 @@
         <v>1393</v>
       </c>
       <c r="B831" s="0" t="s">
-        <v>1394</v>
+        <v>414</v>
       </c>
       <c r="C831" s="0" t="s">
         <v>289</v>
@@ -22556,10 +22558,10 @@
     </row>
     <row r="832" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A832" s="0" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B832" s="0" t="s">
         <v>1395</v>
-      </c>
-      <c r="B832" s="0" t="s">
-        <v>415</v>
       </c>
       <c r="C832" s="0" t="s">
         <v>289</v>
@@ -22573,7 +22575,7 @@
         <v>1396</v>
       </c>
       <c r="B833" s="0" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C833" s="0" t="s">
         <v>289</v>
@@ -22601,7 +22603,7 @@
         <v>1398</v>
       </c>
       <c r="B835" s="0" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C835" s="0" t="s">
         <v>289</v>
@@ -22615,7 +22617,7 @@
         <v>1399</v>
       </c>
       <c r="B836" s="0" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C836" s="0" t="s">
         <v>289</v>
@@ -22629,7 +22631,7 @@
         <v>1400</v>
       </c>
       <c r="B837" s="0" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C837" s="0" t="s">
         <v>289</v>
@@ -22643,7 +22645,7 @@
         <v>1401</v>
       </c>
       <c r="B838" s="0" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C838" s="0" t="s">
         <v>289</v>
@@ -22657,7 +22659,7 @@
         <v>1402</v>
       </c>
       <c r="B839" s="0" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C839" s="0" t="s">
         <v>289</v>
@@ -22671,7 +22673,7 @@
         <v>1403</v>
       </c>
       <c r="B840" s="0" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C840" s="0" t="s">
         <v>289</v>
@@ -22685,7 +22687,7 @@
         <v>1404</v>
       </c>
       <c r="B841" s="0" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C841" s="0" t="s">
         <v>289</v>
@@ -22699,7 +22701,7 @@
         <v>1405</v>
       </c>
       <c r="B842" s="0" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C842" s="0" t="s">
         <v>289</v>
@@ -22713,7 +22715,7 @@
         <v>1406</v>
       </c>
       <c r="B843" s="0" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C843" s="0" t="s">
         <v>289</v>
@@ -22727,7 +22729,7 @@
         <v>1407</v>
       </c>
       <c r="B844" s="0" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C844" s="0" t="s">
         <v>289</v>
@@ -22741,7 +22743,7 @@
         <v>1408</v>
       </c>
       <c r="B845" s="0" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C845" s="0" t="s">
         <v>289</v>
@@ -22755,7 +22757,7 @@
         <v>1409</v>
       </c>
       <c r="B846" s="0" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C846" s="0" t="s">
         <v>289</v>
@@ -22769,7 +22771,7 @@
         <v>1410</v>
       </c>
       <c r="B847" s="0" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C847" s="0" t="s">
         <v>289</v>
@@ -22783,7 +22785,7 @@
         <v>1411</v>
       </c>
       <c r="B848" s="0" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C848" s="0" t="s">
         <v>289</v>
@@ -22797,7 +22799,7 @@
         <v>1412</v>
       </c>
       <c r="B849" s="0" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C849" s="0" t="s">
         <v>289</v>
@@ -22811,7 +22813,7 @@
         <v>1413</v>
       </c>
       <c r="B850" s="0" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C850" s="0" t="s">
         <v>289</v>
@@ -22825,7 +22827,7 @@
         <v>1414</v>
       </c>
       <c r="B851" s="0" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C851" s="0" t="s">
         <v>289</v>
@@ -22839,7 +22841,7 @@
         <v>1415</v>
       </c>
       <c r="B852" s="0" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C852" s="0" t="s">
         <v>289</v>
@@ -22853,7 +22855,7 @@
         <v>1416</v>
       </c>
       <c r="B853" s="0" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C853" s="0" t="s">
         <v>289</v>
@@ -22867,7 +22869,7 @@
         <v>1417</v>
       </c>
       <c r="B854" s="0" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C854" s="0" t="s">
         <v>289</v>
@@ -22881,7 +22883,7 @@
         <v>1418</v>
       </c>
       <c r="B855" s="0" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C855" s="0" t="s">
         <v>289</v>
@@ -22895,7 +22897,7 @@
         <v>1419</v>
       </c>
       <c r="B856" s="0" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C856" s="0" t="s">
         <v>289</v>
@@ -22909,7 +22911,7 @@
         <v>1420</v>
       </c>
       <c r="B857" s="0" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C857" s="0" t="s">
         <v>289</v>
@@ -22923,7 +22925,7 @@
         <v>1421</v>
       </c>
       <c r="B858" s="0" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C858" s="0" t="s">
         <v>289</v>
@@ -22937,7 +22939,7 @@
         <v>1422</v>
       </c>
       <c r="B859" s="0" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C859" s="0" t="s">
         <v>289</v>
@@ -22951,7 +22953,7 @@
         <v>1423</v>
       </c>
       <c r="B860" s="0" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C860" s="0" t="s">
         <v>289</v>
@@ -22965,7 +22967,7 @@
         <v>1424</v>
       </c>
       <c r="B861" s="0" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C861" s="0" t="s">
         <v>289</v>
@@ -22979,7 +22981,7 @@
         <v>1425</v>
       </c>
       <c r="B862" s="0" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C862" s="0" t="s">
         <v>289</v>
@@ -22993,7 +22995,7 @@
         <v>1426</v>
       </c>
       <c r="B863" s="0" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C863" s="0" t="s">
         <v>289</v>
@@ -23007,7 +23009,7 @@
         <v>1427</v>
       </c>
       <c r="B864" s="0" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C864" s="0" t="s">
         <v>289</v>
@@ -23021,7 +23023,7 @@
         <v>1428</v>
       </c>
       <c r="B865" s="0" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C865" s="0" t="s">
         <v>289</v>
@@ -23035,7 +23037,7 @@
         <v>1429</v>
       </c>
       <c r="B866" s="0" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C866" s="0" t="s">
         <v>289</v>
@@ -23049,7 +23051,7 @@
         <v>1430</v>
       </c>
       <c r="B867" s="0" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C867" s="0" t="s">
         <v>289</v>
@@ -23063,7 +23065,7 @@
         <v>1431</v>
       </c>
       <c r="B868" s="0" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C868" s="0" t="s">
         <v>289</v>
@@ -23077,7 +23079,7 @@
         <v>1432</v>
       </c>
       <c r="B869" s="0" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C869" s="0" t="s">
         <v>289</v>
@@ -23091,7 +23093,7 @@
         <v>1433</v>
       </c>
       <c r="B870" s="0" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C870" s="0" t="s">
         <v>289</v>
@@ -23105,7 +23107,7 @@
         <v>1434</v>
       </c>
       <c r="B871" s="0" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C871" s="0" t="s">
         <v>289</v>
@@ -23119,7 +23121,7 @@
         <v>1435</v>
       </c>
       <c r="B872" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C872" s="0" t="s">
         <v>289</v>
@@ -23133,7 +23135,7 @@
         <v>1436</v>
       </c>
       <c r="B873" s="0" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C873" s="0" t="s">
         <v>289</v>
@@ -23147,7 +23149,7 @@
         <v>1437</v>
       </c>
       <c r="B874" s="0" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C874" s="0" t="s">
         <v>289</v>
@@ -23161,7 +23163,13 @@
         <v>1438</v>
       </c>
       <c r="B875" s="0" t="s">
-        <v>288</v>
+        <v>456</v>
+      </c>
+      <c r="C875" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="F875" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="876" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23169,7 +23177,7 @@
         <v>1439</v>
       </c>
       <c r="B876" s="0" t="s">
-        <v>259</v>
+        <v>288</v>
       </c>
     </row>
     <row r="877" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23187,16 +23195,16 @@
       <c r="B878" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="E878" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="879" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A879" s="0" t="s">
         <v>1442</v>
       </c>
       <c r="B879" s="0" t="s">
-        <v>290</v>
+        <v>259</v>
+      </c>
+      <c r="E879" s="0" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="880" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23206,16 +23214,16 @@
       <c r="B880" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="E880" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="881" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A881" s="0" t="s">
         <v>1444</v>
       </c>
       <c r="B881" s="0" t="s">
-        <v>297</v>
+        <v>290</v>
+      </c>
+      <c r="E881" s="0" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="882" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23223,7 +23231,7 @@
         <v>1445</v>
       </c>
       <c r="B882" s="0" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="883" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23263,10 +23271,7 @@
         <v>1450</v>
       </c>
       <c r="B887" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="E887" s="0" t="s">
-        <v>549</v>
+        <v>293</v>
       </c>
     </row>
     <row r="888" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23276,30 +23281,21 @@
       <c r="B888" s="0" t="s">
         <v>296</v>
       </c>
+      <c r="E888" s="0" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="889" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A889" s="0" t="s">
         <v>1452</v>
       </c>
       <c r="B889" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="C889" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="G889" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H889" s="0" t="s">
-        <v>1453</v>
-      </c>
-      <c r="I889" s="0" t="s">
-        <v>1454</v>
+        <v>296</v>
       </c>
     </row>
     <row r="890" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A890" s="0" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="B890" s="0" t="s">
         <v>294</v>
@@ -23311,18 +23307,18 @@
         <v>1</v>
       </c>
       <c r="H890" s="0" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="I890" s="0" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="891" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A891" s="0" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="B891" s="0" t="s">
-        <v>1453</v>
+        <v>294</v>
       </c>
       <c r="C891" s="0" t="s">
         <v>123</v>
@@ -23331,30 +23327,30 @@
         <v>1</v>
       </c>
       <c r="H891" s="0" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="I891" s="0" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="892" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A892" s="0" t="s">
+        <v>1456</v>
+      </c>
+      <c r="B892" s="0" t="s">
+        <v>1454</v>
+      </c>
+      <c r="C892" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G892" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H892" s="0" t="s">
         <v>1457</v>
       </c>
-      <c r="B892" s="0" t="s">
-        <v>295</v>
-      </c>
-      <c r="C892" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="G892" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H892" s="0" t="s">
-        <v>1456</v>
-      </c>
       <c r="I892" s="0" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="893" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23371,10 +23367,10 @@
         <v>1</v>
       </c>
       <c r="H893" s="0" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="I893" s="0" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="894" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23391,10 +23387,10 @@
         <v>1</v>
       </c>
       <c r="H894" s="0" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="I894" s="0" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="895" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23411,10 +23407,10 @@
         <v>1</v>
       </c>
       <c r="H895" s="0" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="I895" s="0" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="896" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23431,10 +23427,10 @@
         <v>1</v>
       </c>
       <c r="H896" s="0" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="I896" s="0" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="897" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23451,10 +23447,10 @@
         <v>1</v>
       </c>
       <c r="H897" s="0" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="I897" s="0" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="898" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23471,10 +23467,10 @@
         <v>1</v>
       </c>
       <c r="H898" s="0" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="I898" s="0" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="899" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23491,29 +23487,41 @@
         <v>1</v>
       </c>
       <c r="H899" s="0" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="I899" s="0" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="900" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A900" s="0" t="s">
-        <v>1459</v>
+        <v>1465</v>
       </c>
       <c r="B900" s="0" t="s">
-        <v>1456</v>
+        <v>295</v>
       </c>
       <c r="C900" s="0" t="s">
         <v>289</v>
       </c>
+      <c r="G900" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H900" s="0" t="s">
+        <v>1457</v>
+      </c>
+      <c r="I900" s="0" t="s">
+        <v>1455</v>
+      </c>
     </row>
     <row r="901" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A901" s="0" t="s">
-        <v>1465</v>
+        <v>1460</v>
       </c>
       <c r="B901" s="0" t="s">
-        <v>300</v>
+        <v>1457</v>
+      </c>
+      <c r="C901" s="0" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="902" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23529,7 +23537,7 @@
         <v>1467</v>
       </c>
       <c r="B903" s="0" t="s">
-        <v>110</v>
+        <v>300</v>
       </c>
     </row>
     <row r="904" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23553,7 +23561,7 @@
         <v>1470</v>
       </c>
       <c r="B906" s="0" t="s">
-        <v>301</v>
+        <v>110</v>
       </c>
     </row>
     <row r="907" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23561,7 +23569,7 @@
         <v>1471</v>
       </c>
       <c r="B907" s="0" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="908" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23593,10 +23601,7 @@
         <v>1475</v>
       </c>
       <c r="B911" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="D911" s="0" t="n">
-        <v>1</v>
+        <v>302</v>
       </c>
     </row>
     <row r="912" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23626,7 +23631,7 @@
         <v>1478</v>
       </c>
       <c r="B914" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D914" s="0" t="n">
         <v>1</v>
@@ -23653,9 +23658,6 @@
       <c r="D916" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E916" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="917" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A917" s="0" t="s">
@@ -23667,13 +23669,19 @@
       <c r="D917" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E917" s="0" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="918" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A918" s="0" t="s">
         <v>1482</v>
       </c>
       <c r="B918" s="0" t="s">
-        <v>307</v>
+        <v>303</v>
+      </c>
+      <c r="D918" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="919" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23681,7 +23689,7 @@
         <v>1483</v>
       </c>
       <c r="B919" s="0" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="920" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23689,7 +23697,7 @@
         <v>1484</v>
       </c>
       <c r="B920" s="0" t="s">
-        <v>105</v>
+        <v>308</v>
       </c>
     </row>
     <row r="921" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23697,7 +23705,7 @@
         <v>1485</v>
       </c>
       <c r="B921" s="0" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="922" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23705,21 +23713,12 @@
         <v>1486</v>
       </c>
       <c r="B922" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="C922" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="G922" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H922" s="0" t="s">
-        <v>1487</v>
+        <v>114</v>
       </c>
     </row>
     <row r="923" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A923" s="0" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="B923" s="0" t="s">
         <v>76</v>
@@ -23731,7 +23730,7 @@
         <v>1</v>
       </c>
       <c r="H923" s="0" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="924" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23748,15 +23747,24 @@
         <v>1</v>
       </c>
       <c r="H924" s="0" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="925" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A925" s="0" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="B925" s="0" t="s">
-        <v>1487</v>
+        <v>76</v>
+      </c>
+      <c r="C925" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G925" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H925" s="0" t="s">
+        <v>1488</v>
       </c>
     </row>
     <row r="926" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23764,7 +23772,7 @@
         <v>1490</v>
       </c>
       <c r="B926" s="0" t="s">
-        <v>458</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="927" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23772,7 +23780,7 @@
         <v>1491</v>
       </c>
       <c r="B927" s="0" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="928" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23780,7 +23788,7 @@
         <v>1492</v>
       </c>
       <c r="B928" s="0" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="929" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23788,7 +23796,7 @@
         <v>1493</v>
       </c>
       <c r="B929" s="0" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="930" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23796,7 +23804,7 @@
         <v>1494</v>
       </c>
       <c r="B930" s="0" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="931" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23804,7 +23812,7 @@
         <v>1495</v>
       </c>
       <c r="B931" s="0" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="932" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23812,21 +23820,15 @@
         <v>1496</v>
       </c>
       <c r="B932" s="0" t="s">
-        <v>1497</v>
-      </c>
-      <c r="C932" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="F932" s="0" t="n">
-        <v>1</v>
+        <v>468</v>
       </c>
     </row>
     <row r="933" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A933" s="0" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B933" s="0" t="s">
         <v>1498</v>
-      </c>
-      <c r="B933" s="0" t="s">
-        <v>1499</v>
       </c>
       <c r="C933" s="0" t="s">
         <v>43</v>
@@ -23837,10 +23839,10 @@
     </row>
     <row r="934" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A934" s="0" t="s">
+        <v>1499</v>
+      </c>
+      <c r="B934" s="0" t="s">
         <v>1500</v>
-      </c>
-      <c r="B934" s="0" t="s">
-        <v>1499</v>
       </c>
       <c r="C934" s="0" t="s">
         <v>43</v>
@@ -23849,12 +23851,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="935" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A935" s="5" t="s">
+    <row r="935" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A935" s="0" t="s">
         <v>1501</v>
       </c>
       <c r="B935" s="0" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="C935" s="0" t="s">
         <v>43</v>
@@ -23863,12 +23865,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="936" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A936" s="7" t="s">
+    <row r="936" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A936" s="5" t="s">
         <v>1502</v>
       </c>
       <c r="B936" s="0" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="C936" s="0" t="s">
         <v>43</v>
@@ -23882,7 +23884,7 @@
         <v>1503</v>
       </c>
       <c r="B937" s="0" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="C937" s="0" t="s">
         <v>43</v>
@@ -23892,11 +23894,11 @@
       </c>
     </row>
     <row r="938" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A938" s="0" t="s">
+      <c r="A938" s="7" t="s">
         <v>1504</v>
       </c>
       <c r="B938" s="0" t="s">
-        <v>1505</v>
+        <v>1500</v>
       </c>
       <c r="C938" s="0" t="s">
         <v>43</v>
@@ -23907,10 +23909,10 @@
     </row>
     <row r="939" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A939" s="0" t="s">
+        <v>1505</v>
+      </c>
+      <c r="B939" s="0" t="s">
         <v>1506</v>
-      </c>
-      <c r="B939" s="0" t="s">
-        <v>1507</v>
       </c>
       <c r="C939" s="0" t="s">
         <v>43</v>
@@ -23921,10 +23923,10 @@
     </row>
     <row r="940" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A940" s="0" t="s">
+        <v>1507</v>
+      </c>
+      <c r="B940" s="0" t="s">
         <v>1508</v>
-      </c>
-      <c r="B940" s="0" t="s">
-        <v>1509</v>
       </c>
       <c r="C940" s="0" t="s">
         <v>43</v>
@@ -23935,7 +23937,7 @@
     </row>
     <row r="941" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A941" s="0" t="s">
-        <v>737</v>
+        <v>1509</v>
       </c>
       <c r="B941" s="0" t="s">
         <v>1510</v>
@@ -23949,10 +23951,10 @@
     </row>
     <row r="942" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A942" s="0" t="s">
+        <v>737</v>
+      </c>
+      <c r="B942" s="0" t="s">
         <v>1511</v>
-      </c>
-      <c r="B942" s="0" t="s">
-        <v>1512</v>
       </c>
       <c r="C942" s="0" t="s">
         <v>43</v>
@@ -23963,10 +23965,10 @@
     </row>
     <row r="943" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A943" s="0" t="s">
+        <v>1512</v>
+      </c>
+      <c r="B943" s="0" t="s">
         <v>1513</v>
-      </c>
-      <c r="B943" s="0" t="s">
-        <v>1514</v>
       </c>
       <c r="C943" s="0" t="s">
         <v>43</v>
@@ -23977,10 +23979,10 @@
     </row>
     <row r="944" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A944" s="0" t="s">
+        <v>1514</v>
+      </c>
+      <c r="B944" s="0" t="s">
         <v>1515</v>
-      </c>
-      <c r="B944" s="0" t="s">
-        <v>1516</v>
       </c>
       <c r="C944" s="0" t="s">
         <v>43</v>
@@ -23991,10 +23993,10 @@
     </row>
     <row r="945" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A945" s="0" t="s">
+        <v>1516</v>
+      </c>
+      <c r="B945" s="0" t="s">
         <v>1517</v>
-      </c>
-      <c r="B945" s="0" t="s">
-        <v>1518</v>
       </c>
       <c r="C945" s="0" t="s">
         <v>43</v>
@@ -24005,10 +24007,10 @@
     </row>
     <row r="946" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A946" s="0" t="s">
+        <v>1518</v>
+      </c>
+      <c r="B946" s="0" t="s">
         <v>1519</v>
-      </c>
-      <c r="B946" s="0" t="s">
-        <v>1520</v>
       </c>
       <c r="C946" s="0" t="s">
         <v>43</v>
@@ -24019,10 +24021,10 @@
     </row>
     <row r="947" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A947" s="0" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B947" s="0" t="s">
         <v>1521</v>
-      </c>
-      <c r="B947" s="0" t="s">
-        <v>1522</v>
       </c>
       <c r="C947" s="0" t="s">
         <v>43</v>
@@ -24033,10 +24035,10 @@
     </row>
     <row r="948" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A948" s="0" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B948" s="0" t="s">
         <v>1523</v>
-      </c>
-      <c r="B948" s="0" t="s">
-        <v>1524</v>
       </c>
       <c r="C948" s="0" t="s">
         <v>43</v>
@@ -24047,10 +24049,10 @@
     </row>
     <row r="949" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A949" s="0" t="s">
+        <v>1524</v>
+      </c>
+      <c r="B949" s="0" t="s">
         <v>1525</v>
-      </c>
-      <c r="B949" s="0" t="s">
-        <v>1526</v>
       </c>
       <c r="C949" s="0" t="s">
         <v>43</v>
@@ -24061,10 +24063,10 @@
     </row>
     <row r="950" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A950" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="B950" s="0" t="s">
         <v>1527</v>
-      </c>
-      <c r="B950" s="0" t="s">
-        <v>1528</v>
       </c>
       <c r="C950" s="0" t="s">
         <v>43</v>
@@ -24075,10 +24077,10 @@
     </row>
     <row r="951" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A951" s="0" t="s">
+        <v>1528</v>
+      </c>
+      <c r="B951" s="0" t="s">
         <v>1529</v>
-      </c>
-      <c r="B951" s="0" t="s">
-        <v>1530</v>
       </c>
       <c r="C951" s="0" t="s">
         <v>43</v>
@@ -24089,10 +24091,10 @@
     </row>
     <row r="952" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A952" s="0" t="s">
+        <v>1530</v>
+      </c>
+      <c r="B952" s="0" t="s">
         <v>1531</v>
-      </c>
-      <c r="B952" s="0" t="s">
-        <v>1532</v>
       </c>
       <c r="C952" s="0" t="s">
         <v>43</v>
@@ -24103,10 +24105,10 @@
     </row>
     <row r="953" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A953" s="0" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B953" s="0" t="s">
         <v>1533</v>
-      </c>
-      <c r="B953" s="0" t="s">
-        <v>1534</v>
       </c>
       <c r="C953" s="0" t="s">
         <v>43</v>
@@ -24117,10 +24119,10 @@
     </row>
     <row r="954" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A954" s="0" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B954" s="0" t="s">
         <v>1535</v>
-      </c>
-      <c r="B954" s="0" t="s">
-        <v>1536</v>
       </c>
       <c r="C954" s="0" t="s">
         <v>43</v>
@@ -24131,10 +24133,10 @@
     </row>
     <row r="955" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A955" s="0" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B955" s="0" t="s">
         <v>1537</v>
-      </c>
-      <c r="B955" s="0" t="s">
-        <v>1538</v>
       </c>
       <c r="C955" s="0" t="s">
         <v>43</v>
@@ -24145,10 +24147,10 @@
     </row>
     <row r="956" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A956" s="0" t="s">
+        <v>1538</v>
+      </c>
+      <c r="B956" s="0" t="s">
         <v>1539</v>
-      </c>
-      <c r="B956" s="0" t="s">
-        <v>1540</v>
       </c>
       <c r="C956" s="0" t="s">
         <v>43</v>
@@ -24159,10 +24161,10 @@
     </row>
     <row r="957" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A957" s="0" t="s">
+        <v>1540</v>
+      </c>
+      <c r="B957" s="0" t="s">
         <v>1541</v>
-      </c>
-      <c r="B957" s="0" t="s">
-        <v>1542</v>
       </c>
       <c r="C957" s="0" t="s">
         <v>43</v>
@@ -24173,10 +24175,10 @@
     </row>
     <row r="958" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A958" s="0" t="s">
+        <v>1542</v>
+      </c>
+      <c r="B958" s="0" t="s">
         <v>1543</v>
-      </c>
-      <c r="B958" s="0" t="s">
-        <v>1544</v>
       </c>
       <c r="C958" s="0" t="s">
         <v>43</v>
@@ -24187,10 +24189,10 @@
     </row>
     <row r="959" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A959" s="0" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B959" s="0" t="s">
         <v>1545</v>
-      </c>
-      <c r="B959" s="0" t="s">
-        <v>1546</v>
       </c>
       <c r="C959" s="0" t="s">
         <v>43</v>
@@ -24200,11 +24202,11 @@
       </c>
     </row>
     <row r="960" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A960" s="0" t="n">
-        <v>1701</v>
+      <c r="A960" s="0" t="s">
+        <v>1546</v>
       </c>
       <c r="B960" s="0" t="s">
-        <v>1499</v>
+        <v>1547</v>
       </c>
       <c r="C960" s="0" t="s">
         <v>43</v>
@@ -24215,10 +24217,10 @@
     </row>
     <row r="961" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A961" s="0" t="n">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="B961" s="0" t="s">
-        <v>1510</v>
+        <v>1500</v>
       </c>
       <c r="C961" s="0" t="s">
         <v>43</v>
@@ -24229,10 +24231,10 @@
     </row>
     <row r="962" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A962" s="0" t="n">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="B962" s="0" t="s">
-        <v>1540</v>
+        <v>1511</v>
       </c>
       <c r="C962" s="0" t="s">
         <v>43</v>
@@ -24243,10 +24245,10 @@
     </row>
     <row r="963" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A963" s="0" t="n">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="B963" s="0" t="s">
-        <v>1514</v>
+        <v>1541</v>
       </c>
       <c r="C963" s="0" t="s">
         <v>43</v>
@@ -24257,10 +24259,10 @@
     </row>
     <row r="964" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A964" s="0" t="n">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="B964" s="0" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="C964" s="0" t="s">
         <v>43</v>
@@ -24271,10 +24273,10 @@
     </row>
     <row r="965" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A965" s="0" t="n">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="B965" s="0" t="s">
-        <v>1512</v>
+        <v>1527</v>
       </c>
       <c r="C965" s="0" t="s">
         <v>43</v>
@@ -24285,10 +24287,10 @@
     </row>
     <row r="966" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A966" s="0" t="n">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="B966" s="0" t="s">
-        <v>1507</v>
+        <v>1513</v>
       </c>
       <c r="C966" s="0" t="s">
         <v>43</v>
@@ -24299,10 +24301,10 @@
     </row>
     <row r="967" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A967" s="0" t="n">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B967" s="0" t="s">
-        <v>1516</v>
+        <v>1508</v>
       </c>
       <c r="C967" s="0" t="s">
         <v>43</v>
@@ -24313,10 +24315,10 @@
     </row>
     <row r="968" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A968" s="0" t="n">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="B968" s="0" t="s">
-        <v>1532</v>
+        <v>1517</v>
       </c>
       <c r="C968" s="0" t="s">
         <v>43</v>
@@ -24327,10 +24329,10 @@
     </row>
     <row r="969" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A969" s="0" t="n">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="B969" s="0" t="s">
-        <v>1542</v>
+        <v>1533</v>
       </c>
       <c r="C969" s="0" t="s">
         <v>43</v>
@@ -24341,10 +24343,10 @@
     </row>
     <row r="970" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A970" s="0" t="n">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="B970" s="0" t="s">
-        <v>1546</v>
+        <v>1543</v>
       </c>
       <c r="C970" s="0" t="s">
         <v>43</v>
@@ -24355,10 +24357,10 @@
     </row>
     <row r="971" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A971" s="0" t="n">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="B971" s="0" t="s">
-        <v>1505</v>
+        <v>1547</v>
       </c>
       <c r="C971" s="0" t="s">
         <v>43</v>
@@ -24369,10 +24371,10 @@
     </row>
     <row r="972" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A972" s="0" t="n">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="B972" s="0" t="s">
-        <v>1518</v>
+        <v>1506</v>
       </c>
       <c r="C972" s="0" t="s">
         <v>43</v>
@@ -24383,10 +24385,10 @@
     </row>
     <row r="973" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A973" s="0" t="n">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="B973" s="0" t="s">
-        <v>1524</v>
+        <v>1519</v>
       </c>
       <c r="C973" s="0" t="s">
         <v>43</v>
@@ -24397,10 +24399,10 @@
     </row>
     <row r="974" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A974" s="0" t="n">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="B974" s="0" t="s">
-        <v>1534</v>
+        <v>1525</v>
       </c>
       <c r="C974" s="0" t="s">
         <v>43</v>
@@ -24411,10 +24413,10 @@
     </row>
     <row r="975" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A975" s="0" t="n">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="B975" s="0" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="C975" s="0" t="s">
         <v>43</v>
@@ -24425,10 +24427,10 @@
     </row>
     <row r="976" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A976" s="0" t="n">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="B976" s="0" t="s">
-        <v>1522</v>
+        <v>1537</v>
       </c>
       <c r="C976" s="0" t="s">
         <v>43</v>
@@ -24439,10 +24441,10 @@
     </row>
     <row r="977" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A977" s="0" t="n">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="B977" s="0" t="s">
-        <v>1509</v>
+        <v>1523</v>
       </c>
       <c r="C977" s="0" t="s">
         <v>43</v>
@@ -24453,10 +24455,10 @@
     </row>
     <row r="978" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A978" s="0" t="n">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="B978" s="0" t="s">
-        <v>1528</v>
+        <v>1510</v>
       </c>
       <c r="C978" s="0" t="s">
         <v>43</v>
@@ -24467,10 +24469,10 @@
     </row>
     <row r="979" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A979" s="0" t="n">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="B979" s="0" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="C979" s="0" t="s">
         <v>43</v>
@@ -24481,10 +24483,10 @@
     </row>
     <row r="980" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A980" s="0" t="n">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="B980" s="0" t="s">
-        <v>1544</v>
+        <v>1531</v>
       </c>
       <c r="C980" s="0" t="s">
         <v>43</v>
@@ -24495,10 +24497,10 @@
     </row>
     <row r="981" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A981" s="0" t="n">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="B981" s="0" t="s">
-        <v>1497</v>
+        <v>1545</v>
       </c>
       <c r="C981" s="0" t="s">
         <v>43</v>
@@ -24509,10 +24511,10 @@
     </row>
     <row r="982" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A982" s="0" t="n">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="B982" s="0" t="s">
-        <v>1520</v>
+        <v>1498</v>
       </c>
       <c r="C982" s="0" t="s">
         <v>43</v>
@@ -24522,42 +24524,39 @@
       </c>
     </row>
     <row r="983" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A983" s="0" t="s">
-        <v>1547</v>
+      <c r="A983" s="0" t="n">
+        <v>1723</v>
       </c>
       <c r="B983" s="0" t="s">
-        <v>1548</v>
+        <v>1521</v>
       </c>
       <c r="C983" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="J983" s="0" t="s">
-        <v>1549</v>
+        <v>43</v>
+      </c>
+      <c r="F983" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="984" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A984" s="0" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
       <c r="B984" s="0" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="C984" s="0" t="s">
         <v>293</v>
       </c>
-      <c r="F984" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="J984" s="0" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="985" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A985" s="0" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
       <c r="B985" s="0" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="C985" s="0" t="s">
         <v>293</v>
@@ -24566,7 +24565,7 @@
         <v>1</v>
       </c>
       <c r="J985" s="0" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="986" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24574,7 +24573,7 @@
         <v>1554</v>
       </c>
       <c r="B986" s="0" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="C986" s="0" t="s">
         <v>293</v>
@@ -24583,15 +24582,15 @@
         <v>1</v>
       </c>
       <c r="J986" s="0" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="987" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A987" s="0" t="s">
-        <v>641</v>
+        <v>1555</v>
       </c>
       <c r="B987" s="0" t="s">
-        <v>1555</v>
+        <v>1552</v>
       </c>
       <c r="C987" s="0" t="s">
         <v>293</v>
@@ -24600,15 +24599,15 @@
         <v>1</v>
       </c>
       <c r="J987" s="0" t="s">
-        <v>1556</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="988" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A988" s="0" t="s">
-        <v>1557</v>
+        <v>641</v>
       </c>
       <c r="B988" s="0" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="C988" s="0" t="s">
         <v>293</v>
@@ -24617,7 +24616,7 @@
         <v>1</v>
       </c>
       <c r="J988" s="0" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="989" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24625,7 +24624,7 @@
         <v>1558</v>
       </c>
       <c r="B989" s="0" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="C989" s="0" t="s">
         <v>293</v>
@@ -24634,7 +24633,7 @@
         <v>1</v>
       </c>
       <c r="J989" s="0" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="990" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24642,7 +24641,7 @@
         <v>1559</v>
       </c>
       <c r="B990" s="0" t="s">
-        <v>1560</v>
+        <v>1556</v>
       </c>
       <c r="C990" s="0" t="s">
         <v>293</v>
@@ -24651,15 +24650,15 @@
         <v>1</v>
       </c>
       <c r="J990" s="0" t="s">
-        <v>1561</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="991" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A991" s="0" t="s">
-        <v>1562</v>
+        <v>1560</v>
       </c>
       <c r="B991" s="0" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="C991" s="0" t="s">
         <v>293</v>
@@ -24668,15 +24667,15 @@
         <v>1</v>
       </c>
       <c r="J991" s="0" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="992" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A992" s="0" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
       <c r="B992" s="0" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="C992" s="0" t="s">
         <v>293</v>
@@ -24685,15 +24684,15 @@
         <v>1</v>
       </c>
       <c r="J992" s="0" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="993" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A993" s="0" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="B993" s="0" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="C993" s="0" t="s">
         <v>293</v>
@@ -24702,15 +24701,15 @@
         <v>1</v>
       </c>
       <c r="J993" s="0" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="994" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A994" s="0" t="s">
-        <v>728</v>
+        <v>1569</v>
       </c>
       <c r="B994" s="0" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="C994" s="0" t="s">
         <v>293</v>
@@ -24719,15 +24718,15 @@
         <v>1</v>
       </c>
       <c r="J994" s="0" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="995" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A995" s="0" t="s">
-        <v>1573</v>
+        <v>728</v>
       </c>
       <c r="B995" s="0" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
       <c r="C995" s="0" t="s">
         <v>293</v>
@@ -24736,15 +24735,15 @@
         <v>1</v>
       </c>
       <c r="J995" s="0" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="996" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A996" s="0" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
       <c r="B996" s="0" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
       <c r="C996" s="0" t="s">
         <v>293</v>
@@ -24753,15 +24752,15 @@
         <v>1</v>
       </c>
       <c r="J996" s="0" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="997" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A997" s="0" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="B997" s="0" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
       <c r="C997" s="0" t="s">
         <v>293</v>
@@ -24770,15 +24769,15 @@
         <v>1</v>
       </c>
       <c r="J997" s="0" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="998" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A998" s="0" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="B998" s="0" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
       <c r="C998" s="0" t="s">
         <v>293</v>
@@ -24787,15 +24786,15 @@
         <v>1</v>
       </c>
       <c r="J998" s="0" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="999" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A999" s="0" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="B999" s="0" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="C999" s="0" t="s">
         <v>293</v>
@@ -24804,15 +24803,15 @@
         <v>1</v>
       </c>
       <c r="J999" s="0" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="1000" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1000" s="0" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
       <c r="B1000" s="0" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
       <c r="C1000" s="0" t="s">
         <v>293</v>
@@ -24821,15 +24820,15 @@
         <v>1</v>
       </c>
       <c r="J1000" s="0" t="s">
-        <v>1590</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="1001" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1001" s="0" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
       <c r="B1001" s="0" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
       <c r="C1001" s="0" t="s">
         <v>293</v>
@@ -24838,15 +24837,15 @@
         <v>1</v>
       </c>
       <c r="J1001" s="0" t="s">
-        <v>1593</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="1002" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1002" s="0" t="s">
-        <v>1108</v>
+        <v>1592</v>
       </c>
       <c r="B1002" s="0" t="s">
-        <v>1109</v>
+        <v>1593</v>
       </c>
       <c r="C1002" s="0" t="s">
         <v>293</v>
@@ -24860,10 +24859,10 @@
     </row>
     <row r="1003" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1003" s="0" t="s">
-        <v>1595</v>
+        <v>1108</v>
       </c>
       <c r="B1003" s="0" t="s">
-        <v>1596</v>
+        <v>1109</v>
       </c>
       <c r="C1003" s="0" t="s">
         <v>293</v>
@@ -24872,15 +24871,15 @@
         <v>1</v>
       </c>
       <c r="J1003" s="0" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="1004" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1004" s="0" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
       <c r="B1004" s="0" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
       <c r="C1004" s="0" t="s">
         <v>293</v>
@@ -24889,15 +24888,15 @@
         <v>1</v>
       </c>
       <c r="J1004" s="0" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="1005" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1005" s="0" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
       <c r="B1005" s="0" t="s">
-        <v>1602</v>
+        <v>1600</v>
       </c>
       <c r="C1005" s="0" t="s">
         <v>293</v>
@@ -24906,15 +24905,15 @@
         <v>1</v>
       </c>
       <c r="J1005" s="0" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="1006" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1006" s="0" t="s">
-        <v>755</v>
+        <v>1602</v>
       </c>
       <c r="B1006" s="0" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="C1006" s="0" t="s">
         <v>293</v>
@@ -24923,15 +24922,15 @@
         <v>1</v>
       </c>
       <c r="J1006" s="0" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="1007" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1007" s="0" t="s">
-        <v>1606</v>
+        <v>755</v>
       </c>
       <c r="B1007" s="0" t="s">
-        <v>1607</v>
+        <v>1605</v>
       </c>
       <c r="C1007" s="0" t="s">
         <v>293</v>
@@ -24940,15 +24939,15 @@
         <v>1</v>
       </c>
       <c r="J1007" s="0" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="1008" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1008" s="0" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B1008" s="0" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="C1008" s="0" t="s">
         <v>293</v>
@@ -24957,15 +24956,15 @@
         <v>1</v>
       </c>
       <c r="J1008" s="0" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="1009" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1009" s="0" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
       <c r="B1009" s="0" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
       <c r="C1009" s="0" t="s">
         <v>293</v>
@@ -24974,15 +24973,15 @@
         <v>1</v>
       </c>
       <c r="J1009" s="0" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="1010" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1010" s="0" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
       <c r="B1010" s="0" t="s">
-        <v>1616</v>
+        <v>1614</v>
       </c>
       <c r="C1010" s="0" t="s">
         <v>293</v>
@@ -24991,15 +24990,15 @@
         <v>1</v>
       </c>
       <c r="J1010" s="0" t="s">
-        <v>1617</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="1011" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1011" s="0" t="s">
-        <v>1618</v>
+        <v>1616</v>
       </c>
       <c r="B1011" s="0" t="s">
-        <v>1619</v>
+        <v>1617</v>
       </c>
       <c r="C1011" s="0" t="s">
         <v>293</v>
@@ -25008,7 +25007,24 @@
         <v>1</v>
       </c>
       <c r="J1011" s="0" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="1012" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1012" s="0" t="s">
+        <v>1619</v>
+      </c>
+      <c r="B1012" s="0" t="s">
         <v>1620</v>
+      </c>
+      <c r="C1012" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="F1012" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J1012" s="0" t="s">
+        <v>1621</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small bugfix and addition.
British Virgin islands was incorrectly coded as entirely removed, making it match it to US virgin islands.

Added "Formet Soviet Union" synonym. Also tagged as defunct.
</commit_message>
<xml_diff>
--- a/inst/extdata/political_units.xlsx
+++ b/inst/extdata/political_units.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3044" uniqueCount="1622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3046" uniqueCount="1623">
   <si>
     <t xml:space="preserve">Abbrev</t>
   </si>
@@ -4350,6 +4350,9 @@
     <t xml:space="preserve">Soviet Union</t>
   </si>
   <si>
+    <t xml:space="preserve">Former Soviet Union</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sovjetunionen</t>
   </si>
   <si>
@@ -4395,10 +4398,10 @@
     <t xml:space="preserve">British Virgin Islands</t>
   </si>
   <si>
+    <t xml:space="preserve">Virgin Islands U.S.</t>
+  </si>
+  <si>
     <t xml:space="preserve">USA_VIR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Virgin Islands U.S.</t>
   </si>
   <si>
     <t xml:space="preserve">Virgin Islands (U.S.)</t>
@@ -5033,35 +5036,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="6.75"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14314,10 +14313,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14571,23 +14570,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1012"/>
+  <dimension ref="A1:J1013"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B777" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B862" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A777" activeCellId="0" sqref="A777"/>
-      <selection pane="bottomRight" activeCell="E802" activeCellId="0" sqref="E802"/>
+      <selection pane="bottomLeft" activeCell="A862" activeCellId="0" sqref="A862"/>
+      <selection pane="bottomRight" activeCell="C892" activeCellId="0" sqref="C892"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.25"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23201,16 +23200,19 @@
       <c r="B878" s="0" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="879" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A879" s="0" t="s">
+      <c r="D878" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="879" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A879" s="5" t="s">
         <v>1442</v>
       </c>
       <c r="B879" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="E879" s="0" t="s">
-        <v>549</v>
+      <c r="D879" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="880" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23218,7 +23220,13 @@
         <v>1443</v>
       </c>
       <c r="B880" s="0" t="s">
-        <v>290</v>
+        <v>259</v>
+      </c>
+      <c r="D880" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E880" s="0" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="881" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23228,16 +23236,16 @@
       <c r="B881" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="E881" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="882" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A882" s="0" t="s">
         <v>1445</v>
       </c>
       <c r="B882" s="0" t="s">
-        <v>297</v>
+        <v>290</v>
+      </c>
+      <c r="E882" s="0" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="883" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23245,7 +23253,7 @@
         <v>1446</v>
       </c>
       <c r="B883" s="0" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="884" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23285,10 +23293,7 @@
         <v>1451</v>
       </c>
       <c r="B888" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="E888" s="0" t="s">
-        <v>549</v>
+        <v>293</v>
       </c>
     </row>
     <row r="889" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23298,30 +23303,21 @@
       <c r="B889" s="0" t="s">
         <v>296</v>
       </c>
+      <c r="E889" s="0" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="890" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A890" s="0" t="s">
         <v>1453</v>
       </c>
       <c r="B890" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="C890" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="G890" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H890" s="0" t="s">
-        <v>1454</v>
-      </c>
-      <c r="I890" s="0" t="s">
-        <v>1455</v>
+        <v>296</v>
       </c>
     </row>
     <row r="891" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A891" s="0" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="B891" s="0" t="s">
         <v>294</v>
@@ -23333,18 +23329,18 @@
         <v>1</v>
       </c>
       <c r="H891" s="0" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="I891" s="0" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="892" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A892" s="0" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="B892" s="0" t="s">
-        <v>1454</v>
+        <v>294</v>
       </c>
       <c r="C892" s="0" t="s">
         <v>123</v>
@@ -23353,35 +23349,32 @@
         <v>1</v>
       </c>
       <c r="H892" s="0" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
       <c r="I892" s="0" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="893" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A893" s="0" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="B893" s="0" t="s">
-        <v>295</v>
+        <v>1455</v>
       </c>
       <c r="C893" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="G893" s="0" t="n">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="H893" s="0" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
       <c r="I893" s="0" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="894" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A894" s="0" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="B894" s="0" t="s">
         <v>295</v>
@@ -23393,10 +23386,10 @@
         <v>1</v>
       </c>
       <c r="H894" s="0" t="s">
-        <v>1457</v>
+        <v>1459</v>
       </c>
       <c r="I894" s="0" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="895" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23413,10 +23406,10 @@
         <v>1</v>
       </c>
       <c r="H895" s="0" t="s">
-        <v>1457</v>
+        <v>1459</v>
       </c>
       <c r="I895" s="0" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="896" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23433,10 +23426,10 @@
         <v>1</v>
       </c>
       <c r="H896" s="0" t="s">
-        <v>1457</v>
+        <v>1459</v>
       </c>
       <c r="I896" s="0" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="897" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23453,10 +23446,10 @@
         <v>1</v>
       </c>
       <c r="H897" s="0" t="s">
-        <v>1457</v>
+        <v>1459</v>
       </c>
       <c r="I897" s="0" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="898" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23473,10 +23466,10 @@
         <v>1</v>
       </c>
       <c r="H898" s="0" t="s">
-        <v>1457</v>
+        <v>1459</v>
       </c>
       <c r="I898" s="0" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="899" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23493,10 +23486,10 @@
         <v>1</v>
       </c>
       <c r="H899" s="0" t="s">
-        <v>1457</v>
+        <v>1459</v>
       </c>
       <c r="I899" s="0" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="900" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23513,29 +23506,41 @@
         <v>1</v>
       </c>
       <c r="H900" s="0" t="s">
-        <v>1457</v>
+        <v>1459</v>
       </c>
       <c r="I900" s="0" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="901" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A901" s="0" t="s">
-        <v>1460</v>
+        <v>1466</v>
       </c>
       <c r="B901" s="0" t="s">
-        <v>1457</v>
+        <v>295</v>
       </c>
       <c r="C901" s="0" t="s">
         <v>289</v>
       </c>
+      <c r="G901" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H901" s="0" t="s">
+        <v>1459</v>
+      </c>
+      <c r="I901" s="0" t="s">
+        <v>1456</v>
+      </c>
     </row>
     <row r="902" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A902" s="0" t="s">
-        <v>1466</v>
+        <v>1461</v>
       </c>
       <c r="B902" s="0" t="s">
-        <v>300</v>
+        <v>1459</v>
+      </c>
+      <c r="C902" s="0" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="903" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23551,7 +23556,7 @@
         <v>1468</v>
       </c>
       <c r="B904" s="0" t="s">
-        <v>110</v>
+        <v>300</v>
       </c>
     </row>
     <row r="905" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23575,7 +23580,7 @@
         <v>1471</v>
       </c>
       <c r="B907" s="0" t="s">
-        <v>301</v>
+        <v>110</v>
       </c>
     </row>
     <row r="908" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23583,7 +23588,7 @@
         <v>1472</v>
       </c>
       <c r="B908" s="0" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="909" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23615,10 +23620,7 @@
         <v>1476</v>
       </c>
       <c r="B912" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="D912" s="0" t="n">
-        <v>1</v>
+        <v>302</v>
       </c>
     </row>
     <row r="913" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23648,7 +23650,7 @@
         <v>1479</v>
       </c>
       <c r="B915" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D915" s="0" t="n">
         <v>1</v>
@@ -23675,9 +23677,6 @@
       <c r="D917" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E917" s="0" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="918" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A918" s="0" t="s">
@@ -23689,13 +23688,19 @@
       <c r="D918" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E918" s="0" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="919" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A919" s="0" t="s">
         <v>1483</v>
       </c>
       <c r="B919" s="0" t="s">
-        <v>307</v>
+        <v>303</v>
+      </c>
+      <c r="D919" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="920" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23703,7 +23708,7 @@
         <v>1484</v>
       </c>
       <c r="B920" s="0" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="921" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23711,7 +23716,7 @@
         <v>1485</v>
       </c>
       <c r="B921" s="0" t="s">
-        <v>105</v>
+        <v>308</v>
       </c>
     </row>
     <row r="922" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23719,7 +23724,7 @@
         <v>1486</v>
       </c>
       <c r="B922" s="0" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="923" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23727,21 +23732,12 @@
         <v>1487</v>
       </c>
       <c r="B923" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="C923" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="G923" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H923" s="0" t="s">
-        <v>1488</v>
+        <v>114</v>
       </c>
     </row>
     <row r="924" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A924" s="0" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="B924" s="0" t="s">
         <v>76</v>
@@ -23753,7 +23749,7 @@
         <v>1</v>
       </c>
       <c r="H924" s="0" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="925" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23770,15 +23766,24 @@
         <v>1</v>
       </c>
       <c r="H925" s="0" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="926" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A926" s="0" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="B926" s="0" t="s">
-        <v>1488</v>
+        <v>76</v>
+      </c>
+      <c r="C926" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G926" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H926" s="0" t="s">
+        <v>1489</v>
       </c>
     </row>
     <row r="927" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23786,7 +23791,7 @@
         <v>1491</v>
       </c>
       <c r="B927" s="0" t="s">
-        <v>458</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="928" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23794,7 +23799,7 @@
         <v>1492</v>
       </c>
       <c r="B928" s="0" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="929" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23802,7 +23807,7 @@
         <v>1493</v>
       </c>
       <c r="B929" s="0" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="930" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23810,7 +23815,7 @@
         <v>1494</v>
       </c>
       <c r="B930" s="0" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="931" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23818,7 +23823,7 @@
         <v>1495</v>
       </c>
       <c r="B931" s="0" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="932" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23826,7 +23831,7 @@
         <v>1496</v>
       </c>
       <c r="B932" s="0" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="933" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23834,21 +23839,15 @@
         <v>1497</v>
       </c>
       <c r="B933" s="0" t="s">
-        <v>1498</v>
-      </c>
-      <c r="C933" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="F933" s="0" t="n">
-        <v>1</v>
+        <v>468</v>
       </c>
     </row>
     <row r="934" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A934" s="0" t="s">
+        <v>1498</v>
+      </c>
+      <c r="B934" s="0" t="s">
         <v>1499</v>
-      </c>
-      <c r="B934" s="0" t="s">
-        <v>1500</v>
       </c>
       <c r="C934" s="0" t="s">
         <v>43</v>
@@ -23859,10 +23858,10 @@
     </row>
     <row r="935" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A935" s="0" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B935" s="0" t="s">
         <v>1501</v>
-      </c>
-      <c r="B935" s="0" t="s">
-        <v>1500</v>
       </c>
       <c r="C935" s="0" t="s">
         <v>43</v>
@@ -23871,12 +23870,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="936" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A936" s="5" t="s">
+    <row r="936" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A936" s="0" t="s">
         <v>1502</v>
       </c>
       <c r="B936" s="0" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="C936" s="0" t="s">
         <v>43</v>
@@ -23885,12 +23884,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="937" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A937" s="7" t="s">
+    <row r="937" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A937" s="5" t="s">
         <v>1503</v>
       </c>
       <c r="B937" s="0" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="C937" s="0" t="s">
         <v>43</v>
@@ -23904,7 +23903,7 @@
         <v>1504</v>
       </c>
       <c r="B938" s="0" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="C938" s="0" t="s">
         <v>43</v>
@@ -23914,11 +23913,11 @@
       </c>
     </row>
     <row r="939" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A939" s="0" t="s">
+      <c r="A939" s="7" t="s">
         <v>1505</v>
       </c>
       <c r="B939" s="0" t="s">
-        <v>1506</v>
+        <v>1501</v>
       </c>
       <c r="C939" s="0" t="s">
         <v>43</v>
@@ -23929,10 +23928,10 @@
     </row>
     <row r="940" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A940" s="0" t="s">
+        <v>1506</v>
+      </c>
+      <c r="B940" s="0" t="s">
         <v>1507</v>
-      </c>
-      <c r="B940" s="0" t="s">
-        <v>1508</v>
       </c>
       <c r="C940" s="0" t="s">
         <v>43</v>
@@ -23943,10 +23942,10 @@
     </row>
     <row r="941" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A941" s="0" t="s">
+        <v>1508</v>
+      </c>
+      <c r="B941" s="0" t="s">
         <v>1509</v>
-      </c>
-      <c r="B941" s="0" t="s">
-        <v>1510</v>
       </c>
       <c r="C941" s="0" t="s">
         <v>43</v>
@@ -23957,7 +23956,7 @@
     </row>
     <row r="942" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A942" s="0" t="s">
-        <v>737</v>
+        <v>1510</v>
       </c>
       <c r="B942" s="0" t="s">
         <v>1511</v>
@@ -23971,10 +23970,10 @@
     </row>
     <row r="943" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A943" s="0" t="s">
+        <v>737</v>
+      </c>
+      <c r="B943" s="0" t="s">
         <v>1512</v>
-      </c>
-      <c r="B943" s="0" t="s">
-        <v>1513</v>
       </c>
       <c r="C943" s="0" t="s">
         <v>43</v>
@@ -23985,10 +23984,10 @@
     </row>
     <row r="944" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A944" s="0" t="s">
+        <v>1513</v>
+      </c>
+      <c r="B944" s="0" t="s">
         <v>1514</v>
-      </c>
-      <c r="B944" s="0" t="s">
-        <v>1515</v>
       </c>
       <c r="C944" s="0" t="s">
         <v>43</v>
@@ -23999,10 +23998,10 @@
     </row>
     <row r="945" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A945" s="0" t="s">
+        <v>1515</v>
+      </c>
+      <c r="B945" s="0" t="s">
         <v>1516</v>
-      </c>
-      <c r="B945" s="0" t="s">
-        <v>1517</v>
       </c>
       <c r="C945" s="0" t="s">
         <v>43</v>
@@ -24013,10 +24012,10 @@
     </row>
     <row r="946" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A946" s="0" t="s">
+        <v>1517</v>
+      </c>
+      <c r="B946" s="0" t="s">
         <v>1518</v>
-      </c>
-      <c r="B946" s="0" t="s">
-        <v>1519</v>
       </c>
       <c r="C946" s="0" t="s">
         <v>43</v>
@@ -24027,10 +24026,10 @@
     </row>
     <row r="947" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A947" s="0" t="s">
+        <v>1519</v>
+      </c>
+      <c r="B947" s="0" t="s">
         <v>1520</v>
-      </c>
-      <c r="B947" s="0" t="s">
-        <v>1521</v>
       </c>
       <c r="C947" s="0" t="s">
         <v>43</v>
@@ -24041,10 +24040,10 @@
     </row>
     <row r="948" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A948" s="0" t="s">
+        <v>1521</v>
+      </c>
+      <c r="B948" s="0" t="s">
         <v>1522</v>
-      </c>
-      <c r="B948" s="0" t="s">
-        <v>1523</v>
       </c>
       <c r="C948" s="0" t="s">
         <v>43</v>
@@ -24055,10 +24054,10 @@
     </row>
     <row r="949" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A949" s="0" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B949" s="0" t="s">
         <v>1524</v>
-      </c>
-      <c r="B949" s="0" t="s">
-        <v>1525</v>
       </c>
       <c r="C949" s="0" t="s">
         <v>43</v>
@@ -24069,10 +24068,10 @@
     </row>
     <row r="950" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A950" s="0" t="s">
+        <v>1525</v>
+      </c>
+      <c r="B950" s="0" t="s">
         <v>1526</v>
-      </c>
-      <c r="B950" s="0" t="s">
-        <v>1527</v>
       </c>
       <c r="C950" s="0" t="s">
         <v>43</v>
@@ -24083,10 +24082,10 @@
     </row>
     <row r="951" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A951" s="0" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B951" s="0" t="s">
         <v>1528</v>
-      </c>
-      <c r="B951" s="0" t="s">
-        <v>1529</v>
       </c>
       <c r="C951" s="0" t="s">
         <v>43</v>
@@ -24097,10 +24096,10 @@
     </row>
     <row r="952" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A952" s="0" t="s">
+        <v>1529</v>
+      </c>
+      <c r="B952" s="0" t="s">
         <v>1530</v>
-      </c>
-      <c r="B952" s="0" t="s">
-        <v>1531</v>
       </c>
       <c r="C952" s="0" t="s">
         <v>43</v>
@@ -24111,10 +24110,10 @@
     </row>
     <row r="953" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A953" s="0" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B953" s="0" t="s">
         <v>1532</v>
-      </c>
-      <c r="B953" s="0" t="s">
-        <v>1533</v>
       </c>
       <c r="C953" s="0" t="s">
         <v>43</v>
@@ -24125,10 +24124,10 @@
     </row>
     <row r="954" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A954" s="0" t="s">
+        <v>1533</v>
+      </c>
+      <c r="B954" s="0" t="s">
         <v>1534</v>
-      </c>
-      <c r="B954" s="0" t="s">
-        <v>1535</v>
       </c>
       <c r="C954" s="0" t="s">
         <v>43</v>
@@ -24139,10 +24138,10 @@
     </row>
     <row r="955" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A955" s="0" t="s">
+        <v>1535</v>
+      </c>
+      <c r="B955" s="0" t="s">
         <v>1536</v>
-      </c>
-      <c r="B955" s="0" t="s">
-        <v>1537</v>
       </c>
       <c r="C955" s="0" t="s">
         <v>43</v>
@@ -24153,10 +24152,10 @@
     </row>
     <row r="956" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A956" s="0" t="s">
+        <v>1537</v>
+      </c>
+      <c r="B956" s="0" t="s">
         <v>1538</v>
-      </c>
-      <c r="B956" s="0" t="s">
-        <v>1539</v>
       </c>
       <c r="C956" s="0" t="s">
         <v>43</v>
@@ -24167,10 +24166,10 @@
     </row>
     <row r="957" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A957" s="0" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B957" s="0" t="s">
         <v>1540</v>
-      </c>
-      <c r="B957" s="0" t="s">
-        <v>1541</v>
       </c>
       <c r="C957" s="0" t="s">
         <v>43</v>
@@ -24181,10 +24180,10 @@
     </row>
     <row r="958" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A958" s="0" t="s">
+        <v>1541</v>
+      </c>
+      <c r="B958" s="0" t="s">
         <v>1542</v>
-      </c>
-      <c r="B958" s="0" t="s">
-        <v>1543</v>
       </c>
       <c r="C958" s="0" t="s">
         <v>43</v>
@@ -24195,10 +24194,10 @@
     </row>
     <row r="959" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A959" s="0" t="s">
+        <v>1543</v>
+      </c>
+      <c r="B959" s="0" t="s">
         <v>1544</v>
-      </c>
-      <c r="B959" s="0" t="s">
-        <v>1545</v>
       </c>
       <c r="C959" s="0" t="s">
         <v>43</v>
@@ -24209,10 +24208,10 @@
     </row>
     <row r="960" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A960" s="0" t="s">
+        <v>1545</v>
+      </c>
+      <c r="B960" s="0" t="s">
         <v>1546</v>
-      </c>
-      <c r="B960" s="0" t="s">
-        <v>1547</v>
       </c>
       <c r="C960" s="0" t="s">
         <v>43</v>
@@ -24222,11 +24221,11 @@
       </c>
     </row>
     <row r="961" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A961" s="0" t="n">
-        <v>1701</v>
+      <c r="A961" s="0" t="s">
+        <v>1547</v>
       </c>
       <c r="B961" s="0" t="s">
-        <v>1500</v>
+        <v>1548</v>
       </c>
       <c r="C961" s="0" t="s">
         <v>43</v>
@@ -24237,10 +24236,10 @@
     </row>
     <row r="962" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A962" s="0" t="n">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="B962" s="0" t="s">
-        <v>1511</v>
+        <v>1501</v>
       </c>
       <c r="C962" s="0" t="s">
         <v>43</v>
@@ -24251,10 +24250,10 @@
     </row>
     <row r="963" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A963" s="0" t="n">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="B963" s="0" t="s">
-        <v>1541</v>
+        <v>1512</v>
       </c>
       <c r="C963" s="0" t="s">
         <v>43</v>
@@ -24265,10 +24264,10 @@
     </row>
     <row r="964" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A964" s="0" t="n">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="B964" s="0" t="s">
-        <v>1515</v>
+        <v>1542</v>
       </c>
       <c r="C964" s="0" t="s">
         <v>43</v>
@@ -24279,10 +24278,10 @@
     </row>
     <row r="965" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A965" s="0" t="n">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="B965" s="0" t="s">
-        <v>1527</v>
+        <v>1516</v>
       </c>
       <c r="C965" s="0" t="s">
         <v>43</v>
@@ -24293,10 +24292,10 @@
     </row>
     <row r="966" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A966" s="0" t="n">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="B966" s="0" t="s">
-        <v>1513</v>
+        <v>1528</v>
       </c>
       <c r="C966" s="0" t="s">
         <v>43</v>
@@ -24307,10 +24306,10 @@
     </row>
     <row r="967" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A967" s="0" t="n">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="B967" s="0" t="s">
-        <v>1508</v>
+        <v>1514</v>
       </c>
       <c r="C967" s="0" t="s">
         <v>43</v>
@@ -24321,10 +24320,10 @@
     </row>
     <row r="968" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A968" s="0" t="n">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B968" s="0" t="s">
-        <v>1517</v>
+        <v>1509</v>
       </c>
       <c r="C968" s="0" t="s">
         <v>43</v>
@@ -24335,10 +24334,10 @@
     </row>
     <row r="969" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A969" s="0" t="n">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="B969" s="0" t="s">
-        <v>1533</v>
+        <v>1518</v>
       </c>
       <c r="C969" s="0" t="s">
         <v>43</v>
@@ -24349,10 +24348,10 @@
     </row>
     <row r="970" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A970" s="0" t="n">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="B970" s="0" t="s">
-        <v>1543</v>
+        <v>1534</v>
       </c>
       <c r="C970" s="0" t="s">
         <v>43</v>
@@ -24363,10 +24362,10 @@
     </row>
     <row r="971" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A971" s="0" t="n">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="B971" s="0" t="s">
-        <v>1547</v>
+        <v>1544</v>
       </c>
       <c r="C971" s="0" t="s">
         <v>43</v>
@@ -24377,10 +24376,10 @@
     </row>
     <row r="972" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A972" s="0" t="n">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="B972" s="0" t="s">
-        <v>1506</v>
+        <v>1548</v>
       </c>
       <c r="C972" s="0" t="s">
         <v>43</v>
@@ -24391,10 +24390,10 @@
     </row>
     <row r="973" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A973" s="0" t="n">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="B973" s="0" t="s">
-        <v>1519</v>
+        <v>1507</v>
       </c>
       <c r="C973" s="0" t="s">
         <v>43</v>
@@ -24405,10 +24404,10 @@
     </row>
     <row r="974" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A974" s="0" t="n">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="B974" s="0" t="s">
-        <v>1525</v>
+        <v>1520</v>
       </c>
       <c r="C974" s="0" t="s">
         <v>43</v>
@@ -24419,10 +24418,10 @@
     </row>
     <row r="975" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A975" s="0" t="n">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="B975" s="0" t="s">
-        <v>1535</v>
+        <v>1526</v>
       </c>
       <c r="C975" s="0" t="s">
         <v>43</v>
@@ -24433,10 +24432,10 @@
     </row>
     <row r="976" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A976" s="0" t="n">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="B976" s="0" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="C976" s="0" t="s">
         <v>43</v>
@@ -24447,10 +24446,10 @@
     </row>
     <row r="977" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A977" s="0" t="n">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="B977" s="0" t="s">
-        <v>1523</v>
+        <v>1538</v>
       </c>
       <c r="C977" s="0" t="s">
         <v>43</v>
@@ -24461,10 +24460,10 @@
     </row>
     <row r="978" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A978" s="0" t="n">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="B978" s="0" t="s">
-        <v>1510</v>
+        <v>1524</v>
       </c>
       <c r="C978" s="0" t="s">
         <v>43</v>
@@ -24475,10 +24474,10 @@
     </row>
     <row r="979" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A979" s="0" t="n">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="B979" s="0" t="s">
-        <v>1529</v>
+        <v>1511</v>
       </c>
       <c r="C979" s="0" t="s">
         <v>43</v>
@@ -24489,10 +24488,10 @@
     </row>
     <row r="980" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A980" s="0" t="n">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="B980" s="0" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="C980" s="0" t="s">
         <v>43</v>
@@ -24503,10 +24502,10 @@
     </row>
     <row r="981" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A981" s="0" t="n">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="B981" s="0" t="s">
-        <v>1545</v>
+        <v>1532</v>
       </c>
       <c r="C981" s="0" t="s">
         <v>43</v>
@@ -24517,10 +24516,10 @@
     </row>
     <row r="982" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A982" s="0" t="n">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="B982" s="0" t="s">
-        <v>1498</v>
+        <v>1546</v>
       </c>
       <c r="C982" s="0" t="s">
         <v>43</v>
@@ -24531,10 +24530,10 @@
     </row>
     <row r="983" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A983" s="0" t="n">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="B983" s="0" t="s">
-        <v>1521</v>
+        <v>1499</v>
       </c>
       <c r="C983" s="0" t="s">
         <v>43</v>
@@ -24544,42 +24543,39 @@
       </c>
     </row>
     <row r="984" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A984" s="0" t="s">
-        <v>1548</v>
+      <c r="A984" s="0" t="n">
+        <v>1723</v>
       </c>
       <c r="B984" s="0" t="s">
-        <v>1549</v>
+        <v>1522</v>
       </c>
       <c r="C984" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="J984" s="0" t="s">
-        <v>1550</v>
+        <v>43</v>
+      </c>
+      <c r="F984" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="985" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A985" s="0" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="B985" s="0" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="C985" s="0" t="s">
         <v>293</v>
       </c>
-      <c r="F985" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="J985" s="0" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="986" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A986" s="0" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
       <c r="B986" s="0" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="C986" s="0" t="s">
         <v>293</v>
@@ -24588,7 +24584,7 @@
         <v>1</v>
       </c>
       <c r="J986" s="0" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="987" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24596,7 +24592,7 @@
         <v>1555</v>
       </c>
       <c r="B987" s="0" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="C987" s="0" t="s">
         <v>293</v>
@@ -24605,15 +24601,15 @@
         <v>1</v>
       </c>
       <c r="J987" s="0" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="988" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A988" s="0" t="s">
-        <v>641</v>
+        <v>1556</v>
       </c>
       <c r="B988" s="0" t="s">
-        <v>1556</v>
+        <v>1553</v>
       </c>
       <c r="C988" s="0" t="s">
         <v>293</v>
@@ -24622,15 +24618,15 @@
         <v>1</v>
       </c>
       <c r="J988" s="0" t="s">
-        <v>1557</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="989" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A989" s="0" t="s">
-        <v>1558</v>
+        <v>641</v>
       </c>
       <c r="B989" s="0" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="C989" s="0" t="s">
         <v>293</v>
@@ -24639,7 +24635,7 @@
         <v>1</v>
       </c>
       <c r="J989" s="0" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="990" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24647,7 +24643,7 @@
         <v>1559</v>
       </c>
       <c r="B990" s="0" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="C990" s="0" t="s">
         <v>293</v>
@@ -24656,7 +24652,7 @@
         <v>1</v>
       </c>
       <c r="J990" s="0" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="991" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24664,7 +24660,7 @@
         <v>1560</v>
       </c>
       <c r="B991" s="0" t="s">
-        <v>1561</v>
+        <v>1557</v>
       </c>
       <c r="C991" s="0" t="s">
         <v>293</v>
@@ -24673,15 +24669,15 @@
         <v>1</v>
       </c>
       <c r="J991" s="0" t="s">
-        <v>1562</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="992" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A992" s="0" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="B992" s="0" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
       <c r="C992" s="0" t="s">
         <v>293</v>
@@ -24690,15 +24686,15 @@
         <v>1</v>
       </c>
       <c r="J992" s="0" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="993" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A993" s="0" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="B993" s="0" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
       <c r="C993" s="0" t="s">
         <v>293</v>
@@ -24707,15 +24703,15 @@
         <v>1</v>
       </c>
       <c r="J993" s="0" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="994" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A994" s="0" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="B994" s="0" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
       <c r="C994" s="0" t="s">
         <v>293</v>
@@ -24724,15 +24720,15 @@
         <v>1</v>
       </c>
       <c r="J994" s="0" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="995" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A995" s="0" t="s">
-        <v>728</v>
+        <v>1570</v>
       </c>
       <c r="B995" s="0" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="C995" s="0" t="s">
         <v>293</v>
@@ -24741,15 +24737,15 @@
         <v>1</v>
       </c>
       <c r="J995" s="0" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="996" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A996" s="0" t="s">
-        <v>1574</v>
+        <v>728</v>
       </c>
       <c r="B996" s="0" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="C996" s="0" t="s">
         <v>293</v>
@@ -24758,15 +24754,15 @@
         <v>1</v>
       </c>
       <c r="J996" s="0" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="997" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A997" s="0" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
       <c r="B997" s="0" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
       <c r="C997" s="0" t="s">
         <v>293</v>
@@ -24775,15 +24771,15 @@
         <v>1</v>
       </c>
       <c r="J997" s="0" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="998" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A998" s="0" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
       <c r="B998" s="0" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
       <c r="C998" s="0" t="s">
         <v>293</v>
@@ -24792,15 +24788,15 @@
         <v>1</v>
       </c>
       <c r="J998" s="0" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="999" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A999" s="0" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
       <c r="B999" s="0" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="C999" s="0" t="s">
         <v>293</v>
@@ -24809,15 +24805,15 @@
         <v>1</v>
       </c>
       <c r="J999" s="0" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="1000" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1000" s="0" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="B1000" s="0" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="C1000" s="0" t="s">
         <v>293</v>
@@ -24826,15 +24822,15 @@
         <v>1</v>
       </c>
       <c r="J1000" s="0" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="1001" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1001" s="0" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
       <c r="B1001" s="0" t="s">
-        <v>1590</v>
+        <v>1588</v>
       </c>
       <c r="C1001" s="0" t="s">
         <v>293</v>
@@ -24843,15 +24839,15 @@
         <v>1</v>
       </c>
       <c r="J1001" s="0" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="1002" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1002" s="0" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
       <c r="B1002" s="0" t="s">
-        <v>1593</v>
+        <v>1591</v>
       </c>
       <c r="C1002" s="0" t="s">
         <v>293</v>
@@ -24860,15 +24856,15 @@
         <v>1</v>
       </c>
       <c r="J1002" s="0" t="s">
-        <v>1594</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="1003" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1003" s="0" t="s">
-        <v>1108</v>
+        <v>1593</v>
       </c>
       <c r="B1003" s="0" t="s">
-        <v>1109</v>
+        <v>1594</v>
       </c>
       <c r="C1003" s="0" t="s">
         <v>293</v>
@@ -24882,10 +24878,10 @@
     </row>
     <row r="1004" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1004" s="0" t="s">
-        <v>1596</v>
+        <v>1108</v>
       </c>
       <c r="B1004" s="0" t="s">
-        <v>1597</v>
+        <v>1109</v>
       </c>
       <c r="C1004" s="0" t="s">
         <v>293</v>
@@ -24894,15 +24890,15 @@
         <v>1</v>
       </c>
       <c r="J1004" s="0" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="1005" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1005" s="0" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
       <c r="B1005" s="0" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
       <c r="C1005" s="0" t="s">
         <v>293</v>
@@ -24911,15 +24907,15 @@
         <v>1</v>
       </c>
       <c r="J1005" s="0" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="1006" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1006" s="0" t="s">
-        <v>1602</v>
+        <v>1600</v>
       </c>
       <c r="B1006" s="0" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
       <c r="C1006" s="0" t="s">
         <v>293</v>
@@ -24928,15 +24924,15 @@
         <v>1</v>
       </c>
       <c r="J1006" s="0" t="s">
-        <v>1604</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="1007" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1007" s="0" t="s">
-        <v>755</v>
+        <v>1603</v>
       </c>
       <c r="B1007" s="0" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="C1007" s="0" t="s">
         <v>293</v>
@@ -24945,15 +24941,15 @@
         <v>1</v>
       </c>
       <c r="J1007" s="0" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="1008" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1008" s="0" t="s">
-        <v>1607</v>
+        <v>755</v>
       </c>
       <c r="B1008" s="0" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
       <c r="C1008" s="0" t="s">
         <v>293</v>
@@ -24962,15 +24958,15 @@
         <v>1</v>
       </c>
       <c r="J1008" s="0" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="1009" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1009" s="0" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="B1009" s="0" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
       <c r="C1009" s="0" t="s">
         <v>293</v>
@@ -24979,15 +24975,15 @@
         <v>1</v>
       </c>
       <c r="J1009" s="0" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="1010" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1010" s="0" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
       <c r="B1010" s="0" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
       <c r="C1010" s="0" t="s">
         <v>293</v>
@@ -24996,15 +24992,15 @@
         <v>1</v>
       </c>
       <c r="J1010" s="0" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="1011" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1011" s="0" t="s">
-        <v>1616</v>
+        <v>1614</v>
       </c>
       <c r="B1011" s="0" t="s">
-        <v>1617</v>
+        <v>1615</v>
       </c>
       <c r="C1011" s="0" t="s">
         <v>293</v>
@@ -25013,15 +25009,15 @@
         <v>1</v>
       </c>
       <c r="J1011" s="0" t="s">
-        <v>1618</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="1012" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1012" s="0" t="s">
-        <v>1619</v>
+        <v>1617</v>
       </c>
       <c r="B1012" s="0" t="s">
-        <v>1620</v>
+        <v>1618</v>
       </c>
       <c r="C1012" s="0" t="s">
         <v>293</v>
@@ -25030,7 +25026,24 @@
         <v>1</v>
       </c>
       <c r="J1012" s="0" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="1013" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1013" s="0" t="s">
+        <v>1620</v>
+      </c>
+      <c r="B1013" s="0" t="s">
         <v>1621</v>
+      </c>
+      <c r="C1013" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="F1013" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J1013" s="0" t="s">
+        <v>1622</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pu_translate(). Big update. Various new units, support for multiple superunits, detailed manual.
</commit_message>
<xml_diff>
--- a/inst/extdata/political_units.xlsx
+++ b/inst/extdata/political_units.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3106" uniqueCount="1643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3108" uniqueCount="1644">
   <si>
     <t xml:space="preserve">Abbrev</t>
   </si>
@@ -4951,6 +4951,9 @@
   </si>
   <si>
     <t xml:space="preserve">VE-V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">world</t>
   </si>
 </sst>
 </file>
@@ -5359,32 +5362,32 @@
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="9" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="21.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="22.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="8.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="8.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="6.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="6.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="6.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="6.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="6.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="35" style="0" width="8.71"/>
@@ -14897,14 +14900,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1035"/>
+  <dimension ref="A1:J1036"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B1027" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A48" activeCellId="0" sqref="A48"/>
-      <selection pane="bottomRight" activeCell="A71" activeCellId="0" sqref="A71"/>
+      <selection pane="bottomLeft" activeCell="A1027" activeCellId="0" sqref="A1027"/>
+      <selection pane="bottomRight" activeCell="F1052" activeCellId="0" sqref="F1052"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14913,7 +14916,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25604,6 +25609,14 @@
       </c>
       <c r="J1035" s="0" t="s">
         <v>1642</v>
+      </c>
+    </row>
+    <row r="1036" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1036" s="0" t="s">
+        <v>1643</v>
+      </c>
+      <c r="B1036" s="0" t="s">
+        <v>1643</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update pol units with italian regions and provinces
</commit_message>
<xml_diff>
--- a/inst/extdata/political_units.xlsx
+++ b/inst/extdata/political_units.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4055" uniqueCount="2072">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4539" uniqueCount="2314">
   <si>
     <t xml:space="preserve">Abbrev</t>
   </si>
@@ -6238,6 +6238,732 @@
   </si>
   <si>
     <t xml:space="preserve">Ho Chi Minh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agrigento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-AG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alessandria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-AL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ancona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-AN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aosta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-AO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ascoli Piceno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-AP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aquila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-AQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arezzo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-AR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-AT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avellino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-AV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-BA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bergamo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-BG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belluno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-BL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benevento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-BN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bologna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-BO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brindisi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-BR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brescia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-BS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bolzano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-BZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cagliari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campobasso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-CB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caserta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-CE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chieti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-CH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caltanissetta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-CL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuneo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-CN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cremona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-CR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cosenza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-CS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-CT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catanzaro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-CZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-EN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ferrara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-FE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foggia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-FG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Firenze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-FI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forlì</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-FC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frosinone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-FR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-GE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gorizia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-GO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grosseto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-GR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imperia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-IM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isernia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-IS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crotone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-KR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lecco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-LC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lodi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-LO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lecce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-LE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Livorno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-LI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-LT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lucca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-LU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macerata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-MC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Messina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-ME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-MI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mantova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-MN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-MO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Massa Carrara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-MS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-MT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Napoli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Novara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nuoro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-NU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oristano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-OR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palermo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-PA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piacenza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-PC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Padova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-PD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pescara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-PE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perugia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-PG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pisa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-PI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pordenone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-PN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-PO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-PR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pesaro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-PU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pistoia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-PT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pavia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-PV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potenza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-PZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ravenna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-RA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reggio Calabria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-RC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reggio Emilia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-RE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ragusa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-RG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rieti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-RI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-RM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rimini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-RN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rovigo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-RO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salerno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sondrio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-SO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La Spezia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-SP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siracusa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-SR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sassari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-SS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Savona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-SV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taranto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-TA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teramo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-TE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-TN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-TO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trapani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-TP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-TR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trieste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-TS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treviso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Udine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-UD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Varese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-VA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verbania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-VB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vercelli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-VC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venezia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-VE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vicenza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-VI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-VR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viterbo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-VT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abruzzo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-ABR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basilicata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-BAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calabria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-CAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-CAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emilia-Romagna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-EMI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Friuli-Venezia Giulia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-FRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lazio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-LAZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liguria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-LIG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lombardia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-LOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-MAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-MOL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piemonte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-PIE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puglia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-PUG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sardegna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-SAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sicilia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-SIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toscana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-TOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trentino-Alto Adige</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-TRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umbria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-UMB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valle D'Aosta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-VAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veneto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA-VEN</t>
   </si>
 </sst>
 </file>
@@ -6249,7 +6975,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -6277,6 +7003,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -6321,7 +7052,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6351,6 +7082,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -15922,14 +16657,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1332"/>
+  <dimension ref="A1:J1453"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B1044" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B1414" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A1044" activeCellId="0" sqref="A1044"/>
-      <selection pane="bottomRight" activeCell="G1064" activeCellId="0" sqref="G1064"/>
+      <selection pane="bottomLeft" activeCell="A1414" activeCellId="0" sqref="A1414"/>
+      <selection pane="bottomRight" activeCell="A1437" activeCellId="0" sqref="A1437"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30473,6 +31208,2063 @@
         <v>2012</v>
       </c>
     </row>
+    <row r="1333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1333" s="0" t="s">
+        <v>2072</v>
+      </c>
+      <c r="B1333" s="0" t="s">
+        <v>2073</v>
+      </c>
+      <c r="C1333" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1333" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1333" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1334" s="0" t="s">
+        <v>2074</v>
+      </c>
+      <c r="B1334" s="0" t="s">
+        <v>2075</v>
+      </c>
+      <c r="C1334" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1334" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1334" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1335" s="0" t="s">
+        <v>2076</v>
+      </c>
+      <c r="B1335" s="0" t="s">
+        <v>2077</v>
+      </c>
+      <c r="C1335" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1335" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1335" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1336" s="0" t="s">
+        <v>2078</v>
+      </c>
+      <c r="B1336" s="0" t="s">
+        <v>2079</v>
+      </c>
+      <c r="C1336" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1336" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1336" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1337" s="0" t="s">
+        <v>2080</v>
+      </c>
+      <c r="B1337" s="0" t="s">
+        <v>2081</v>
+      </c>
+      <c r="C1337" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1337" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1337" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1338" s="0" t="s">
+        <v>2082</v>
+      </c>
+      <c r="B1338" s="0" t="s">
+        <v>2083</v>
+      </c>
+      <c r="C1338" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1338" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1338" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1339" s="0" t="s">
+        <v>2084</v>
+      </c>
+      <c r="B1339" s="0" t="s">
+        <v>2085</v>
+      </c>
+      <c r="C1339" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1339" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1339" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1340" s="0" t="s">
+        <v>2086</v>
+      </c>
+      <c r="B1340" s="0" t="s">
+        <v>2087</v>
+      </c>
+      <c r="C1340" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1340" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1340" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1341" s="0" t="s">
+        <v>2088</v>
+      </c>
+      <c r="B1341" s="0" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C1341" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1341" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1341" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1342" s="0" t="s">
+        <v>2090</v>
+      </c>
+      <c r="B1342" s="0" t="s">
+        <v>2091</v>
+      </c>
+      <c r="C1342" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1342" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1342" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1343" s="0" t="s">
+        <v>2092</v>
+      </c>
+      <c r="B1343" s="0" t="s">
+        <v>2093</v>
+      </c>
+      <c r="C1343" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1343" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1343" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1344" s="0" t="s">
+        <v>2094</v>
+      </c>
+      <c r="B1344" s="0" t="s">
+        <v>2095</v>
+      </c>
+      <c r="C1344" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1344" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1344" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1345" s="0" t="s">
+        <v>2096</v>
+      </c>
+      <c r="B1345" s="0" t="s">
+        <v>2097</v>
+      </c>
+      <c r="C1345" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1345" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1345" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1346" s="0" t="s">
+        <v>2098</v>
+      </c>
+      <c r="B1346" s="0" t="s">
+        <v>2099</v>
+      </c>
+      <c r="C1346" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1346" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1346" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1347" s="0" t="s">
+        <v>2100</v>
+      </c>
+      <c r="B1347" s="0" t="s">
+        <v>2101</v>
+      </c>
+      <c r="C1347" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1347" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1347" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1348" s="0" t="s">
+        <v>2102</v>
+      </c>
+      <c r="B1348" s="0" t="s">
+        <v>2103</v>
+      </c>
+      <c r="C1348" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1348" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1348" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1349" s="0" t="s">
+        <v>2104</v>
+      </c>
+      <c r="B1349" s="0" t="s">
+        <v>2105</v>
+      </c>
+      <c r="C1349" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1349" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1349" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1350" s="0" t="s">
+        <v>2106</v>
+      </c>
+      <c r="B1350" s="0" t="s">
+        <v>2107</v>
+      </c>
+      <c r="C1350" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1350" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1350" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1351" s="0" t="s">
+        <v>2108</v>
+      </c>
+      <c r="B1351" s="0" t="s">
+        <v>2109</v>
+      </c>
+      <c r="C1351" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1351" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1351" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1352" s="0" t="s">
+        <v>2110</v>
+      </c>
+      <c r="B1352" s="0" t="s">
+        <v>2111</v>
+      </c>
+      <c r="C1352" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1352" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1352" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1353" s="0" t="s">
+        <v>2112</v>
+      </c>
+      <c r="B1353" s="0" t="s">
+        <v>2113</v>
+      </c>
+      <c r="C1353" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1353" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1353" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1354" s="0" t="s">
+        <v>2114</v>
+      </c>
+      <c r="B1354" s="0" t="s">
+        <v>2115</v>
+      </c>
+      <c r="C1354" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1354" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1354" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1355" s="0" t="s">
+        <v>2116</v>
+      </c>
+      <c r="B1355" s="0" t="s">
+        <v>2117</v>
+      </c>
+      <c r="C1355" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1355" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1355" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1356" s="0" t="s">
+        <v>2118</v>
+      </c>
+      <c r="B1356" s="0" t="s">
+        <v>2119</v>
+      </c>
+      <c r="C1356" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1356" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1356" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1357" s="0" t="s">
+        <v>2120</v>
+      </c>
+      <c r="B1357" s="0" t="s">
+        <v>2121</v>
+      </c>
+      <c r="C1357" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1357" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1357" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1358" s="0" t="s">
+        <v>2122</v>
+      </c>
+      <c r="B1358" s="0" t="s">
+        <v>2123</v>
+      </c>
+      <c r="C1358" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1358" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1358" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1359" s="0" t="s">
+        <v>2124</v>
+      </c>
+      <c r="B1359" s="0" t="s">
+        <v>2125</v>
+      </c>
+      <c r="C1359" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1359" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1359" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1360" s="0" t="s">
+        <v>2126</v>
+      </c>
+      <c r="B1360" s="0" t="s">
+        <v>2127</v>
+      </c>
+      <c r="C1360" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1360" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1360" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1361" s="0" t="s">
+        <v>2128</v>
+      </c>
+      <c r="B1361" s="0" t="s">
+        <v>2129</v>
+      </c>
+      <c r="C1361" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1361" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1361" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1362" s="0" t="s">
+        <v>2130</v>
+      </c>
+      <c r="B1362" s="0" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1362" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1362" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1362" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1363" s="0" t="s">
+        <v>2132</v>
+      </c>
+      <c r="B1363" s="0" t="s">
+        <v>2133</v>
+      </c>
+      <c r="C1363" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1363" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1363" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1364" s="0" t="s">
+        <v>2134</v>
+      </c>
+      <c r="B1364" s="0" t="s">
+        <v>2135</v>
+      </c>
+      <c r="C1364" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1364" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1364" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1365" s="0" t="s">
+        <v>2136</v>
+      </c>
+      <c r="B1365" s="0" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1365" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1365" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1365" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1366" s="0" t="s">
+        <v>2138</v>
+      </c>
+      <c r="B1366" s="0" t="s">
+        <v>2139</v>
+      </c>
+      <c r="C1366" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1366" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1366" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1367" s="0" t="s">
+        <v>2140</v>
+      </c>
+      <c r="B1367" s="0" t="s">
+        <v>2141</v>
+      </c>
+      <c r="C1367" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1367" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1367" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1368" s="0" t="s">
+        <v>2142</v>
+      </c>
+      <c r="B1368" s="0" t="s">
+        <v>2143</v>
+      </c>
+      <c r="C1368" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1368" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1368" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1369" s="0" t="s">
+        <v>2144</v>
+      </c>
+      <c r="B1369" s="0" t="s">
+        <v>2145</v>
+      </c>
+      <c r="C1369" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1369" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1369" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1370" s="0" t="s">
+        <v>2146</v>
+      </c>
+      <c r="B1370" s="0" t="s">
+        <v>2147</v>
+      </c>
+      <c r="C1370" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1370" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1370" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1371" s="0" t="s">
+        <v>2148</v>
+      </c>
+      <c r="B1371" s="0" t="s">
+        <v>2149</v>
+      </c>
+      <c r="C1371" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1371" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1371" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1372" s="0" t="s">
+        <v>2150</v>
+      </c>
+      <c r="B1372" s="0" t="s">
+        <v>2151</v>
+      </c>
+      <c r="C1372" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1372" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1372" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1373" s="0" t="s">
+        <v>2152</v>
+      </c>
+      <c r="B1373" s="0" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C1373" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1373" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1373" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1374" s="0" t="s">
+        <v>2154</v>
+      </c>
+      <c r="B1374" s="0" t="s">
+        <v>2155</v>
+      </c>
+      <c r="C1374" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1374" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1374" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1375" s="0" t="s">
+        <v>2156</v>
+      </c>
+      <c r="B1375" s="0" t="s">
+        <v>2157</v>
+      </c>
+      <c r="C1375" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1375" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1375" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1376" s="0" t="s">
+        <v>2158</v>
+      </c>
+      <c r="B1376" s="0" t="s">
+        <v>2159</v>
+      </c>
+      <c r="C1376" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1376" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1376" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1377" s="0" t="s">
+        <v>2160</v>
+      </c>
+      <c r="B1377" s="0" t="s">
+        <v>2161</v>
+      </c>
+      <c r="C1377" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1377" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1377" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1378" s="0" t="s">
+        <v>2162</v>
+      </c>
+      <c r="B1378" s="0" t="s">
+        <v>2163</v>
+      </c>
+      <c r="C1378" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1378" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1378" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1379" s="0" t="s">
+        <v>2164</v>
+      </c>
+      <c r="B1379" s="0" t="s">
+        <v>2165</v>
+      </c>
+      <c r="C1379" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1379" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1379" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1380" s="0" t="s">
+        <v>2166</v>
+      </c>
+      <c r="B1380" s="0" t="s">
+        <v>2167</v>
+      </c>
+      <c r="C1380" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1380" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1380" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1381" s="0" t="s">
+        <v>2168</v>
+      </c>
+      <c r="B1381" s="0" t="s">
+        <v>2169</v>
+      </c>
+      <c r="C1381" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1381" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1381" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1382" s="0" t="s">
+        <v>2170</v>
+      </c>
+      <c r="B1382" s="0" t="s">
+        <v>2171</v>
+      </c>
+      <c r="C1382" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1382" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1382" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1383" s="0" t="s">
+        <v>2172</v>
+      </c>
+      <c r="B1383" s="0" t="s">
+        <v>2173</v>
+      </c>
+      <c r="C1383" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1383" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1383" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1384" s="0" t="s">
+        <v>2174</v>
+      </c>
+      <c r="B1384" s="0" t="s">
+        <v>2175</v>
+      </c>
+      <c r="C1384" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1384" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1384" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1385" s="0" t="s">
+        <v>2176</v>
+      </c>
+      <c r="B1385" s="0" t="s">
+        <v>2177</v>
+      </c>
+      <c r="C1385" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1385" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1385" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1386" s="0" t="s">
+        <v>2178</v>
+      </c>
+      <c r="B1386" s="0" t="s">
+        <v>2179</v>
+      </c>
+      <c r="C1386" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1386" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1386" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1387" s="0" t="s">
+        <v>2180</v>
+      </c>
+      <c r="B1387" s="0" t="s">
+        <v>2181</v>
+      </c>
+      <c r="C1387" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1387" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1387" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1388" s="0" t="s">
+        <v>2182</v>
+      </c>
+      <c r="B1388" s="0" t="s">
+        <v>2183</v>
+      </c>
+      <c r="C1388" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1388" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1388" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1389" s="0" t="s">
+        <v>2184</v>
+      </c>
+      <c r="B1389" s="0" t="s">
+        <v>2185</v>
+      </c>
+      <c r="C1389" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1389" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1389" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1390" s="0" t="s">
+        <v>2186</v>
+      </c>
+      <c r="B1390" s="0" t="s">
+        <v>2187</v>
+      </c>
+      <c r="C1390" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1390" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1390" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1391" s="0" t="s">
+        <v>2188</v>
+      </c>
+      <c r="B1391" s="0" t="s">
+        <v>2189</v>
+      </c>
+      <c r="C1391" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1391" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1391" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1392" s="0" t="s">
+        <v>2190</v>
+      </c>
+      <c r="B1392" s="0" t="s">
+        <v>2191</v>
+      </c>
+      <c r="C1392" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1392" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1392" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1393" s="0" t="s">
+        <v>2192</v>
+      </c>
+      <c r="B1393" s="0" t="s">
+        <v>2193</v>
+      </c>
+      <c r="C1393" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1393" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1393" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1394" s="0" t="s">
+        <v>2194</v>
+      </c>
+      <c r="B1394" s="0" t="s">
+        <v>2195</v>
+      </c>
+      <c r="C1394" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1394" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1394" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1395" s="0" t="s">
+        <v>2196</v>
+      </c>
+      <c r="B1395" s="0" t="s">
+        <v>2197</v>
+      </c>
+      <c r="C1395" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1395" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1395" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1396" s="0" t="s">
+        <v>2198</v>
+      </c>
+      <c r="B1396" s="0" t="s">
+        <v>2199</v>
+      </c>
+      <c r="C1396" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1396" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1396" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1397" s="0" t="s">
+        <v>2200</v>
+      </c>
+      <c r="B1397" s="0" t="s">
+        <v>2201</v>
+      </c>
+      <c r="C1397" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1397" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1397" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1398" s="0" t="s">
+        <v>2202</v>
+      </c>
+      <c r="B1398" s="0" t="s">
+        <v>2203</v>
+      </c>
+      <c r="C1398" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1398" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1398" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1399" s="0" t="s">
+        <v>2204</v>
+      </c>
+      <c r="B1399" s="0" t="s">
+        <v>2205</v>
+      </c>
+      <c r="C1399" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1399" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1399" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1400" s="0" t="s">
+        <v>2206</v>
+      </c>
+      <c r="B1400" s="0" t="s">
+        <v>2207</v>
+      </c>
+      <c r="C1400" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1400" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1400" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1401" s="0" t="s">
+        <v>2208</v>
+      </c>
+      <c r="B1401" s="0" t="s">
+        <v>2209</v>
+      </c>
+      <c r="C1401" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1401" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1401" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1402" s="0" t="s">
+        <v>2210</v>
+      </c>
+      <c r="B1402" s="0" t="s">
+        <v>2211</v>
+      </c>
+      <c r="C1402" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1402" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1402" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1403" s="0" t="s">
+        <v>2212</v>
+      </c>
+      <c r="B1403" s="0" t="s">
+        <v>2213</v>
+      </c>
+      <c r="C1403" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1403" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1403" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1404" s="0" t="s">
+        <v>2214</v>
+      </c>
+      <c r="B1404" s="0" t="s">
+        <v>2215</v>
+      </c>
+      <c r="C1404" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1404" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1404" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1405" s="0" t="s">
+        <v>2216</v>
+      </c>
+      <c r="B1405" s="0" t="s">
+        <v>2217</v>
+      </c>
+      <c r="C1405" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1405" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1405" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1406" s="0" t="s">
+        <v>2218</v>
+      </c>
+      <c r="B1406" s="0" t="s">
+        <v>2219</v>
+      </c>
+      <c r="C1406" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1406" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1406" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1407" s="0" t="s">
+        <v>2220</v>
+      </c>
+      <c r="B1407" s="0" t="s">
+        <v>2221</v>
+      </c>
+      <c r="C1407" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1407" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1407" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1408" s="0" t="s">
+        <v>2222</v>
+      </c>
+      <c r="B1408" s="0" t="s">
+        <v>2223</v>
+      </c>
+      <c r="C1408" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1408" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1408" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1409" s="0" t="s">
+        <v>2224</v>
+      </c>
+      <c r="B1409" s="0" t="s">
+        <v>2225</v>
+      </c>
+      <c r="C1409" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1409" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1409" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1410" s="0" t="s">
+        <v>2226</v>
+      </c>
+      <c r="B1410" s="0" t="s">
+        <v>2227</v>
+      </c>
+      <c r="C1410" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1410" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1410" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1411" s="0" t="s">
+        <v>2228</v>
+      </c>
+      <c r="B1411" s="0" t="s">
+        <v>2229</v>
+      </c>
+      <c r="C1411" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1411" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1411" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1412" s="0" t="s">
+        <v>2230</v>
+      </c>
+      <c r="B1412" s="0" t="s">
+        <v>2231</v>
+      </c>
+      <c r="C1412" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1412" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1412" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1413" s="0" t="s">
+        <v>2232</v>
+      </c>
+      <c r="B1413" s="0" t="s">
+        <v>2233</v>
+      </c>
+      <c r="C1413" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1413" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1413" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1414" s="0" t="s">
+        <v>2234</v>
+      </c>
+      <c r="B1414" s="0" t="s">
+        <v>2235</v>
+      </c>
+      <c r="C1414" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1414" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1414" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1415" s="0" t="s">
+        <v>2236</v>
+      </c>
+      <c r="B1415" s="0" t="s">
+        <v>2237</v>
+      </c>
+      <c r="C1415" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1415" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1415" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1416" s="0" t="s">
+        <v>2238</v>
+      </c>
+      <c r="B1416" s="0" t="s">
+        <v>2239</v>
+      </c>
+      <c r="C1416" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1416" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1416" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1417" s="0" t="s">
+        <v>2240</v>
+      </c>
+      <c r="B1417" s="0" t="s">
+        <v>2241</v>
+      </c>
+      <c r="C1417" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1417" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1417" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1418" s="0" t="s">
+        <v>2242</v>
+      </c>
+      <c r="B1418" s="0" t="s">
+        <v>2243</v>
+      </c>
+      <c r="C1418" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1418" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1418" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1419" s="0" t="s">
+        <v>2244</v>
+      </c>
+      <c r="B1419" s="0" t="s">
+        <v>2245</v>
+      </c>
+      <c r="C1419" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1419" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1419" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1420" s="0" t="s">
+        <v>2246</v>
+      </c>
+      <c r="B1420" s="0" t="s">
+        <v>2247</v>
+      </c>
+      <c r="C1420" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1420" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1420" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1421" s="0" t="s">
+        <v>2248</v>
+      </c>
+      <c r="B1421" s="0" t="s">
+        <v>2249</v>
+      </c>
+      <c r="C1421" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1421" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1421" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1422" s="0" t="s">
+        <v>2250</v>
+      </c>
+      <c r="B1422" s="0" t="s">
+        <v>2251</v>
+      </c>
+      <c r="C1422" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1422" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1422" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1423" s="0" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1423" s="0" t="s">
+        <v>2253</v>
+      </c>
+      <c r="C1423" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1423" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1423" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1424" s="0" t="s">
+        <v>2254</v>
+      </c>
+      <c r="B1424" s="0" t="s">
+        <v>2255</v>
+      </c>
+      <c r="C1424" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1424" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1424" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1425" s="0" t="s">
+        <v>2256</v>
+      </c>
+      <c r="B1425" s="0" t="s">
+        <v>2257</v>
+      </c>
+      <c r="C1425" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1425" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1425" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1426" s="0" t="s">
+        <v>2258</v>
+      </c>
+      <c r="B1426" s="0" t="s">
+        <v>2259</v>
+      </c>
+      <c r="C1426" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1426" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1426" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1427" s="0" t="s">
+        <v>2260</v>
+      </c>
+      <c r="B1427" s="0" t="s">
+        <v>2261</v>
+      </c>
+      <c r="C1427" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1427" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1427" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1428" s="0" t="s">
+        <v>2262</v>
+      </c>
+      <c r="B1428" s="0" t="s">
+        <v>2263</v>
+      </c>
+      <c r="C1428" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1428" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1428" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1429" s="0" t="s">
+        <v>2264</v>
+      </c>
+      <c r="B1429" s="0" t="s">
+        <v>2265</v>
+      </c>
+      <c r="C1429" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1429" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1429" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1430" s="0" t="s">
+        <v>2266</v>
+      </c>
+      <c r="B1430" s="0" t="s">
+        <v>2267</v>
+      </c>
+      <c r="C1430" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1430" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1430" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1431" s="0" t="s">
+        <v>2268</v>
+      </c>
+      <c r="B1431" s="0" t="s">
+        <v>2269</v>
+      </c>
+      <c r="C1431" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1431" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1431" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1432" s="0" t="s">
+        <v>2270</v>
+      </c>
+      <c r="B1432" s="0" t="s">
+        <v>2271</v>
+      </c>
+      <c r="C1432" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1432" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1432" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1433" s="0" t="s">
+        <v>2272</v>
+      </c>
+      <c r="B1433" s="0" t="s">
+        <v>2273</v>
+      </c>
+      <c r="C1433" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1433" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1433" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1434" s="0" t="s">
+        <v>2274</v>
+      </c>
+      <c r="B1434" s="0" t="s">
+        <v>2275</v>
+      </c>
+      <c r="C1434" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1434" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1434" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1435" s="0" t="s">
+        <v>2276</v>
+      </c>
+      <c r="B1435" s="0" t="s">
+        <v>2277</v>
+      </c>
+      <c r="C1435" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1435" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1435" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1436" s="0" t="s">
+        <v>2278</v>
+      </c>
+      <c r="B1436" s="0" t="s">
+        <v>2279</v>
+      </c>
+      <c r="C1436" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1436" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1436" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1437" s="0" t="s">
+        <v>2280</v>
+      </c>
+      <c r="B1437" s="0" t="s">
+        <v>2281</v>
+      </c>
+      <c r="C1437" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1437" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1437" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1438" s="0" t="s">
+        <v>2282</v>
+      </c>
+      <c r="B1438" s="0" t="s">
+        <v>2283</v>
+      </c>
+      <c r="C1438" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1438" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1438" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1439" s="0" t="s">
+        <v>2284</v>
+      </c>
+      <c r="B1439" s="0" t="s">
+        <v>2285</v>
+      </c>
+      <c r="C1439" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1439" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1439" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1440" s="0" t="s">
+        <v>2286</v>
+      </c>
+      <c r="B1440" s="0" t="s">
+        <v>2287</v>
+      </c>
+      <c r="C1440" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1440" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1440" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1441" s="0" t="s">
+        <v>2288</v>
+      </c>
+      <c r="B1441" s="0" t="s">
+        <v>2289</v>
+      </c>
+      <c r="C1441" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1441" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1441" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1442" s="0" t="s">
+        <v>2290</v>
+      </c>
+      <c r="B1442" s="0" t="s">
+        <v>2291</v>
+      </c>
+      <c r="C1442" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1442" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1442" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1443" s="0" t="s">
+        <v>2292</v>
+      </c>
+      <c r="B1443" s="0" t="s">
+        <v>2293</v>
+      </c>
+      <c r="C1443" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1443" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1443" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1444" s="0" t="s">
+        <v>2294</v>
+      </c>
+      <c r="B1444" s="0" t="s">
+        <v>2295</v>
+      </c>
+      <c r="C1444" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1444" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1444" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1445" s="0" t="s">
+        <v>2296</v>
+      </c>
+      <c r="B1445" s="0" t="s">
+        <v>2297</v>
+      </c>
+      <c r="C1445" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1445" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1445" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1446" s="0" t="s">
+        <v>2298</v>
+      </c>
+      <c r="B1446" s="0" t="s">
+        <v>2299</v>
+      </c>
+      <c r="C1446" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1446" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1446" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1447" s="0" t="s">
+        <v>2300</v>
+      </c>
+      <c r="B1447" s="0" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C1447" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1447" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1447" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1448" s="0" t="s">
+        <v>2302</v>
+      </c>
+      <c r="B1448" s="0" t="s">
+        <v>2303</v>
+      </c>
+      <c r="C1448" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1448" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1448" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1449" s="0" t="s">
+        <v>2304</v>
+      </c>
+      <c r="B1449" s="0" t="s">
+        <v>2305</v>
+      </c>
+      <c r="C1449" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1449" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1449" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1450" s="0" t="s">
+        <v>2306</v>
+      </c>
+      <c r="B1450" s="0" t="s">
+        <v>2307</v>
+      </c>
+      <c r="C1450" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1450" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1450" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1451" s="0" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1451" s="0" t="s">
+        <v>2309</v>
+      </c>
+      <c r="C1451" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1451" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1451" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1452" s="0" t="s">
+        <v>2310</v>
+      </c>
+      <c r="B1452" s="0" t="s">
+        <v>2311</v>
+      </c>
+      <c r="C1452" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1452" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1452" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1453" s="0" t="s">
+        <v>2312</v>
+      </c>
+      <c r="B1453" s="0" t="s">
+        <v>2313</v>
+      </c>
+      <c r="C1453" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1453" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F1453" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
fix cryptic bug in cor_matrix() with weights par being strange data type
fix bug in GG_proportions() related to R being updated I think

fix bug in pu_translate() data (Turkey vs. Tunesia)

update some tests
</commit_message>
<xml_diff>
--- a/inst/extdata/political_units.xlsx
+++ b/inst/extdata/political_units.xlsx
@@ -7250,18 +7250,18 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -7272,14 +7272,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="bottomRight" activeCell="C19" activeCellId="2" sqref="B965 B964 C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.21875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.76"/>
@@ -7293,20 +7291,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="25.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="9.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="9.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="7.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="6.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="9.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="9.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="7.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="6.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="6.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="35" style="0" width="8.21"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16538,7 +16531,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -16547,22 +16540,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="2" sqref="B965 B964 A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="7.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="9.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="7.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="7.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16803,7 +16794,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -16812,32 +16803,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J1493"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B939" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="bottomLeft" activeCell="A939" activeCellId="0" sqref="A939"/>
+      <selection pane="bottomRight" activeCell="B964" activeCellId="1" sqref="B965 B964"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="7.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="7.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="7.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26305,7 +26293,7 @@
         <v>1509</v>
       </c>
       <c r="B963" s="0" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E963" s="0" t="s">
         <v>553</v>
@@ -34374,7 +34362,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>